<commit_message>
Added Punk voices to Game/media/voices and updated metadata and cuesheet
</commit_message>
<xml_diff>
--- a/Docs/TDS/CueSheet.xlsx
+++ b/Docs/TDS/CueSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="643">
   <si>
     <t>Cue-Sheets</t>
   </si>
@@ -1447,255 +1447,144 @@
     <t>Enumerado por personaje</t>
   </si>
   <si>
-    <t>V-001</t>
-  </si>
-  <si>
     <t>Sí</t>
   </si>
   <si>
-    <t>Personaje 1</t>
-  </si>
-  <si>
     <t>Indeterminado</t>
   </si>
   <si>
     <t>Voz de seleccion</t>
   </si>
   <si>
-    <t>V-002</t>
-  </si>
-  <si>
     <t>Voz de que algo ha salido bien</t>
   </si>
   <si>
-    <t>V-003</t>
-  </si>
-  <si>
     <t>Voz de que algo ha salido bien 2</t>
   </si>
   <si>
-    <t>V-004</t>
-  </si>
-  <si>
     <t>Voz de que algo ha salido mal</t>
   </si>
   <si>
     <t>1.5</t>
   </si>
   <si>
-    <t>V-005</t>
-  </si>
-  <si>
     <t>Voz de que algo ha salido mal 2</t>
   </si>
   <si>
     <t>1.6</t>
   </si>
   <si>
-    <t>V-006</t>
-  </si>
-  <si>
     <t>Voz emitida cuando haya un choque</t>
   </si>
   <si>
     <t>1.7</t>
   </si>
   <si>
-    <t>V-007</t>
-  </si>
-  <si>
     <t>Victoria</t>
   </si>
   <si>
     <t>1.8</t>
   </si>
   <si>
-    <t>V-008</t>
-  </si>
-  <si>
     <t>Derrota</t>
   </si>
   <si>
     <t>1.9</t>
   </si>
   <si>
-    <t>V-009</t>
-  </si>
-  <si>
     <t>Acelerón</t>
   </si>
   <si>
     <t>2.1</t>
   </si>
   <si>
-    <t>V-010</t>
-  </si>
-  <si>
     <t>Personaje 2</t>
   </si>
   <si>
     <t>2.2</t>
   </si>
   <si>
-    <t>V-011</t>
-  </si>
-  <si>
     <t>2.3</t>
   </si>
   <si>
-    <t>V-012</t>
-  </si>
-  <si>
     <t>2.4</t>
   </si>
   <si>
-    <t>V-013</t>
-  </si>
-  <si>
     <t>2.5</t>
   </si>
   <si>
-    <t>V-014</t>
-  </si>
-  <si>
     <t>2.6</t>
   </si>
   <si>
-    <t>V-015</t>
-  </si>
-  <si>
     <t>2.7</t>
   </si>
   <si>
-    <t>V-016</t>
-  </si>
-  <si>
     <t>2.8</t>
   </si>
   <si>
-    <t>V-017</t>
-  </si>
-  <si>
     <t>2.9</t>
   </si>
   <si>
-    <t>V-018</t>
-  </si>
-  <si>
     <t>3.1</t>
   </si>
   <si>
-    <t>V-019</t>
-  </si>
-  <si>
     <t>Personaje 3</t>
   </si>
   <si>
     <t>3.2</t>
   </si>
   <si>
-    <t>V-020</t>
-  </si>
-  <si>
     <t>3.3</t>
   </si>
   <si>
-    <t>V-021</t>
-  </si>
-  <si>
     <t>3.4</t>
   </si>
   <si>
-    <t>V-022</t>
-  </si>
-  <si>
     <t>3.5</t>
   </si>
   <si>
-    <t>V-023</t>
-  </si>
-  <si>
     <t>3.6</t>
   </si>
   <si>
-    <t>V-024</t>
-  </si>
-  <si>
     <t>3.7</t>
   </si>
   <si>
-    <t>V-025</t>
-  </si>
-  <si>
     <t>3.8</t>
   </si>
   <si>
-    <t>V-026</t>
-  </si>
-  <si>
     <t>3.9</t>
   </si>
   <si>
-    <t>V-027</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
-    <t>V-028</t>
-  </si>
-  <si>
     <t>Personaje 4</t>
   </si>
   <si>
     <t>4.2</t>
   </si>
   <si>
-    <t>V-029</t>
-  </si>
-  <si>
     <t>4.3</t>
   </si>
   <si>
-    <t>V-030</t>
-  </si>
-  <si>
     <t>4.4</t>
   </si>
   <si>
-    <t>V-031</t>
-  </si>
-  <si>
     <t>4.5</t>
   </si>
   <si>
-    <t>V-032</t>
-  </si>
-  <si>
     <t>4.6</t>
   </si>
   <si>
-    <t>V-033</t>
-  </si>
-  <si>
     <t>4.7</t>
   </si>
   <si>
-    <t>V-034</t>
-  </si>
-  <si>
     <t>4.8</t>
   </si>
   <si>
-    <t>V-035</t>
-  </si>
-  <si>
     <t>4.9</t>
   </si>
   <si>
-    <t>V-036</t>
-  </si>
-  <si>
     <t>Sonidos generales de todos los niveles</t>
   </si>
   <si>
@@ -1937,6 +1826,261 @@
   </si>
   <si>
     <t>Musica de fondo del nivel 1</t>
+  </si>
+  <si>
+    <t>V-210 V-215</t>
+  </si>
+  <si>
+    <t>V-220 V-225</t>
+  </si>
+  <si>
+    <t>V-230 V-235</t>
+  </si>
+  <si>
+    <t>V-240 V-245</t>
+  </si>
+  <si>
+    <t>V-250 V-255</t>
+  </si>
+  <si>
+    <t>V-260 V-265</t>
+  </si>
+  <si>
+    <t>V-270 V-275</t>
+  </si>
+  <si>
+    <t>V-280 V-285</t>
+  </si>
+  <si>
+    <t>V-290 V-295</t>
+  </si>
+  <si>
+    <t>V-310 V-315</t>
+  </si>
+  <si>
+    <t>V-320 V-325</t>
+  </si>
+  <si>
+    <t>V-330 V-335</t>
+  </si>
+  <si>
+    <t>V-340 V-345</t>
+  </si>
+  <si>
+    <t>V-350 V-355</t>
+  </si>
+  <si>
+    <t>V-360 V-365</t>
+  </si>
+  <si>
+    <t>V-370 V-375</t>
+  </si>
+  <si>
+    <t>V-380 V-385</t>
+  </si>
+  <si>
+    <t>V-390 V-395</t>
+  </si>
+  <si>
+    <t>V-410 V-415</t>
+  </si>
+  <si>
+    <t>V-420 V-425</t>
+  </si>
+  <si>
+    <t>V-430 V-435</t>
+  </si>
+  <si>
+    <t>V-440 V-445</t>
+  </si>
+  <si>
+    <t>V-450 V-455</t>
+  </si>
+  <si>
+    <t>V-460 V-465</t>
+  </si>
+  <si>
+    <t>V-470 V-475</t>
+  </si>
+  <si>
+    <t>V-480 V-485</t>
+  </si>
+  <si>
+    <t>V-490 V-495</t>
+  </si>
+  <si>
+    <t>Punk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-110 </t>
+  </si>
+  <si>
+    <t>V-115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-120 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-121 </t>
+  </si>
+  <si>
+    <t>V-122</t>
+  </si>
+  <si>
+    <t>V-125</t>
+  </si>
+  <si>
+    <t>V-126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-130 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-131 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-135 </t>
+  </si>
+  <si>
+    <t>V-136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-140 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-141 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-145 </t>
+  </si>
+  <si>
+    <t>V-146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-150 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-151 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-155 </t>
+  </si>
+  <si>
+    <t>V-156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-160 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-161 </t>
+  </si>
+  <si>
+    <t>V-165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-170 </t>
+  </si>
+  <si>
+    <t>V-175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-180 </t>
+  </si>
+  <si>
+    <t>V-185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-190 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-191 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-192 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-195 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-196 </t>
+  </si>
+  <si>
+    <t>V-197</t>
+  </si>
+  <si>
+    <t>Voz de selección (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido bien 1</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido bien 2 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 1</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido bien 1.1</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido bien 1.2</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido bien 2.1</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido bien 2.1 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 1.1</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido bien 1 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido bien 1.1 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 1 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 1.1 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 2.1</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 2 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 2.1 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Voz emitida cuando haya un choque 1</t>
+  </si>
+  <si>
+    <t>Voz emitida cuando haya un choque (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Victoria (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Derrota (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Acelerón 1</t>
+  </si>
+  <si>
+    <t>Acelerón 2</t>
+  </si>
+  <si>
+    <t>Acelerón (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Acelerón 1 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Acelerón 2 (INGLÉS)</t>
   </si>
 </sst>
 </file>
@@ -2104,7 +2248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -2597,12 +2741,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2963,21 +3200,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2991,9 +3213,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3010,6 +3229,47 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -3917,27 +4177,27 @@
         <v>15</v>
       </c>
       <c r="C7" s="17">
-        <f>Personajes!E42</f>
+        <f>Personajes!E65</f>
         <v>0</v>
       </c>
       <c r="D7" s="17">
-        <f>Personajes!F42</f>
+        <f>Personajes!F65</f>
         <v>0</v>
       </c>
       <c r="E7" s="17">
-        <f>Personajes!G42</f>
+        <f>Personajes!G65</f>
         <v>0</v>
       </c>
       <c r="F7" s="17">
-        <f>Personajes!H42</f>
+        <f>Personajes!H65</f>
         <v>0</v>
       </c>
       <c r="G7" s="17">
-        <f>Personajes!I42</f>
+        <f>Personajes!I65</f>
         <v>0</v>
       </c>
       <c r="H7" s="17">
-        <f>Personajes!J42</f>
+        <f>Personajes!J65</f>
         <v>36</v>
       </c>
       <c r="I7" s="18">
@@ -4049,7 +4309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AMK22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
@@ -4070,7 +4330,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>590</v>
+        <v>553</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>409</v>
@@ -4148,7 +4408,7 @@
     </row>
     <row r="4" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
-        <v>591</v>
+        <v>554</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="49"/>
@@ -4166,14 +4426,14 @@
       <c r="P4" s="53"/>
     </row>
     <row r="5" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="126" t="s">
         <v>285</v>
       </c>
       <c r="C5" s="56" t="s">
         <v>414</v>
       </c>
-      <c r="D5" s="134" t="s">
-        <v>592</v>
+      <c r="D5" s="129" t="s">
+        <v>555</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>200</v>
@@ -4190,10 +4450,10 @@
       <c r="M5" s="57"/>
       <c r="N5" s="57"/>
       <c r="O5" s="56" t="s">
-        <v>593</v>
+        <v>556</v>
       </c>
       <c r="P5" s="56" t="s">
-        <v>594</v>
+        <v>557</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4535,82 +4795,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="127" t="s">
+      <c r="C3" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="128" t="s">
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="127" t="s">
+      <c r="G3" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="127" t="s">
+      <c r="H3" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="127" t="s">
+      <c r="I3" s="147" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="127" t="s">
+      <c r="J3" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="127" t="s">
+      <c r="K3" s="147" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="127" t="s">
+      <c r="L3" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="127" t="s">
+      <c r="M3" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="128" t="s">
+      <c r="N3" s="148" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="127"/>
-      <c r="B4" s="127"/>
+      <c r="A4" s="147"/>
+      <c r="B4" s="147"/>
       <c r="C4" s="27" t="s">
         <v>31</v>
       </c>
@@ -4620,15 +4880,15 @@
       <c r="E4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="128"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
-      <c r="N4" s="128"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="147"/>
+      <c r="L4" s="147"/>
+      <c r="M4" s="147"/>
+      <c r="N4" s="148"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -6696,79 +6956,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="146" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="147" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="127" t="s">
+      <c r="C3" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="127" t="s">
+      <c r="D3" s="147" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127" t="s">
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147" t="s">
         <v>194</v>
       </c>
-      <c r="J3" s="127" t="s">
+      <c r="J3" s="147" t="s">
         <v>195</v>
       </c>
-      <c r="K3" s="127" t="s">
+      <c r="K3" s="147" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="127" t="s">
+      <c r="L3" s="147" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="127" t="s">
+      <c r="M3" s="147" t="s">
         <v>198</v>
       </c>
-      <c r="N3" s="127" t="s">
+      <c r="N3" s="147" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="128"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
+      <c r="A4" s="148"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="147"/>
       <c r="D4" s="27" t="s">
         <v>200</v>
       </c>
@@ -6784,12 +7044,12 @@
       <c r="H4" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
-      <c r="N4" s="127"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="147"/>
+      <c r="L4" s="147"/>
+      <c r="M4" s="147"/>
+      <c r="N4" s="147"/>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -8380,7 +8640,7 @@
       <c r="Q4" s="53"/>
     </row>
     <row r="5" spans="2:17" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="126" t="s">
         <v>285</v>
       </c>
       <c r="C5" s="54">
@@ -8389,7 +8649,7 @@
       <c r="D5" s="55">
         <v>2.31481481481481E-4</v>
       </c>
-      <c r="E5" s="134" t="s">
+      <c r="E5" s="129" t="s">
         <v>286</v>
       </c>
       <c r="F5" s="57" t="s">
@@ -8418,7 +8678,7 @@
       </c>
     </row>
     <row r="6" spans="2:17" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="127" t="s">
         <v>292</v>
       </c>
       <c r="C6" s="60">
@@ -8427,7 +8687,7 @@
       <c r="D6" s="61">
         <v>4.6296296296296298E-4</v>
       </c>
-      <c r="E6" s="135" t="s">
+      <c r="E6" s="130" t="s">
         <v>293</v>
       </c>
       <c r="F6" s="63" t="s">
@@ -8794,82 +9054,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="146" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="149" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="130" t="s">
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="127" t="s">
+      <c r="G3" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="127" t="s">
+      <c r="H3" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="127" t="s">
+      <c r="I3" s="147" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="127" t="s">
+      <c r="J3" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="127" t="s">
+      <c r="K3" s="147" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="127" t="s">
+      <c r="L3" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="127" t="s">
+      <c r="M3" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="128" t="s">
+      <c r="N3" s="148" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="127"/>
-      <c r="B4" s="127"/>
+      <c r="A4" s="147"/>
+      <c r="B4" s="147"/>
       <c r="C4" s="97" t="s">
         <v>31</v>
       </c>
@@ -8879,15 +9139,15 @@
       <c r="E4" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="130"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
-      <c r="N4" s="128"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="147"/>
+      <c r="L4" s="147"/>
+      <c r="M4" s="147"/>
+      <c r="N4" s="148"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -10190,79 +10450,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="146" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="147" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="127" t="s">
+      <c r="C3" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="127" t="s">
+      <c r="D3" s="147" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127" t="s">
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147" t="s">
         <v>194</v>
       </c>
-      <c r="J3" s="127" t="s">
+      <c r="J3" s="147" t="s">
         <v>195</v>
       </c>
-      <c r="K3" s="127" t="s">
+      <c r="K3" s="147" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="127" t="s">
+      <c r="L3" s="147" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="127" t="s">
+      <c r="M3" s="147" t="s">
         <v>198</v>
       </c>
-      <c r="N3" s="127" t="s">
+      <c r="N3" s="147" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="128"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
+      <c r="A4" s="148"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="147"/>
       <c r="D4" s="27" t="s">
         <v>200</v>
       </c>
@@ -10278,12 +10538,12 @@
       <c r="H4" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
-      <c r="N4" s="127"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
+      <c r="K4" s="147"/>
+      <c r="L4" s="147"/>
+      <c r="M4" s="147"/>
+      <c r="N4" s="147"/>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -11401,13 +11661,13 @@
       <c r="P4" s="53"/>
     </row>
     <row r="5" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="126" t="s">
         <v>285</v>
       </c>
       <c r="C5" s="56" t="s">
         <v>414</v>
       </c>
-      <c r="D5" s="134" t="s">
+      <c r="D5" s="129" t="s">
         <v>293</v>
       </c>
       <c r="E5" s="57" t="s">
@@ -11436,13 +11696,13 @@
       </c>
     </row>
     <row r="6" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="127" t="s">
         <v>292</v>
       </c>
       <c r="C6" s="100" t="s">
         <v>415</v>
       </c>
-      <c r="D6" s="141" t="s">
+      <c r="D6" s="135" t="s">
         <v>416</v>
       </c>
       <c r="E6" s="64"/>
@@ -11469,13 +11729,13 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="132" t="s">
+      <c r="B7" s="127" t="s">
         <v>419</v>
       </c>
       <c r="C7" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D7" s="141" t="s">
+      <c r="D7" s="135" t="s">
         <v>421</v>
       </c>
       <c r="E7" s="64"/>
@@ -11502,13 +11762,13 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="127" t="s">
         <v>423</v>
       </c>
       <c r="C8" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D8" s="135" t="s">
+      <c r="D8" s="130" t="s">
         <v>424</v>
       </c>
       <c r="E8" s="64"/>
@@ -11535,13 +11795,13 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="133" t="s">
-        <v>442</v>
+      <c r="B9" s="128" t="s">
+        <v>437</v>
       </c>
       <c r="C9" s="114" t="s">
         <v>426</v>
       </c>
-      <c r="D9" s="142" t="s">
+      <c r="D9" s="136" t="s">
         <v>427</v>
       </c>
       <c r="E9" s="102"/>
@@ -11819,10 +12079,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK44"/>
+  <dimension ref="A1:AMK67"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -11830,15 +12090,15 @@
     <col min="1" max="1" width="5.85546875" style="31" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="32" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="32" customWidth="1"/>
     <col min="5" max="9" width="2" style="32" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" style="32" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="32" customWidth="1"/>
     <col min="11" max="11" width="7.28515625" style="32" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" style="32" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" style="32" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" style="32" customWidth="1"/>
     <col min="15" max="15" width="22.7109375" style="32" customWidth="1"/>
-    <col min="16" max="16" width="31.7109375" style="32" customWidth="1"/>
+    <col min="16" max="16" width="43.140625" style="32" customWidth="1"/>
     <col min="17" max="1025" width="11.42578125" style="32"/>
   </cols>
   <sheetData>
@@ -11887,7 +12147,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="41"/>
       <c r="C3" s="42" t="s">
         <v>412</v>
@@ -11920,7 +12180,7 @@
       <c r="O3" s="45"/>
       <c r="P3" s="46"/>
     </row>
-    <row r="4" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="99" t="s">
         <v>430</v>
       </c>
@@ -11931,7 +12191,7 @@
       <c r="G4" s="51"/>
       <c r="H4" s="51"/>
       <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
+      <c r="J4" s="145"/>
       <c r="K4" s="51"/>
       <c r="L4" s="51"/>
       <c r="M4" s="51"/>
@@ -11939,79 +12199,77 @@
       <c r="O4" s="48"/>
       <c r="P4" s="53"/>
     </row>
-    <row r="5" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="138" t="s">
+    <row r="5" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="132" t="s">
         <v>285</v>
       </c>
       <c r="C5" s="59"/>
-      <c r="D5" s="136" t="s">
-        <v>431</v>
+      <c r="D5" s="143" t="s">
+        <v>586</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
       <c r="G5" s="58"/>
       <c r="H5" s="58"/>
       <c r="I5" s="58"/>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="142" t="s">
         <v>204</v>
       </c>
-      <c r="K5" s="58" t="s">
+      <c r="K5" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L5" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M5" s="138" t="s">
         <v>432</v>
       </c>
-      <c r="L5" s="58" t="s">
+      <c r="N5" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O5" s="59"/>
+      <c r="P5" s="151" t="s">
         <v>433</v>
       </c>
-      <c r="M5" s="58" t="s">
-        <v>434</v>
-      </c>
-      <c r="N5" s="58" t="s">
-        <v>220</v>
-      </c>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="139" t="s">
-        <v>292</v>
-      </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="137" t="s">
-        <v>436</v>
-      </c>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
+    </row>
+    <row r="6" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="141"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="144" t="s">
+        <v>587</v>
+      </c>
+      <c r="E6" s="139"/>
+      <c r="F6" s="139"/>
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="139"/>
       <c r="J6" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K6" s="64" t="s">
+      <c r="K6" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L6" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M6" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L6" s="64" t="s">
-        <v>433</v>
-      </c>
-      <c r="M6" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N6" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="139" t="s">
-        <v>419</v>
+      <c r="O6" s="142"/>
+      <c r="P6" s="142" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="133" t="s">
+        <v>292</v>
       </c>
       <c r="C7" s="65"/>
-      <c r="D7" s="137" t="s">
-        <v>438</v>
+      <c r="D7" s="135" t="s">
+        <v>588</v>
       </c>
       <c r="E7" s="64"/>
       <c r="F7" s="64"/>
@@ -12021,30 +12279,28 @@
       <c r="J7" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K7" s="64" t="s">
+      <c r="K7" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L7" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M7" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L7" s="64" t="s">
-        <v>433</v>
-      </c>
-      <c r="M7" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N7" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O7" s="65"/>
       <c r="P7" s="65" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="139" t="s">
-        <v>423</v>
-      </c>
+        <v>619</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="133"/>
       <c r="C8" s="65"/>
-      <c r="D8" s="137" t="s">
-        <v>440</v>
+      <c r="D8" s="135" t="s">
+        <v>589</v>
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="64"/>
@@ -12054,30 +12310,28 @@
       <c r="J8" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K8" s="64" t="s">
+      <c r="K8" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L8" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M8" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L8" s="64" t="s">
-        <v>433</v>
-      </c>
-      <c r="M8" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N8" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O8" s="65"/>
       <c r="P8" s="65" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="139" t="s">
-        <v>442</v>
-      </c>
+        <v>622</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="133"/>
       <c r="C9" s="65"/>
-      <c r="D9" s="137" t="s">
-        <v>443</v>
+      <c r="D9" s="135" t="s">
+        <v>590</v>
       </c>
       <c r="E9" s="64"/>
       <c r="F9" s="64"/>
@@ -12087,30 +12341,28 @@
       <c r="J9" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="64" t="s">
+      <c r="K9" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L9" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M9" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L9" s="64" t="s">
-        <v>433</v>
-      </c>
-      <c r="M9" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N9" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O9" s="65"/>
       <c r="P9" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="139" t="s">
-        <v>445</v>
-      </c>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="133"/>
       <c r="C10" s="65"/>
-      <c r="D10" s="137" t="s">
-        <v>446</v>
+      <c r="D10" s="135" t="s">
+        <v>591</v>
       </c>
       <c r="E10" s="64"/>
       <c r="F10" s="64"/>
@@ -12120,30 +12372,28 @@
       <c r="J10" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K10" s="64" t="s">
+      <c r="K10" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L10" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M10" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L10" s="64" t="s">
-        <v>433</v>
-      </c>
-      <c r="M10" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N10" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O10" s="65"/>
       <c r="P10" s="65" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="139" t="s">
-        <v>448</v>
-      </c>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="133"/>
       <c r="C11" s="65"/>
-      <c r="D11" s="137" t="s">
-        <v>449</v>
+      <c r="D11" s="135" t="s">
+        <v>592</v>
       </c>
       <c r="E11" s="64"/>
       <c r="F11" s="64"/>
@@ -12153,30 +12403,30 @@
       <c r="J11" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L11" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M11" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L11" s="64" t="s">
-        <v>433</v>
-      </c>
-      <c r="M11" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N11" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O11" s="65"/>
       <c r="P11" s="65" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="139" t="s">
-        <v>451</v>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="133" t="s">
+        <v>419</v>
       </c>
       <c r="C12" s="65"/>
-      <c r="D12" s="137" t="s">
-        <v>452</v>
+      <c r="D12" s="135" t="s">
+        <v>593</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -12186,30 +12436,28 @@
       <c r="J12" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K12" s="64" t="s">
+      <c r="K12" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L12" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M12" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L12" s="64" t="s">
-        <v>433</v>
-      </c>
-      <c r="M12" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N12" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O12" s="65"/>
       <c r="P12" s="65" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="139" t="s">
-        <v>454</v>
-      </c>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="133"/>
       <c r="C13" s="65"/>
-      <c r="D13" s="137" t="s">
-        <v>455</v>
+      <c r="D13" s="135" t="s">
+        <v>594</v>
       </c>
       <c r="E13" s="64"/>
       <c r="F13" s="64"/>
@@ -12219,30 +12467,28 @@
       <c r="J13" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K13" s="64" t="s">
+      <c r="K13" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L13" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M13" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L13" s="64" t="s">
-        <v>433</v>
-      </c>
-      <c r="M13" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N13" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O13" s="65"/>
       <c r="P13" s="65" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="139" t="s">
-        <v>457</v>
-      </c>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="133"/>
       <c r="C14" s="65"/>
-      <c r="D14" s="137" t="s">
-        <v>458</v>
+      <c r="D14" s="135" t="s">
+        <v>595</v>
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
@@ -12252,30 +12498,28 @@
       <c r="J14" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K14" s="64" t="s">
+      <c r="K14" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L14" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M14" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L14" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M14" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N14" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O14" s="65"/>
       <c r="P14" s="65" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="139" t="s">
-        <v>460</v>
-      </c>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="133"/>
       <c r="C15" s="65"/>
-      <c r="D15" s="137" t="s">
-        <v>461</v>
+      <c r="D15" s="135" t="s">
+        <v>596</v>
       </c>
       <c r="E15" s="64"/>
       <c r="F15" s="64"/>
@@ -12285,30 +12529,30 @@
       <c r="J15" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K15" s="64" t="s">
+      <c r="K15" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L15" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M15" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L15" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M15" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N15" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O15" s="65"/>
       <c r="P15" s="65" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="139" t="s">
-        <v>462</v>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="133" t="s">
+        <v>423</v>
       </c>
       <c r="C16" s="65"/>
-      <c r="D16" s="137" t="s">
-        <v>463</v>
+      <c r="D16" s="135" t="s">
+        <v>597</v>
       </c>
       <c r="E16" s="64"/>
       <c r="F16" s="64"/>
@@ -12318,30 +12562,28 @@
       <c r="J16" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K16" s="64" t="s">
+      <c r="K16" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L16" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M16" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L16" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M16" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N16" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O16" s="65"/>
       <c r="P16" s="65" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="139" t="s">
-        <v>464</v>
-      </c>
+        <v>621</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="133"/>
       <c r="C17" s="65"/>
-      <c r="D17" s="137" t="s">
-        <v>465</v>
+      <c r="D17" s="135" t="s">
+        <v>598</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="64"/>
@@ -12351,30 +12593,28 @@
       <c r="J17" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K17" s="64" t="s">
+      <c r="K17" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L17" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M17" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L17" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M17" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N17" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O17" s="65"/>
       <c r="P17" s="65" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="139" t="s">
-        <v>466</v>
-      </c>
+        <v>626</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="133"/>
       <c r="C18" s="65"/>
-      <c r="D18" s="137" t="s">
-        <v>467</v>
+      <c r="D18" s="135" t="s">
+        <v>599</v>
       </c>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
@@ -12384,30 +12624,28 @@
       <c r="J18" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K18" s="64" t="s">
+      <c r="K18" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L18" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M18" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L18" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M18" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N18" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O18" s="65"/>
       <c r="P18" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="139" t="s">
-        <v>468</v>
-      </c>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="133"/>
       <c r="C19" s="65"/>
-      <c r="D19" s="137" t="s">
-        <v>469</v>
+      <c r="D19" s="135" t="s">
+        <v>600</v>
       </c>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
@@ -12417,30 +12655,30 @@
       <c r="J19" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K19" s="64" t="s">
+      <c r="K19" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L19" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M19" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L19" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M19" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N19" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O19" s="65"/>
       <c r="P19" s="65" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="139" t="s">
-        <v>470</v>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="133" t="s">
+        <v>437</v>
       </c>
       <c r="C20" s="65"/>
-      <c r="D20" s="137" t="s">
-        <v>471</v>
+      <c r="D20" s="135" t="s">
+        <v>601</v>
       </c>
       <c r="E20" s="64"/>
       <c r="F20" s="64"/>
@@ -12450,30 +12688,28 @@
       <c r="J20" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K20" s="64" t="s">
+      <c r="K20" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L20" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M20" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L20" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M20" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N20" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O20" s="65"/>
       <c r="P20" s="65" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="139" t="s">
-        <v>472</v>
-      </c>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="133"/>
       <c r="C21" s="65"/>
-      <c r="D21" s="137" t="s">
-        <v>473</v>
+      <c r="D21" s="135" t="s">
+        <v>602</v>
       </c>
       <c r="E21" s="64"/>
       <c r="F21" s="64"/>
@@ -12483,30 +12719,28 @@
       <c r="J21" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K21" s="64" t="s">
+      <c r="K21" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L21" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M21" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L21" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M21" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N21" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O21" s="65"/>
       <c r="P21" s="65" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="139" t="s">
-        <v>474</v>
-      </c>
+        <v>631</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="133"/>
       <c r="C22" s="65"/>
-      <c r="D22" s="137" t="s">
-        <v>475</v>
+      <c r="D22" s="135" t="s">
+        <v>603</v>
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="64"/>
@@ -12516,30 +12750,28 @@
       <c r="J22" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K22" s="64" t="s">
+      <c r="K22" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L22" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M22" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L22" s="64" t="s">
-        <v>459</v>
-      </c>
-      <c r="M22" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N22" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O22" s="65"/>
       <c r="P22" s="65" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="139" t="s">
-        <v>476</v>
-      </c>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="133"/>
       <c r="C23" s="65"/>
-      <c r="D23" s="137" t="s">
-        <v>477</v>
+      <c r="D23" s="135" t="s">
+        <v>604</v>
       </c>
       <c r="E23" s="64"/>
       <c r="F23" s="64"/>
@@ -12549,30 +12781,30 @@
       <c r="J23" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K23" s="64" t="s">
+      <c r="K23" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L23" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M23" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L23" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M23" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N23" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O23" s="65"/>
       <c r="P23" s="65" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="139" t="s">
-        <v>479</v>
+        <v>633</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="133" t="s">
+        <v>439</v>
       </c>
       <c r="C24" s="65"/>
-      <c r="D24" s="137" t="s">
-        <v>480</v>
+      <c r="D24" s="135" t="s">
+        <v>605</v>
       </c>
       <c r="E24" s="64"/>
       <c r="F24" s="64"/>
@@ -12582,30 +12814,28 @@
       <c r="J24" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K24" s="64" t="s">
+      <c r="K24" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L24" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M24" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L24" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M24" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N24" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O24" s="65"/>
       <c r="P24" s="65" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="139" t="s">
-        <v>481</v>
-      </c>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="133"/>
       <c r="C25" s="65"/>
-      <c r="D25" s="137" t="s">
-        <v>482</v>
+      <c r="D25" s="135" t="s">
+        <v>606</v>
       </c>
       <c r="E25" s="64"/>
       <c r="F25" s="64"/>
@@ -12615,30 +12845,28 @@
       <c r="J25" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K25" s="64" t="s">
+      <c r="K25" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L25" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M25" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L25" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M25" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N25" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O25" s="65"/>
       <c r="P25" s="65" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="139" t="s">
-        <v>483</v>
-      </c>
+        <v>634</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="133"/>
       <c r="C26" s="65"/>
-      <c r="D26" s="137" t="s">
-        <v>484</v>
+      <c r="D26" s="135" t="s">
+        <v>607</v>
       </c>
       <c r="E26" s="64"/>
       <c r="F26" s="64"/>
@@ -12648,30 +12876,30 @@
       <c r="J26" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K26" s="64" t="s">
+      <c r="K26" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L26" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M26" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L26" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M26" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N26" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O26" s="65"/>
       <c r="P26" s="65" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="133" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="139" t="s">
-        <v>485</v>
-      </c>
       <c r="C27" s="65"/>
-      <c r="D27" s="137" t="s">
-        <v>486</v>
+      <c r="D27" s="135" t="s">
+        <v>608</v>
       </c>
       <c r="E27" s="64"/>
       <c r="F27" s="64"/>
@@ -12681,30 +12909,28 @@
       <c r="J27" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K27" s="64" t="s">
+      <c r="K27" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L27" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M27" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L27" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M27" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N27" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O27" s="65"/>
       <c r="P27" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="139" t="s">
-        <v>487</v>
-      </c>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="133"/>
       <c r="C28" s="65"/>
-      <c r="D28" s="137" t="s">
-        <v>488</v>
+      <c r="D28" s="135" t="s">
+        <v>609</v>
       </c>
       <c r="E28" s="64"/>
       <c r="F28" s="64"/>
@@ -12714,30 +12940,30 @@
       <c r="J28" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K28" s="64" t="s">
+      <c r="K28" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L28" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M28" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L28" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M28" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N28" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O28" s="65"/>
       <c r="P28" s="65" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="139" t="s">
-        <v>489</v>
+        <v>636</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="133" t="s">
+        <v>443</v>
       </c>
       <c r="C29" s="65"/>
-      <c r="D29" s="137" t="s">
-        <v>490</v>
+      <c r="D29" s="135" t="s">
+        <v>610</v>
       </c>
       <c r="E29" s="64"/>
       <c r="F29" s="64"/>
@@ -12747,30 +12973,28 @@
       <c r="J29" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K29" s="64" t="s">
+      <c r="K29" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L29" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M29" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L29" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M29" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N29" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O29" s="65"/>
       <c r="P29" s="65" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="139" t="s">
-        <v>491</v>
-      </c>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="133"/>
       <c r="C30" s="65"/>
-      <c r="D30" s="137" t="s">
-        <v>492</v>
+      <c r="D30" s="135" t="s">
+        <v>611</v>
       </c>
       <c r="E30" s="64"/>
       <c r="F30" s="64"/>
@@ -12780,30 +13004,30 @@
       <c r="J30" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K30" s="64" t="s">
+      <c r="K30" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L30" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M30" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L30" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M30" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N30" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O30" s="65"/>
       <c r="P30" s="65" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="139" t="s">
-        <v>493</v>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="133" t="s">
+        <v>445</v>
       </c>
       <c r="C31" s="65"/>
-      <c r="D31" s="137" t="s">
-        <v>494</v>
+      <c r="D31" s="135" t="s">
+        <v>612</v>
       </c>
       <c r="E31" s="64"/>
       <c r="F31" s="64"/>
@@ -12813,30 +13037,28 @@
       <c r="J31" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K31" s="64" t="s">
+      <c r="K31" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L31" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M31" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L31" s="64" t="s">
-        <v>478</v>
-      </c>
-      <c r="M31" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N31" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O31" s="65"/>
       <c r="P31" s="65" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="139" t="s">
-        <v>495</v>
-      </c>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="133"/>
       <c r="C32" s="65"/>
-      <c r="D32" s="137" t="s">
-        <v>496</v>
+      <c r="D32" s="135" t="s">
+        <v>613</v>
       </c>
       <c r="E32" s="64"/>
       <c r="F32" s="64"/>
@@ -12846,30 +13068,28 @@
       <c r="J32" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K32" s="64" t="s">
+      <c r="K32" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L32" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M32" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L32" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M32" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N32" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O32" s="65"/>
       <c r="P32" s="65" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="139" t="s">
-        <v>498</v>
-      </c>
+        <v>638</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="133"/>
       <c r="C33" s="65"/>
-      <c r="D33" s="137" t="s">
-        <v>499</v>
+      <c r="D33" s="135" t="s">
+        <v>614</v>
       </c>
       <c r="E33" s="64"/>
       <c r="F33" s="64"/>
@@ -12879,30 +13099,28 @@
       <c r="J33" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K33" s="64" t="s">
+      <c r="K33" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L33" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M33" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L33" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M33" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N33" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O33" s="65"/>
       <c r="P33" s="65" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="139" t="s">
-        <v>500</v>
-      </c>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="133"/>
       <c r="C34" s="65"/>
-      <c r="D34" s="137" t="s">
-        <v>501</v>
+      <c r="D34" s="135" t="s">
+        <v>615</v>
       </c>
       <c r="E34" s="64"/>
       <c r="F34" s="64"/>
@@ -12912,30 +13130,28 @@
       <c r="J34" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K34" s="64" t="s">
+      <c r="K34" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L34" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M34" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L34" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M34" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N34" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O34" s="65"/>
       <c r="P34" s="65" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="139" t="s">
-        <v>502</v>
-      </c>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="133"/>
       <c r="C35" s="65"/>
-      <c r="D35" s="137" t="s">
-        <v>503</v>
+      <c r="D35" s="135" t="s">
+        <v>616</v>
       </c>
       <c r="E35" s="64"/>
       <c r="F35" s="64"/>
@@ -12945,30 +13161,28 @@
       <c r="J35" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K35" s="64" t="s">
+      <c r="K35" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L35" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M35" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L35" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M35" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N35" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O35" s="65"/>
       <c r="P35" s="65" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="139" t="s">
-        <v>504</v>
-      </c>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="133"/>
       <c r="C36" s="65"/>
-      <c r="D36" s="137" t="s">
-        <v>505</v>
+      <c r="D36" s="135" t="s">
+        <v>617</v>
       </c>
       <c r="E36" s="64"/>
       <c r="F36" s="64"/>
@@ -12978,30 +13192,30 @@
       <c r="J36" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="K36" s="64" t="s">
+      <c r="K36" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="L36" s="140" t="s">
+        <v>585</v>
+      </c>
+      <c r="M36" s="138" t="s">
         <v>432</v>
-      </c>
-      <c r="L36" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M36" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N36" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O36" s="65"/>
       <c r="P36" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="139" t="s">
-        <v>506</v>
+        <v>642</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="133" t="s">
+        <v>447</v>
       </c>
       <c r="C37" s="65"/>
-      <c r="D37" s="137" t="s">
-        <v>507</v>
+      <c r="D37" s="131" t="s">
+        <v>558</v>
       </c>
       <c r="E37" s="64"/>
       <c r="F37" s="64"/>
@@ -13012,29 +13226,29 @@
         <v>204</v>
       </c>
       <c r="K37" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L37" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M37" s="64" t="s">
         <v>432</v>
-      </c>
-      <c r="L37" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M37" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N37" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O37" s="65"/>
       <c r="P37" s="65" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="38" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="139" t="s">
-        <v>508</v>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="133" t="s">
+        <v>449</v>
       </c>
       <c r="C38" s="65"/>
-      <c r="D38" s="137" t="s">
-        <v>509</v>
+      <c r="D38" s="131" t="s">
+        <v>559</v>
       </c>
       <c r="E38" s="64"/>
       <c r="F38" s="64"/>
@@ -13045,29 +13259,29 @@
         <v>204</v>
       </c>
       <c r="K38" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L38" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M38" s="64" t="s">
         <v>432</v>
-      </c>
-      <c r="L38" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M38" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N38" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O38" s="65"/>
       <c r="P38" s="65" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="133" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="139" t="s">
-        <v>510</v>
-      </c>
       <c r="C39" s="65"/>
-      <c r="D39" s="137" t="s">
-        <v>511</v>
+      <c r="D39" s="131" t="s">
+        <v>560</v>
       </c>
       <c r="E39" s="64"/>
       <c r="F39" s="64"/>
@@ -13078,29 +13292,29 @@
         <v>204</v>
       </c>
       <c r="K39" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L39" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M39" s="64" t="s">
         <v>432</v>
-      </c>
-      <c r="L39" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M39" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N39" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O39" s="65"/>
       <c r="P39" s="65" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="139" t="s">
-        <v>512</v>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="133" t="s">
+        <v>451</v>
       </c>
       <c r="C40" s="65"/>
-      <c r="D40" s="137" t="s">
-        <v>513</v>
+      <c r="D40" s="131" t="s">
+        <v>561</v>
       </c>
       <c r="E40" s="64"/>
       <c r="F40" s="64"/>
@@ -13111,109 +13325,902 @@
         <v>204</v>
       </c>
       <c r="K40" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L40" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M40" s="64" t="s">
         <v>432</v>
-      </c>
-      <c r="L40" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="M40" s="64" t="s">
-        <v>434</v>
       </c>
       <c r="N40" s="64" t="s">
         <v>220</v>
       </c>
       <c r="O40" s="65"/>
       <c r="P40" s="65" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="133" t="s">
+        <v>452</v>
+      </c>
+      <c r="C41" s="65"/>
+      <c r="D41" s="131" t="s">
+        <v>562</v>
+      </c>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K41" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L41" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M41" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N41" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O41" s="65"/>
+      <c r="P41" s="65" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="133" t="s">
+        <v>453</v>
+      </c>
+      <c r="C42" s="65"/>
+      <c r="D42" s="131" t="s">
+        <v>563</v>
+      </c>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="64"/>
+      <c r="J42" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K42" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L42" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M42" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N42" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O42" s="65"/>
+      <c r="P42" s="65" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="133" t="s">
+        <v>454</v>
+      </c>
+      <c r="C43" s="65"/>
+      <c r="D43" s="131" t="s">
+        <v>564</v>
+      </c>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K43" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L43" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M43" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N43" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O43" s="65"/>
+      <c r="P43" s="65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="133" t="s">
+        <v>455</v>
+      </c>
+      <c r="C44" s="65"/>
+      <c r="D44" s="131" t="s">
+        <v>565</v>
+      </c>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K44" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L44" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M44" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N44" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O44" s="65"/>
+      <c r="P44" s="65" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="133" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="107"/>
-      <c r="C41" s="108"/>
-      <c r="D41" s="108"/>
-      <c r="E41" s="109"/>
-      <c r="F41" s="109"/>
-      <c r="G41" s="109"/>
-      <c r="H41" s="109"/>
-      <c r="I41" s="109"/>
-      <c r="J41" s="108"/>
-      <c r="K41" s="109"/>
-      <c r="L41" s="109"/>
-      <c r="M41" s="109"/>
-      <c r="N41" s="109"/>
-      <c r="O41" s="108"/>
-      <c r="P41" s="108"/>
-    </row>
-    <row r="42" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="89"/>
-      <c r="C42" s="91" t="s">
+      <c r="C45" s="65"/>
+      <c r="D45" s="131" t="s">
+        <v>566</v>
+      </c>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K45" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L45" s="64" t="s">
+        <v>448</v>
+      </c>
+      <c r="M45" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N45" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O45" s="65"/>
+      <c r="P45" s="65" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="133" t="s">
+        <v>457</v>
+      </c>
+      <c r="C46" s="65"/>
+      <c r="D46" s="131" t="s">
+        <v>567</v>
+      </c>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K46" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L46" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M46" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N46" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O46" s="65"/>
+      <c r="P46" s="65" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="133" t="s">
+        <v>459</v>
+      </c>
+      <c r="C47" s="65"/>
+      <c r="D47" s="131" t="s">
+        <v>568</v>
+      </c>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K47" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L47" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M47" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N47" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O47" s="65"/>
+      <c r="P47" s="65" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="133" t="s">
+        <v>460</v>
+      </c>
+      <c r="C48" s="65"/>
+      <c r="D48" s="131" t="s">
+        <v>569</v>
+      </c>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K48" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L48" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M48" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N48" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O48" s="65"/>
+      <c r="P48" s="65" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="133" t="s">
+        <v>461</v>
+      </c>
+      <c r="C49" s="65"/>
+      <c r="D49" s="131" t="s">
+        <v>570</v>
+      </c>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K49" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L49" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M49" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N49" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O49" s="65"/>
+      <c r="P49" s="65" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="133" t="s">
+        <v>462</v>
+      </c>
+      <c r="C50" s="65"/>
+      <c r="D50" s="131" t="s">
+        <v>571</v>
+      </c>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="64"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K50" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L50" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M50" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N50" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O50" s="65"/>
+      <c r="P50" s="65" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="133" t="s">
+        <v>463</v>
+      </c>
+      <c r="C51" s="65"/>
+      <c r="D51" s="131" t="s">
+        <v>572</v>
+      </c>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
+      <c r="H51" s="64"/>
+      <c r="I51" s="64"/>
+      <c r="J51" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K51" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L51" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M51" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N51" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O51" s="65"/>
+      <c r="P51" s="65" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="133" t="s">
+        <v>464</v>
+      </c>
+      <c r="C52" s="65"/>
+      <c r="D52" s="131" t="s">
+        <v>573</v>
+      </c>
+      <c r="E52" s="64"/>
+      <c r="F52" s="64"/>
+      <c r="G52" s="64"/>
+      <c r="H52" s="64"/>
+      <c r="I52" s="64"/>
+      <c r="J52" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K52" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L52" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M52" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N52" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O52" s="65"/>
+      <c r="P52" s="65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="133" t="s">
+        <v>465</v>
+      </c>
+      <c r="C53" s="65"/>
+      <c r="D53" s="131" t="s">
+        <v>574</v>
+      </c>
+      <c r="E53" s="64"/>
+      <c r="F53" s="64"/>
+      <c r="G53" s="64"/>
+      <c r="H53" s="64"/>
+      <c r="I53" s="64"/>
+      <c r="J53" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K53" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L53" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M53" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N53" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O53" s="65"/>
+      <c r="P53" s="65" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="133" t="s">
+        <v>466</v>
+      </c>
+      <c r="C54" s="65"/>
+      <c r="D54" s="131" t="s">
+        <v>575</v>
+      </c>
+      <c r="E54" s="64"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="64"/>
+      <c r="H54" s="64"/>
+      <c r="I54" s="64"/>
+      <c r="J54" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K54" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L54" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="M54" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N54" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O54" s="65"/>
+      <c r="P54" s="65" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="133" t="s">
+        <v>467</v>
+      </c>
+      <c r="C55" s="65"/>
+      <c r="D55" s="131" t="s">
+        <v>576</v>
+      </c>
+      <c r="E55" s="64"/>
+      <c r="F55" s="64"/>
+      <c r="G55" s="64"/>
+      <c r="H55" s="64"/>
+      <c r="I55" s="64"/>
+      <c r="J55" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K55" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L55" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M55" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N55" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O55" s="65"/>
+      <c r="P55" s="65" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="133" t="s">
+        <v>469</v>
+      </c>
+      <c r="C56" s="65"/>
+      <c r="D56" s="131" t="s">
+        <v>577</v>
+      </c>
+      <c r="E56" s="64"/>
+      <c r="F56" s="64"/>
+      <c r="G56" s="64"/>
+      <c r="H56" s="64"/>
+      <c r="I56" s="64"/>
+      <c r="J56" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K56" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L56" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M56" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N56" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O56" s="65"/>
+      <c r="P56" s="65" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="133" t="s">
+        <v>470</v>
+      </c>
+      <c r="C57" s="65"/>
+      <c r="D57" s="131" t="s">
+        <v>578</v>
+      </c>
+      <c r="E57" s="64"/>
+      <c r="F57" s="64"/>
+      <c r="G57" s="64"/>
+      <c r="H57" s="64"/>
+      <c r="I57" s="64"/>
+      <c r="J57" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K57" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L57" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M57" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N57" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O57" s="65"/>
+      <c r="P57" s="65" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="133" t="s">
+        <v>471</v>
+      </c>
+      <c r="C58" s="65"/>
+      <c r="D58" s="131" t="s">
+        <v>579</v>
+      </c>
+      <c r="E58" s="64"/>
+      <c r="F58" s="64"/>
+      <c r="G58" s="64"/>
+      <c r="H58" s="64"/>
+      <c r="I58" s="64"/>
+      <c r="J58" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K58" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L58" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M58" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N58" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O58" s="65"/>
+      <c r="P58" s="65" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="133" t="s">
+        <v>472</v>
+      </c>
+      <c r="C59" s="65"/>
+      <c r="D59" s="131" t="s">
+        <v>580</v>
+      </c>
+      <c r="E59" s="64"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="64"/>
+      <c r="H59" s="64"/>
+      <c r="I59" s="64"/>
+      <c r="J59" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K59" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L59" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M59" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N59" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O59" s="65"/>
+      <c r="P59" s="65" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="133" t="s">
+        <v>473</v>
+      </c>
+      <c r="C60" s="65"/>
+      <c r="D60" s="131" t="s">
+        <v>581</v>
+      </c>
+      <c r="E60" s="64"/>
+      <c r="F60" s="64"/>
+      <c r="G60" s="64"/>
+      <c r="H60" s="64"/>
+      <c r="I60" s="64"/>
+      <c r="J60" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K60" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L60" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M60" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N60" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O60" s="65"/>
+      <c r="P60" s="65" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="133" t="s">
+        <v>474</v>
+      </c>
+      <c r="C61" s="65"/>
+      <c r="D61" s="131" t="s">
+        <v>582</v>
+      </c>
+      <c r="E61" s="64"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="64"/>
+      <c r="H61" s="64"/>
+      <c r="I61" s="64"/>
+      <c r="J61" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K61" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L61" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M61" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N61" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O61" s="65"/>
+      <c r="P61" s="65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="133" t="s">
+        <v>475</v>
+      </c>
+      <c r="C62" s="65"/>
+      <c r="D62" s="131" t="s">
+        <v>583</v>
+      </c>
+      <c r="E62" s="64"/>
+      <c r="F62" s="64"/>
+      <c r="G62" s="64"/>
+      <c r="H62" s="64"/>
+      <c r="I62" s="64"/>
+      <c r="J62" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K62" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L62" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M62" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N62" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O62" s="65"/>
+      <c r="P62" s="65" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="133" t="s">
+        <v>476</v>
+      </c>
+      <c r="C63" s="65"/>
+      <c r="D63" s="131" t="s">
+        <v>584</v>
+      </c>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="64"/>
+      <c r="I63" s="64"/>
+      <c r="J63" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K63" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L63" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="M63" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N63" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O63" s="65"/>
+      <c r="P63" s="65" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="107"/>
+      <c r="C64" s="108"/>
+      <c r="D64" s="108"/>
+      <c r="E64" s="109"/>
+      <c r="F64" s="109"/>
+      <c r="G64" s="109"/>
+      <c r="H64" s="109"/>
+      <c r="I64" s="109"/>
+      <c r="J64" s="108"/>
+      <c r="K64" s="109"/>
+      <c r="L64" s="109"/>
+      <c r="M64" s="109"/>
+      <c r="N64" s="109"/>
+      <c r="O64" s="108"/>
+      <c r="P64" s="108"/>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B65" s="89"/>
+      <c r="C65" s="91" t="s">
         <v>297</v>
       </c>
-      <c r="D42" s="91"/>
-      <c r="E42" s="92">
+      <c r="D65" s="91"/>
+      <c r="E65" s="92">
         <v>0</v>
       </c>
-      <c r="F42" s="92">
+      <c r="F65" s="92">
         <v>0</v>
       </c>
-      <c r="G42" s="92">
+      <c r="G65" s="92">
         <v>0</v>
       </c>
-      <c r="H42" s="92">
+      <c r="H65" s="92">
         <v>0</v>
       </c>
-      <c r="I42" s="92">
+      <c r="I65" s="92">
         <v>0</v>
       </c>
-      <c r="J42" s="92">
+      <c r="J65" s="92">
         <v>36</v>
       </c>
-      <c r="K42" s="93"/>
-      <c r="L42" s="93"/>
-      <c r="M42" s="93"/>
-      <c r="N42" s="90"/>
-      <c r="O42" s="90"/>
-      <c r="P42" s="90"/>
-    </row>
-    <row r="43" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="90"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="93"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
-      <c r="L43" s="93"/>
-      <c r="M43" s="93"/>
-      <c r="N43" s="90"/>
-      <c r="O43" s="90"/>
-      <c r="P43" s="90"/>
-    </row>
-    <row r="44" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="90"/>
-      <c r="C44" s="90"/>
-      <c r="D44" s="93"/>
-      <c r="E44" s="94"/>
-      <c r="F44" s="94"/>
-      <c r="G44" s="94"/>
-      <c r="H44" s="94"/>
-      <c r="I44" s="94"/>
-      <c r="J44" s="95" t="s">
+      <c r="K65" s="93"/>
+      <c r="L65" s="93"/>
+      <c r="M65" s="93"/>
+      <c r="N65" s="90"/>
+      <c r="O65" s="90"/>
+      <c r="P65" s="90"/>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B66" s="90"/>
+      <c r="C66" s="91"/>
+      <c r="D66" s="93"/>
+      <c r="E66" s="93"/>
+      <c r="F66" s="93"/>
+      <c r="G66" s="93"/>
+      <c r="H66" s="93"/>
+      <c r="I66" s="93"/>
+      <c r="J66" s="93"/>
+      <c r="K66" s="93"/>
+      <c r="L66" s="93"/>
+      <c r="M66" s="93"/>
+      <c r="N66" s="90"/>
+      <c r="O66" s="90"/>
+      <c r="P66" s="90"/>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B67" s="90"/>
+      <c r="C67" s="90"/>
+      <c r="D67" s="93"/>
+      <c r="E67" s="94"/>
+      <c r="F67" s="94"/>
+      <c r="G67" s="94"/>
+      <c r="H67" s="94"/>
+      <c r="I67" s="94"/>
+      <c r="J67" s="95" t="s">
         <v>299</v>
       </c>
-      <c r="K44" s="96">
+      <c r="K67" s="96">
         <v>36</v>
       </c>
-      <c r="L44" s="93"/>
-      <c r="M44" s="93"/>
-      <c r="N44" s="90"/>
-      <c r="O44" s="90"/>
-      <c r="P44" s="90"/>
+      <c r="L67" s="93"/>
+      <c r="M67" s="93"/>
+      <c r="N67" s="90"/>
+      <c r="O67" s="90"/>
+      <c r="P67" s="90"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" location="'Metadatos V'!B4" xr:uid="{0BD1436B-6291-47FC-8FE2-9F631D4A5D8B}"/>
+    <hyperlink ref="D6" r:id="rId2" location="'Metadatos V'!B5" xr:uid="{98012A51-0003-4C45-ADC0-B25C4082F0F6}"/>
+    <hyperlink ref="D7" r:id="rId3" location="'Metadatos V'!B6" xr:uid="{09CB2D60-9401-469B-A76D-4B52FCF147E7}"/>
+    <hyperlink ref="D8" r:id="rId4" location="'Metadatos V'!B7" xr:uid="{06441420-AF16-4817-80DD-783F86540945}"/>
+    <hyperlink ref="D9" r:id="rId5" location="'Metadatos V'!B8" xr:uid="{A0128460-B47C-4750-BD62-F7D0DD2256CB}"/>
+    <hyperlink ref="D10" r:id="rId6" location="'Metadatos V'!B9" xr:uid="{88F31584-2C7F-4A2B-B050-9A2F5B51DAE3}"/>
+    <hyperlink ref="D11" r:id="rId7" location="'Metadatos V'!B10" xr:uid="{BFFCD561-ECA6-4E38-A05E-9E9D7C3E00E3}"/>
+    <hyperlink ref="D12" r:id="rId8" location="'Metadatos V'!B11" xr:uid="{622BBCCC-05B3-420D-BCE0-22E89EAB2F59}"/>
+    <hyperlink ref="D13" r:id="rId9" location="'Metadatos V'!B12" xr:uid="{86B5AC53-90B9-4298-8F17-CCA00DE85D36}"/>
+    <hyperlink ref="D14" r:id="rId10" location="'Metadatos V'!B13" xr:uid="{A1E1AE46-F14D-49E5-88B1-E1778D6E85EC}"/>
+    <hyperlink ref="D15" r:id="rId11" location="'Metadatos V'!B14" xr:uid="{E5A504A1-A0E7-41DB-BDC0-D3972E993224}"/>
+    <hyperlink ref="D16" r:id="rId12" location="'Metadatos V'!B15" xr:uid="{8AAA86F4-6B02-4767-BD7F-87D3FA8737F8}"/>
+    <hyperlink ref="D17" r:id="rId13" location="'Metadatos V'!B16" xr:uid="{D945EC01-224F-429C-91BE-A6AE3AF675EE}"/>
+    <hyperlink ref="D18" r:id="rId14" location="'Metadatos V'!B17" xr:uid="{F74010C6-48AF-421F-8CB5-9ECD4F69827F}"/>
+    <hyperlink ref="D19" r:id="rId15" location="'Metadatos V'!B18" xr:uid="{85B568FA-D77E-4E0C-A20C-16302F6445B6}"/>
+    <hyperlink ref="D20" r:id="rId16" location="'Metadatos V'!B19" xr:uid="{0D0AC1A1-23D3-4C7A-B9A6-95A52943F935}"/>
+    <hyperlink ref="D21" r:id="rId17" location="'Metadatos V'!B20" xr:uid="{91EB44F3-FDCD-446C-B423-521EC3E08CFC}"/>
+    <hyperlink ref="D22" r:id="rId18" location="'Metadatos V'!B21" xr:uid="{7CC451FE-01F6-4AAD-8761-EB362C8B93AB}"/>
+    <hyperlink ref="D23" r:id="rId19" location="'Metadatos V'!B22" xr:uid="{8E5B01BD-8506-4B2A-820D-3C8778A072C9}"/>
+    <hyperlink ref="D24" r:id="rId20" location="'Metadatos V'!B23" xr:uid="{B38C39CE-9F9F-4FE0-AACD-A1B4F3B69E2E}"/>
+    <hyperlink ref="D25" r:id="rId21" location="'Metadatos V'!B24" xr:uid="{66FB0936-72FB-40BF-9F43-22388C20062F}"/>
+    <hyperlink ref="D26" r:id="rId22" location="'Metadatos V'!B25" xr:uid="{5D379C2D-D0F3-4425-985E-CDEF94335E2E}"/>
+    <hyperlink ref="D27" r:id="rId23" location="'Metadatos V'!B26" xr:uid="{1249F71D-4AB4-4CD9-A227-C6B0F2C3B228}"/>
+    <hyperlink ref="D28" r:id="rId24" location="'Metadatos V'!B27" xr:uid="{4260577E-DC60-47E1-BAB4-568E61FA7E8A}"/>
+    <hyperlink ref="D29" r:id="rId25" location="'Metadatos V'!B28" xr:uid="{45141514-FCF0-4841-BEEE-BE087102CF59}"/>
+    <hyperlink ref="D30" r:id="rId26" location="'Metadatos V'!B29" xr:uid="{89EF11CF-14B3-4C98-9531-04E18ECDF7D1}"/>
+    <hyperlink ref="D31" r:id="rId27" location="'Metadatos V'!B30" xr:uid="{BA2E6FF6-DDEE-4EC6-B5C6-D5D998337350}"/>
+    <hyperlink ref="D32" r:id="rId28" location="'Metadatos V'!B31" xr:uid="{F2A50E4B-136B-44E5-8F43-847EBDD8F1AC}"/>
+    <hyperlink ref="D33" r:id="rId29" location="'Metadatos V'!B32" xr:uid="{F1D0BDE0-B3E8-4C6D-A376-FA6E21D2EE2D}"/>
+    <hyperlink ref="D34" r:id="rId30" location="'Metadatos V'!B33" xr:uid="{8FA923E8-C75C-4DAD-835A-7B7C5B507A30}"/>
+    <hyperlink ref="D35" r:id="rId31" location="'Metadatos V'!B34" xr:uid="{B5999E1E-211B-4435-BB6C-42AFE3F80781}"/>
+    <hyperlink ref="D36" r:id="rId32" location="'Metadatos V'!B35" xr:uid="{26BB993F-1B41-4033-BF0E-ED5CF3051DDC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -13245,7 +14252,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>514</v>
+        <v>477</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>409</v>
@@ -13341,14 +14348,14 @@
       <c r="P4" s="53"/>
     </row>
     <row r="5" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="126" t="s">
         <v>285</v>
       </c>
       <c r="C5" s="110" t="s">
-        <v>515</v>
-      </c>
-      <c r="D5" s="134" t="s">
-        <v>516</v>
+        <v>478</v>
+      </c>
+      <c r="D5" s="129" t="s">
+        <v>479</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
@@ -13366,18 +14373,18 @@
         <v>207</v>
       </c>
       <c r="N5" s="58" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O5" s="59"/>
       <c r="P5" s="56" t="s">
-        <v>518</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="140"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="65"/>
-      <c r="D6" s="135" t="s">
-        <v>519</v>
+      <c r="D6" s="130" t="s">
+        <v>482</v>
       </c>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
@@ -13395,22 +14402,22 @@
         <v>207</v>
       </c>
       <c r="N6" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O6" s="65"/>
       <c r="P6" s="62" t="s">
-        <v>520</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="132" t="s">
+      <c r="B7" s="127" t="s">
         <v>292</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>515</v>
-      </c>
-      <c r="D7" s="135" t="s">
-        <v>521</v>
+        <v>478</v>
+      </c>
+      <c r="D7" s="130" t="s">
+        <v>484</v>
       </c>
       <c r="E7" s="64"/>
       <c r="F7" s="64"/>
@@ -13428,20 +14435,20 @@
         <v>207</v>
       </c>
       <c r="N7" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O7" s="65"/>
       <c r="P7" s="62" t="s">
-        <v>522</v>
+        <v>485</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="140"/>
+      <c r="B8" s="134"/>
       <c r="C8" s="100">
         <v>2</v>
       </c>
-      <c r="D8" s="135" t="s">
-        <v>523</v>
+      <c r="D8" s="130" t="s">
+        <v>486</v>
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="64"/>
@@ -13459,20 +14466,20 @@
       </c>
       <c r="M8" s="64"/>
       <c r="N8" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O8" s="65"/>
       <c r="P8" s="62" t="s">
-        <v>524</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="140"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D9" s="135" t="s">
-        <v>525</v>
+      <c r="D9" s="130" t="s">
+        <v>488</v>
       </c>
       <c r="E9" s="64"/>
       <c r="F9" s="64"/>
@@ -13490,22 +14497,22 @@
       </c>
       <c r="M9" s="64"/>
       <c r="N9" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O9" s="65"/>
       <c r="P9" s="62" t="s">
-        <v>526</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="127" t="s">
         <v>419</v>
       </c>
       <c r="C10" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D10" s="135" t="s">
-        <v>527</v>
+      <c r="D10" s="130" t="s">
+        <v>490</v>
       </c>
       <c r="E10" s="64"/>
       <c r="F10" s="64"/>
@@ -13523,22 +14530,22 @@
       </c>
       <c r="M10" s="64"/>
       <c r="N10" s="64" t="s">
-        <v>528</v>
+        <v>491</v>
       </c>
       <c r="O10" s="65"/>
       <c r="P10" s="62" t="s">
-        <v>529</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="132" t="s">
+      <c r="B11" s="127" t="s">
         <v>423</v>
       </c>
       <c r="C11" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D11" s="135" t="s">
-        <v>530</v>
+      <c r="D11" s="130" t="s">
+        <v>493</v>
       </c>
       <c r="E11" s="64"/>
       <c r="F11" s="64"/>
@@ -13556,22 +14563,22 @@
       </c>
       <c r="M11" s="64"/>
       <c r="N11" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O11" s="65"/>
       <c r="P11" s="62" t="s">
-        <v>531</v>
+        <v>494</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="132" t="s">
-        <v>442</v>
+      <c r="B12" s="127" t="s">
+        <v>437</v>
       </c>
       <c r="C12" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D12" s="135" t="s">
-        <v>532</v>
+      <c r="D12" s="130" t="s">
+        <v>495</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -13591,16 +14598,16 @@
       <c r="N12" s="64"/>
       <c r="O12" s="65"/>
       <c r="P12" s="62" t="s">
-        <v>533</v>
+        <v>496</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="140"/>
+      <c r="B13" s="134"/>
       <c r="C13" s="100">
         <v>8</v>
       </c>
-      <c r="D13" s="135" t="s">
-        <v>534</v>
+      <c r="D13" s="130" t="s">
+        <v>497</v>
       </c>
       <c r="E13" s="64" t="s">
         <v>200</v>
@@ -13618,24 +14625,24 @@
         <v>207</v>
       </c>
       <c r="N13" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O13" s="65" t="s">
-        <v>535</v>
+        <v>498</v>
       </c>
       <c r="P13" s="62" t="s">
-        <v>536</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="132" t="s">
-        <v>445</v>
+      <c r="B14" s="127" t="s">
+        <v>439</v>
       </c>
       <c r="C14" s="100">
         <v>2</v>
       </c>
-      <c r="D14" s="135" t="s">
-        <v>537</v>
+      <c r="D14" s="130" t="s">
+        <v>500</v>
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
@@ -13653,20 +14660,20 @@
       </c>
       <c r="M14" s="64"/>
       <c r="N14" s="64" t="s">
-        <v>538</v>
+        <v>501</v>
       </c>
       <c r="O14" s="65"/>
       <c r="P14" s="62" t="s">
-        <v>539</v>
+        <v>502</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="140"/>
+      <c r="B15" s="134"/>
       <c r="C15" s="100" t="s">
-        <v>540</v>
-      </c>
-      <c r="D15" s="135" t="s">
-        <v>541</v>
+        <v>503</v>
+      </c>
+      <c r="D15" s="130" t="s">
+        <v>504</v>
       </c>
       <c r="E15" s="64"/>
       <c r="F15" s="64"/>
@@ -13684,16 +14691,16 @@
       <c r="N15" s="64"/>
       <c r="O15" s="65"/>
       <c r="P15" s="62" t="s">
-        <v>542</v>
+        <v>505</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="140"/>
+      <c r="B16" s="134"/>
       <c r="C16" s="100" t="s">
-        <v>540</v>
-      </c>
-      <c r="D16" s="135" t="s">
-        <v>543</v>
+        <v>503</v>
+      </c>
+      <c r="D16" s="130" t="s">
+        <v>506</v>
       </c>
       <c r="E16" s="64"/>
       <c r="F16" s="64"/>
@@ -13711,18 +14718,18 @@
       <c r="N16" s="64"/>
       <c r="O16" s="65"/>
       <c r="P16" s="62" t="s">
-        <v>544</v>
+        <v>507</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="132" t="s">
-        <v>448</v>
+      <c r="B17" s="127" t="s">
+        <v>441</v>
       </c>
       <c r="C17" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D17" s="135" t="s">
-        <v>545</v>
+      <c r="D17" s="130" t="s">
+        <v>508</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="64"/>
@@ -13740,22 +14747,22 @@
       </c>
       <c r="M17" s="64"/>
       <c r="N17" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O17" s="65"/>
       <c r="P17" s="62" t="s">
-        <v>546</v>
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="132" t="s">
-        <v>451</v>
+      <c r="B18" s="127" t="s">
+        <v>443</v>
       </c>
       <c r="C18" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D18" s="135" t="s">
-        <v>547</v>
+      <c r="D18" s="130" t="s">
+        <v>510</v>
       </c>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
@@ -13773,20 +14780,20 @@
         <v>207</v>
       </c>
       <c r="N18" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O18" s="65"/>
       <c r="P18" s="62" t="s">
-        <v>548</v>
+        <v>511</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="132"/>
+      <c r="B19" s="127"/>
       <c r="C19" s="100">
         <v>1</v>
       </c>
-      <c r="D19" s="135" t="s">
-        <v>549</v>
+      <c r="D19" s="130" t="s">
+        <v>512</v>
       </c>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
@@ -13804,22 +14811,22 @@
         <v>207</v>
       </c>
       <c r="N19" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O19" s="65"/>
       <c r="P19" s="62" t="s">
-        <v>550</v>
+        <v>513</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="132" t="s">
-        <v>454</v>
+      <c r="B20" s="127" t="s">
+        <v>445</v>
       </c>
       <c r="C20" s="100">
         <v>1</v>
       </c>
-      <c r="D20" s="135" t="s">
-        <v>551</v>
+      <c r="D20" s="130" t="s">
+        <v>514</v>
       </c>
       <c r="E20" s="64"/>
       <c r="F20" s="64"/>
@@ -13837,22 +14844,22 @@
         <v>207</v>
       </c>
       <c r="N20" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O20" s="65"/>
       <c r="P20" s="62" t="s">
-        <v>552</v>
+        <v>515</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="132" t="s">
-        <v>553</v>
+      <c r="B21" s="127" t="s">
+        <v>516</v>
       </c>
       <c r="C21" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D21" s="135" t="s">
-        <v>554</v>
+      <c r="D21" s="130" t="s">
+        <v>517</v>
       </c>
       <c r="E21" s="64"/>
       <c r="F21" s="64"/>
@@ -13870,22 +14877,22 @@
         <v>207</v>
       </c>
       <c r="N21" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O21" s="65"/>
       <c r="P21" s="62" t="s">
-        <v>555</v>
+        <v>518</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="132" t="s">
-        <v>556</v>
+      <c r="B22" s="127" t="s">
+        <v>519</v>
       </c>
       <c r="C22" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D22" s="135" t="s">
-        <v>554</v>
+      <c r="D22" s="130" t="s">
+        <v>517</v>
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="64"/>
@@ -13903,22 +14910,22 @@
         <v>207</v>
       </c>
       <c r="N22" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O22" s="65"/>
       <c r="P22" s="62" t="s">
-        <v>557</v>
+        <v>520</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="132" t="s">
-        <v>558</v>
+      <c r="B23" s="127" t="s">
+        <v>521</v>
       </c>
       <c r="C23" s="100">
         <v>2</v>
       </c>
-      <c r="D23" s="135" t="s">
-        <v>559</v>
+      <c r="D23" s="130" t="s">
+        <v>522</v>
       </c>
       <c r="E23" s="64" t="s">
         <v>200</v>
@@ -13936,20 +14943,20 @@
         <v>207</v>
       </c>
       <c r="N23" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O23" s="65"/>
       <c r="P23" s="62" t="s">
-        <v>560</v>
+        <v>523</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="140"/>
+      <c r="B24" s="134"/>
       <c r="C24" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D24" s="135" t="s">
-        <v>561</v>
+      <c r="D24" s="130" t="s">
+        <v>524</v>
       </c>
       <c r="E24" s="64"/>
       <c r="F24" s="64"/>
@@ -13967,20 +14974,20 @@
         <v>207</v>
       </c>
       <c r="N24" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O24" s="65"/>
       <c r="P24" s="62" t="s">
-        <v>562</v>
+        <v>525</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="140"/>
+      <c r="B25" s="134"/>
       <c r="C25" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D25" s="135" t="s">
-        <v>563</v>
+      <c r="D25" s="130" t="s">
+        <v>526</v>
       </c>
       <c r="E25" s="64"/>
       <c r="F25" s="64"/>
@@ -13998,22 +15005,22 @@
         <v>207</v>
       </c>
       <c r="N25" s="64" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="O25" s="65"/>
       <c r="P25" s="62" t="s">
-        <v>564</v>
+        <v>527</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="140" t="s">
-        <v>565</v>
+      <c r="B26" s="134" t="s">
+        <v>528</v>
       </c>
       <c r="C26" s="100">
         <v>1</v>
       </c>
-      <c r="D26" s="135" t="s">
-        <v>566</v>
+      <c r="D26" s="130" t="s">
+        <v>529</v>
       </c>
       <c r="E26" s="64"/>
       <c r="F26" s="64"/>
@@ -14031,22 +15038,22 @@
         <v>207</v>
       </c>
       <c r="N26" s="64" t="s">
-        <v>567</v>
+        <v>530</v>
       </c>
       <c r="O26" s="65"/>
       <c r="P26" s="62" t="s">
-        <v>568</v>
+        <v>531</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="140" t="s">
-        <v>569</v>
+      <c r="B27" s="134" t="s">
+        <v>532</v>
       </c>
       <c r="C27" s="100" t="s">
         <v>420</v>
       </c>
-      <c r="D27" s="135" t="s">
-        <v>570</v>
+      <c r="D27" s="130" t="s">
+        <v>533</v>
       </c>
       <c r="E27" s="64"/>
       <c r="F27" s="64"/>
@@ -14066,16 +15073,16 @@
       <c r="N27" s="64"/>
       <c r="O27" s="65"/>
       <c r="P27" s="62" t="s">
-        <v>571</v>
+        <v>534</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="140" t="s">
-        <v>572</v>
+      <c r="B28" s="134" t="s">
+        <v>535</v>
       </c>
       <c r="C28" s="65"/>
-      <c r="D28" s="135" t="s">
-        <v>573</v>
+      <c r="D28" s="130" t="s">
+        <v>536</v>
       </c>
       <c r="E28" s="64"/>
       <c r="F28" s="64"/>
@@ -14093,16 +15100,16 @@
       <c r="N28" s="64"/>
       <c r="O28" s="65"/>
       <c r="P28" s="62" t="s">
-        <v>574</v>
+        <v>537</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="140" t="s">
-        <v>575</v>
+      <c r="B29" s="134" t="s">
+        <v>538</v>
       </c>
       <c r="C29" s="65"/>
-      <c r="D29" s="135" t="s">
-        <v>576</v>
+      <c r="D29" s="130" t="s">
+        <v>539</v>
       </c>
       <c r="E29" s="64"/>
       <c r="F29" s="64"/>
@@ -14120,16 +15127,16 @@
       <c r="N29" s="64"/>
       <c r="O29" s="65"/>
       <c r="P29" s="62" t="s">
-        <v>577</v>
+        <v>540</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="140" t="s">
-        <v>578</v>
+      <c r="B30" s="134" t="s">
+        <v>541</v>
       </c>
       <c r="C30" s="65"/>
-      <c r="D30" s="135" t="s">
-        <v>579</v>
+      <c r="D30" s="130" t="s">
+        <v>542</v>
       </c>
       <c r="E30" s="64" t="s">
         <v>200</v>
@@ -14147,16 +15154,16 @@
       <c r="N30" s="64"/>
       <c r="O30" s="65"/>
       <c r="P30" s="62" t="s">
-        <v>580</v>
+        <v>543</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="140" t="s">
-        <v>581</v>
+      <c r="B31" s="134" t="s">
+        <v>544</v>
       </c>
       <c r="C31" s="65"/>
-      <c r="D31" s="135" t="s">
-        <v>582</v>
+      <c r="D31" s="130" t="s">
+        <v>545</v>
       </c>
       <c r="E31" s="64" t="s">
         <v>200</v>
@@ -14173,19 +15180,19 @@
       <c r="M31" s="64"/>
       <c r="N31" s="64"/>
       <c r="O31" s="65" t="s">
-        <v>535</v>
+        <v>498</v>
       </c>
       <c r="P31" s="62" t="s">
-        <v>583</v>
+        <v>546</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="140" t="s">
-        <v>584</v>
+      <c r="B32" s="134" t="s">
+        <v>547</v>
       </c>
       <c r="C32" s="65"/>
-      <c r="D32" s="135" t="s">
-        <v>585</v>
+      <c r="D32" s="130" t="s">
+        <v>548</v>
       </c>
       <c r="E32" s="64" t="s">
         <v>200</v>
@@ -14202,19 +15209,19 @@
       <c r="M32" s="64"/>
       <c r="N32" s="64"/>
       <c r="O32" s="65" t="s">
-        <v>535</v>
+        <v>498</v>
       </c>
       <c r="P32" s="62" t="s">
-        <v>586</v>
+        <v>549</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="140" t="s">
-        <v>587</v>
+      <c r="B33" s="134" t="s">
+        <v>550</v>
       </c>
       <c r="C33" s="65"/>
-      <c r="D33" s="135" t="s">
-        <v>588</v>
+      <c r="D33" s="130" t="s">
+        <v>551</v>
       </c>
       <c r="E33" s="64"/>
       <c r="F33" s="64"/>
@@ -14232,7 +15239,7 @@
       <c r="N33" s="64"/>
       <c r="O33" s="65"/>
       <c r="P33" s="62" t="s">
-        <v>589</v>
+        <v>552</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cocodrila sounds included in Game/media/audio/voices. Cuesheet and metadata table updated
</commit_message>
<xml_diff>
--- a/Docs/TDS/CueSheet.xlsx
+++ b/Docs/TDS/CueSheet.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="664">
   <si>
     <t>Cue-Sheets</t>
   </si>
@@ -1498,9 +1498,6 @@
     <t>2.1</t>
   </si>
   <si>
-    <t>Personaje 2</t>
-  </si>
-  <si>
     <t>2.2</t>
   </si>
   <si>
@@ -1828,33 +1825,6 @@
     <t>Musica de fondo del nivel 1</t>
   </si>
   <si>
-    <t>V-210 V-215</t>
-  </si>
-  <si>
-    <t>V-220 V-225</t>
-  </si>
-  <si>
-    <t>V-230 V-235</t>
-  </si>
-  <si>
-    <t>V-240 V-245</t>
-  </si>
-  <si>
-    <t>V-250 V-255</t>
-  </si>
-  <si>
-    <t>V-260 V-265</t>
-  </si>
-  <si>
-    <t>V-270 V-275</t>
-  </si>
-  <si>
-    <t>V-280 V-285</t>
-  </si>
-  <si>
-    <t>V-290 V-295</t>
-  </si>
-  <si>
     <t>V-310 V-315</t>
   </si>
   <si>
@@ -2081,6 +2051,99 @@
   </si>
   <si>
     <t>Acelerón 2 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Cocodrila</t>
+  </si>
+  <si>
+    <t>V-210</t>
+  </si>
+  <si>
+    <t>V-211</t>
+  </si>
+  <si>
+    <t>V-215</t>
+  </si>
+  <si>
+    <t>V-220</t>
+  </si>
+  <si>
+    <t>V-221</t>
+  </si>
+  <si>
+    <t>V-225</t>
+  </si>
+  <si>
+    <t>V-226</t>
+  </si>
+  <si>
+    <t>V-230</t>
+  </si>
+  <si>
+    <t>V-235</t>
+  </si>
+  <si>
+    <t>V-236</t>
+  </si>
+  <si>
+    <t>V-240</t>
+  </si>
+  <si>
+    <t>V-241</t>
+  </si>
+  <si>
+    <t>V-245</t>
+  </si>
+  <si>
+    <t>V-246</t>
+  </si>
+  <si>
+    <t>V-250</t>
+  </si>
+  <si>
+    <t>V-255</t>
+  </si>
+  <si>
+    <t>V-260</t>
+  </si>
+  <si>
+    <t>V-261</t>
+  </si>
+  <si>
+    <t>V-265</t>
+  </si>
+  <si>
+    <t>V-266</t>
+  </si>
+  <si>
+    <t>V-270</t>
+  </si>
+  <si>
+    <t>V-271</t>
+  </si>
+  <si>
+    <t>V-275</t>
+  </si>
+  <si>
+    <t>V-280</t>
+  </si>
+  <si>
+    <t>V-285</t>
+  </si>
+  <si>
+    <t>V-290</t>
+  </si>
+  <si>
+    <t>V-295</t>
+  </si>
+  <si>
+    <t>Voz de selección 1</t>
+  </si>
+  <si>
+    <t>Voz emitida cuando haya un choque 1 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Victoria 1</t>
   </si>
 </sst>
 </file>
@@ -3252,6 +3315,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3266,9 +3332,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4177,27 +4240,27 @@
         <v>15</v>
       </c>
       <c r="C7" s="17">
-        <f>Personajes!E65</f>
+        <f>Personajes!E83</f>
         <v>0</v>
       </c>
       <c r="D7" s="17">
-        <f>Personajes!F65</f>
+        <f>Personajes!F83</f>
         <v>0</v>
       </c>
       <c r="E7" s="17">
-        <f>Personajes!G65</f>
+        <f>Personajes!G83</f>
         <v>0</v>
       </c>
       <c r="F7" s="17">
-        <f>Personajes!H65</f>
+        <f>Personajes!H83</f>
         <v>0</v>
       </c>
       <c r="G7" s="17">
-        <f>Personajes!I65</f>
+        <f>Personajes!I83</f>
         <v>0</v>
       </c>
       <c r="H7" s="17">
-        <f>Personajes!J65</f>
+        <f>Personajes!J83</f>
         <v>36</v>
       </c>
       <c r="I7" s="18">
@@ -4330,7 +4393,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>409</v>
@@ -4408,7 +4471,7 @@
     </row>
     <row r="4" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="49"/>
@@ -4433,7 +4496,7 @@
         <v>414</v>
       </c>
       <c r="D5" s="129" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>200</v>
@@ -4450,10 +4513,10 @@
       <c r="M5" s="57"/>
       <c r="N5" s="57"/>
       <c r="O5" s="56" t="s">
+        <v>555</v>
+      </c>
+      <c r="P5" s="56" t="s">
         <v>556</v>
-      </c>
-      <c r="P5" s="56" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4795,82 +4858,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
+      <c r="M1" s="147"/>
+      <c r="N1" s="147"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="146"/>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="146"/>
-      <c r="N2" s="146"/>
+      <c r="A2" s="147"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="147"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="147" t="s">
+      <c r="A3" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="148" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="148" t="s">
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="149" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="147" t="s">
+      <c r="G3" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="147" t="s">
+      <c r="H3" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="147" t="s">
+      <c r="I3" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="147" t="s">
+      <c r="J3" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="147" t="s">
+      <c r="K3" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="147" t="s">
+      <c r="L3" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="147" t="s">
+      <c r="M3" s="148" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="148" t="s">
+      <c r="N3" s="149" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="147"/>
-      <c r="B4" s="147"/>
+      <c r="A4" s="148"/>
+      <c r="B4" s="148"/>
       <c r="C4" s="27" t="s">
         <v>31</v>
       </c>
@@ -4880,15 +4943,15 @@
       <c r="E4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="148"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="148"/>
+      <c r="F4" s="149"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
+      <c r="M4" s="148"/>
+      <c r="N4" s="149"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -6956,79 +7019,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="147" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
+      <c r="M1" s="147"/>
+      <c r="N1" s="147"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="146"/>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="146"/>
-      <c r="N2" s="146"/>
+      <c r="A2" s="147"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="147"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="148" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="148" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147" t="s">
+      <c r="E3" s="148"/>
+      <c r="F3" s="148"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148" t="s">
         <v>194</v>
       </c>
-      <c r="J3" s="147" t="s">
+      <c r="J3" s="148" t="s">
         <v>195</v>
       </c>
-      <c r="K3" s="147" t="s">
+      <c r="K3" s="148" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="147" t="s">
+      <c r="L3" s="148" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="147" t="s">
+      <c r="M3" s="148" t="s">
         <v>198</v>
       </c>
-      <c r="N3" s="147" t="s">
+      <c r="N3" s="148" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="148"/>
-      <c r="B4" s="147"/>
-      <c r="C4" s="147"/>
+      <c r="A4" s="149"/>
+      <c r="B4" s="148"/>
+      <c r="C4" s="148"/>
       <c r="D4" s="27" t="s">
         <v>200</v>
       </c>
@@ -7044,12 +7107,12 @@
       <c r="H4" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="147"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
+      <c r="M4" s="148"/>
+      <c r="N4" s="148"/>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -9054,82 +9117,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="147" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
+      <c r="M1" s="147"/>
+      <c r="N1" s="147"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="146"/>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="146"/>
-      <c r="N2" s="146"/>
+      <c r="A2" s="147"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="147"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="147" t="s">
+      <c r="A3" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="148" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149"/>
-      <c r="F3" s="150" t="s">
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="151" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="147" t="s">
+      <c r="G3" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="147" t="s">
+      <c r="H3" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="147" t="s">
+      <c r="I3" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="147" t="s">
+      <c r="J3" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="147" t="s">
+      <c r="K3" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="147" t="s">
+      <c r="L3" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="147" t="s">
+      <c r="M3" s="148" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="148" t="s">
+      <c r="N3" s="149" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="147"/>
-      <c r="B4" s="147"/>
+      <c r="A4" s="148"/>
+      <c r="B4" s="148"/>
       <c r="C4" s="97" t="s">
         <v>31</v>
       </c>
@@ -9139,15 +9202,15 @@
       <c r="E4" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="150"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="148"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
+      <c r="M4" s="148"/>
+      <c r="N4" s="149"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -10450,79 +10513,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="147" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-      <c r="L1" s="146"/>
-      <c r="M1" s="146"/>
-      <c r="N1" s="146"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
+      <c r="M1" s="147"/>
+      <c r="N1" s="147"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="146"/>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="146"/>
-      <c r="N2" s="146"/>
+      <c r="A2" s="147"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="147"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="148" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="148" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147" t="s">
+      <c r="E3" s="148"/>
+      <c r="F3" s="148"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148" t="s">
         <v>194</v>
       </c>
-      <c r="J3" s="147" t="s">
+      <c r="J3" s="148" t="s">
         <v>195</v>
       </c>
-      <c r="K3" s="147" t="s">
+      <c r="K3" s="148" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="147" t="s">
+      <c r="L3" s="148" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="147" t="s">
+      <c r="M3" s="148" t="s">
         <v>198</v>
       </c>
-      <c r="N3" s="147" t="s">
+      <c r="N3" s="148" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="148"/>
-      <c r="B4" s="147"/>
-      <c r="C4" s="147"/>
+      <c r="A4" s="149"/>
+      <c r="B4" s="148"/>
+      <c r="C4" s="148"/>
       <c r="D4" s="27" t="s">
         <v>200</v>
       </c>
@@ -10538,12 +10601,12 @@
       <c r="H4" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="147"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
+      <c r="M4" s="148"/>
+      <c r="N4" s="148"/>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
@@ -12079,10 +12142,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK67"/>
+  <dimension ref="A1:AMK85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+      <selection activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -12205,7 +12268,7 @@
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="143" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
@@ -12219,7 +12282,7 @@
         <v>431</v>
       </c>
       <c r="L5" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M5" s="138" t="s">
         <v>432</v>
@@ -12228,7 +12291,7 @@
         <v>220</v>
       </c>
       <c r="O5" s="59"/>
-      <c r="P5" s="151" t="s">
+      <c r="P5" s="146" t="s">
         <v>433</v>
       </c>
     </row>
@@ -12236,7 +12299,7 @@
       <c r="B6" s="141"/>
       <c r="C6" s="142"/>
       <c r="D6" s="144" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
       <c r="E6" s="139"/>
       <c r="F6" s="139"/>
@@ -12250,7 +12313,7 @@
         <v>431</v>
       </c>
       <c r="L6" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M6" s="138" t="s">
         <v>432</v>
@@ -12260,7 +12323,7 @@
       </c>
       <c r="O6" s="142"/>
       <c r="P6" s="142" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12269,7 +12332,7 @@
       </c>
       <c r="C7" s="65"/>
       <c r="D7" s="135" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="E7" s="64"/>
       <c r="F7" s="64"/>
@@ -12283,7 +12346,7 @@
         <v>431</v>
       </c>
       <c r="L7" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M7" s="138" t="s">
         <v>432</v>
@@ -12293,14 +12356,14 @@
       </c>
       <c r="O7" s="65"/>
       <c r="P7" s="65" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="133"/>
       <c r="C8" s="65"/>
       <c r="D8" s="135" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="64"/>
@@ -12314,7 +12377,7 @@
         <v>431</v>
       </c>
       <c r="L8" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M8" s="138" t="s">
         <v>432</v>
@@ -12324,14 +12387,14 @@
       </c>
       <c r="O8" s="65"/>
       <c r="P8" s="65" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="133"/>
       <c r="C9" s="65"/>
       <c r="D9" s="135" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="E9" s="64"/>
       <c r="F9" s="64"/>
@@ -12345,7 +12408,7 @@
         <v>431</v>
       </c>
       <c r="L9" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M9" s="138" t="s">
         <v>432</v>
@@ -12355,14 +12418,14 @@
       </c>
       <c r="O9" s="65"/>
       <c r="P9" s="65" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="133"/>
       <c r="C10" s="65"/>
       <c r="D10" s="135" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="E10" s="64"/>
       <c r="F10" s="64"/>
@@ -12376,7 +12439,7 @@
         <v>431</v>
       </c>
       <c r="L10" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M10" s="138" t="s">
         <v>432</v>
@@ -12386,14 +12449,14 @@
       </c>
       <c r="O10" s="65"/>
       <c r="P10" s="65" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="133"/>
       <c r="C11" s="65"/>
       <c r="D11" s="135" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="E11" s="64"/>
       <c r="F11" s="64"/>
@@ -12407,7 +12470,7 @@
         <v>431</v>
       </c>
       <c r="L11" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M11" s="138" t="s">
         <v>432</v>
@@ -12417,7 +12480,7 @@
       </c>
       <c r="O11" s="65"/>
       <c r="P11" s="65" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12426,7 +12489,7 @@
       </c>
       <c r="C12" s="65"/>
       <c r="D12" s="135" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -12440,7 +12503,7 @@
         <v>431</v>
       </c>
       <c r="L12" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M12" s="138" t="s">
         <v>432</v>
@@ -12457,7 +12520,7 @@
       <c r="B13" s="133"/>
       <c r="C13" s="65"/>
       <c r="D13" s="135" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="E13" s="64"/>
       <c r="F13" s="64"/>
@@ -12471,7 +12534,7 @@
         <v>431</v>
       </c>
       <c r="L13" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M13" s="138" t="s">
         <v>432</v>
@@ -12481,14 +12544,14 @@
       </c>
       <c r="O13" s="65"/>
       <c r="P13" s="65" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="133"/>
       <c r="C14" s="65"/>
       <c r="D14" s="135" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
@@ -12502,7 +12565,7 @@
         <v>431</v>
       </c>
       <c r="L14" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M14" s="138" t="s">
         <v>432</v>
@@ -12512,14 +12575,14 @@
       </c>
       <c r="O14" s="65"/>
       <c r="P14" s="65" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="133"/>
       <c r="C15" s="65"/>
       <c r="D15" s="135" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="E15" s="64"/>
       <c r="F15" s="64"/>
@@ -12533,7 +12596,7 @@
         <v>431</v>
       </c>
       <c r="L15" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M15" s="138" t="s">
         <v>432</v>
@@ -12543,7 +12606,7 @@
       </c>
       <c r="O15" s="65"/>
       <c r="P15" s="65" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12552,7 +12615,7 @@
       </c>
       <c r="C16" s="65"/>
       <c r="D16" s="135" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="E16" s="64"/>
       <c r="F16" s="64"/>
@@ -12566,7 +12629,7 @@
         <v>431</v>
       </c>
       <c r="L16" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M16" s="138" t="s">
         <v>432</v>
@@ -12576,14 +12639,14 @@
       </c>
       <c r="O16" s="65"/>
       <c r="P16" s="65" t="s">
-        <v>621</v>
+        <v>611</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="133"/>
       <c r="C17" s="65"/>
       <c r="D17" s="135" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="64"/>
@@ -12597,7 +12660,7 @@
         <v>431</v>
       </c>
       <c r="L17" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M17" s="138" t="s">
         <v>432</v>
@@ -12607,14 +12670,14 @@
       </c>
       <c r="O17" s="65"/>
       <c r="P17" s="65" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="133"/>
       <c r="C18" s="65"/>
       <c r="D18" s="135" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
@@ -12628,7 +12691,7 @@
         <v>431</v>
       </c>
       <c r="L18" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M18" s="138" t="s">
         <v>432</v>
@@ -12638,14 +12701,14 @@
       </c>
       <c r="O18" s="65"/>
       <c r="P18" s="65" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="133"/>
       <c r="C19" s="65"/>
       <c r="D19" s="135" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
@@ -12659,7 +12722,7 @@
         <v>431</v>
       </c>
       <c r="L19" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M19" s="138" t="s">
         <v>432</v>
@@ -12669,7 +12732,7 @@
       </c>
       <c r="O19" s="65"/>
       <c r="P19" s="65" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12678,7 +12741,7 @@
       </c>
       <c r="C20" s="65"/>
       <c r="D20" s="135" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="E20" s="64"/>
       <c r="F20" s="64"/>
@@ -12692,7 +12755,7 @@
         <v>431</v>
       </c>
       <c r="L20" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M20" s="138" t="s">
         <v>432</v>
@@ -12709,7 +12772,7 @@
       <c r="B21" s="133"/>
       <c r="C21" s="65"/>
       <c r="D21" s="135" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
       <c r="E21" s="64"/>
       <c r="F21" s="64"/>
@@ -12723,7 +12786,7 @@
         <v>431</v>
       </c>
       <c r="L21" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M21" s="138" t="s">
         <v>432</v>
@@ -12733,14 +12796,14 @@
       </c>
       <c r="O21" s="65"/>
       <c r="P21" s="65" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="133"/>
       <c r="C22" s="65"/>
       <c r="D22" s="135" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="64"/>
@@ -12754,7 +12817,7 @@
         <v>431</v>
       </c>
       <c r="L22" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M22" s="138" t="s">
         <v>432</v>
@@ -12764,14 +12827,14 @@
       </c>
       <c r="O22" s="65"/>
       <c r="P22" s="65" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="133"/>
       <c r="C23" s="65"/>
       <c r="D23" s="135" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
       <c r="E23" s="64"/>
       <c r="F23" s="64"/>
@@ -12785,7 +12848,7 @@
         <v>431</v>
       </c>
       <c r="L23" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M23" s="138" t="s">
         <v>432</v>
@@ -12795,7 +12858,7 @@
       </c>
       <c r="O23" s="65"/>
       <c r="P23" s="65" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12804,7 +12867,7 @@
       </c>
       <c r="C24" s="65"/>
       <c r="D24" s="135" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="E24" s="64"/>
       <c r="F24" s="64"/>
@@ -12818,7 +12881,7 @@
         <v>431</v>
       </c>
       <c r="L24" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M24" s="138" t="s">
         <v>432</v>
@@ -12835,7 +12898,7 @@
       <c r="B25" s="133"/>
       <c r="C25" s="65"/>
       <c r="D25" s="135" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="E25" s="64"/>
       <c r="F25" s="64"/>
@@ -12849,7 +12912,7 @@
         <v>431</v>
       </c>
       <c r="L25" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M25" s="138" t="s">
         <v>432</v>
@@ -12859,14 +12922,14 @@
       </c>
       <c r="O25" s="65"/>
       <c r="P25" s="65" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="133"/>
       <c r="C26" s="65"/>
       <c r="D26" s="135" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="E26" s="64"/>
       <c r="F26" s="64"/>
@@ -12880,7 +12943,7 @@
         <v>431</v>
       </c>
       <c r="L26" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M26" s="138" t="s">
         <v>432</v>
@@ -12890,7 +12953,7 @@
       </c>
       <c r="O26" s="65"/>
       <c r="P26" s="65" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12899,7 +12962,7 @@
       </c>
       <c r="C27" s="65"/>
       <c r="D27" s="135" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="E27" s="64"/>
       <c r="F27" s="64"/>
@@ -12913,7 +12976,7 @@
         <v>431</v>
       </c>
       <c r="L27" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M27" s="138" t="s">
         <v>432</v>
@@ -12930,7 +12993,7 @@
       <c r="B28" s="133"/>
       <c r="C28" s="65"/>
       <c r="D28" s="135" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="E28" s="64"/>
       <c r="F28" s="64"/>
@@ -12944,7 +13007,7 @@
         <v>431</v>
       </c>
       <c r="L28" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M28" s="138" t="s">
         <v>432</v>
@@ -12954,7 +13017,7 @@
       </c>
       <c r="O28" s="65"/>
       <c r="P28" s="65" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12963,7 +13026,7 @@
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="135" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="E29" s="64"/>
       <c r="F29" s="64"/>
@@ -12977,7 +13040,7 @@
         <v>431</v>
       </c>
       <c r="L29" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M29" s="138" t="s">
         <v>432</v>
@@ -12994,7 +13057,7 @@
       <c r="B30" s="133"/>
       <c r="C30" s="65"/>
       <c r="D30" s="135" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="E30" s="64"/>
       <c r="F30" s="64"/>
@@ -13008,7 +13071,7 @@
         <v>431</v>
       </c>
       <c r="L30" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M30" s="138" t="s">
         <v>432</v>
@@ -13018,7 +13081,7 @@
       </c>
       <c r="O30" s="65"/>
       <c r="P30" s="65" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13027,7 +13090,7 @@
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="135" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="E31" s="64"/>
       <c r="F31" s="64"/>
@@ -13041,7 +13104,7 @@
         <v>431</v>
       </c>
       <c r="L31" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M31" s="138" t="s">
         <v>432</v>
@@ -13058,7 +13121,7 @@
       <c r="B32" s="133"/>
       <c r="C32" s="65"/>
       <c r="D32" s="135" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="E32" s="64"/>
       <c r="F32" s="64"/>
@@ -13072,7 +13135,7 @@
         <v>431</v>
       </c>
       <c r="L32" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M32" s="138" t="s">
         <v>432</v>
@@ -13082,14 +13145,14 @@
       </c>
       <c r="O32" s="65"/>
       <c r="P32" s="65" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="133"/>
       <c r="C33" s="65"/>
       <c r="D33" s="135" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="E33" s="64"/>
       <c r="F33" s="64"/>
@@ -13103,7 +13166,7 @@
         <v>431</v>
       </c>
       <c r="L33" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M33" s="138" t="s">
         <v>432</v>
@@ -13113,14 +13176,14 @@
       </c>
       <c r="O33" s="65"/>
       <c r="P33" s="65" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="133"/>
       <c r="C34" s="65"/>
       <c r="D34" s="135" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="E34" s="64"/>
       <c r="F34" s="64"/>
@@ -13134,7 +13197,7 @@
         <v>431</v>
       </c>
       <c r="L34" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M34" s="138" t="s">
         <v>432</v>
@@ -13144,14 +13207,14 @@
       </c>
       <c r="O34" s="65"/>
       <c r="P34" s="65" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="133"/>
       <c r="C35" s="65"/>
       <c r="D35" s="135" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
       <c r="E35" s="64"/>
       <c r="F35" s="64"/>
@@ -13165,7 +13228,7 @@
         <v>431</v>
       </c>
       <c r="L35" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M35" s="138" t="s">
         <v>432</v>
@@ -13175,14 +13238,14 @@
       </c>
       <c r="O35" s="65"/>
       <c r="P35" s="65" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="133"/>
       <c r="C36" s="65"/>
       <c r="D36" s="135" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
       <c r="E36" s="64"/>
       <c r="F36" s="64"/>
@@ -13196,7 +13259,7 @@
         <v>431</v>
       </c>
       <c r="L36" s="140" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="M36" s="138" t="s">
         <v>432</v>
@@ -13206,16 +13269,16 @@
       </c>
       <c r="O36" s="65"/>
       <c r="P36" s="65" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="133" t="s">
         <v>447</v>
       </c>
       <c r="C37" s="65"/>
-      <c r="D37" s="131" t="s">
-        <v>558</v>
+      <c r="D37" s="135" t="s">
+        <v>634</v>
       </c>
       <c r="E37" s="64"/>
       <c r="F37" s="64"/>
@@ -13229,7 +13292,7 @@
         <v>431</v>
       </c>
       <c r="L37" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M37" s="64" t="s">
         <v>432</v>
@@ -13242,13 +13305,11 @@
         <v>433</v>
       </c>
     </row>
-    <row r="38" spans="2:16" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="133" t="s">
-        <v>449</v>
-      </c>
+    <row r="38" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="133"/>
       <c r="C38" s="65"/>
-      <c r="D38" s="131" t="s">
-        <v>559</v>
+      <c r="D38" s="135" t="s">
+        <v>635</v>
       </c>
       <c r="E38" s="64"/>
       <c r="F38" s="64"/>
@@ -13262,7 +13323,7 @@
         <v>431</v>
       </c>
       <c r="L38" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M38" s="64" t="s">
         <v>432</v>
@@ -13272,16 +13333,14 @@
       </c>
       <c r="O38" s="65"/>
       <c r="P38" s="65" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="133" t="s">
-        <v>450</v>
-      </c>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="133"/>
       <c r="C39" s="65"/>
-      <c r="D39" s="131" t="s">
-        <v>560</v>
+      <c r="D39" s="135" t="s">
+        <v>636</v>
       </c>
       <c r="E39" s="64"/>
       <c r="F39" s="64"/>
@@ -13295,7 +13354,7 @@
         <v>431</v>
       </c>
       <c r="L39" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M39" s="64" t="s">
         <v>432</v>
@@ -13305,16 +13364,16 @@
       </c>
       <c r="O39" s="65"/>
       <c r="P39" s="65" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="133" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C40" s="65"/>
-      <c r="D40" s="131" t="s">
-        <v>561</v>
+      <c r="D40" s="135" t="s">
+        <v>637</v>
       </c>
       <c r="E40" s="64"/>
       <c r="F40" s="64"/>
@@ -13328,7 +13387,7 @@
         <v>431</v>
       </c>
       <c r="L40" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M40" s="64" t="s">
         <v>432</v>
@@ -13338,16 +13397,14 @@
       </c>
       <c r="O40" s="65"/>
       <c r="P40" s="65" t="s">
-        <v>436</v>
+        <v>609</v>
       </c>
     </row>
     <row r="41" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="133" t="s">
-        <v>452</v>
-      </c>
+      <c r="B41" s="133"/>
       <c r="C41" s="65"/>
-      <c r="D41" s="131" t="s">
-        <v>562</v>
+      <c r="D41" s="135" t="s">
+        <v>638</v>
       </c>
       <c r="E41" s="64"/>
       <c r="F41" s="64"/>
@@ -13361,7 +13418,7 @@
         <v>431</v>
       </c>
       <c r="L41" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M41" s="64" t="s">
         <v>432</v>
@@ -13371,16 +13428,14 @@
       </c>
       <c r="O41" s="65"/>
       <c r="P41" s="65" t="s">
-        <v>438</v>
+        <v>612</v>
       </c>
     </row>
     <row r="42" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="133" t="s">
-        <v>453</v>
-      </c>
+      <c r="B42" s="133"/>
       <c r="C42" s="65"/>
-      <c r="D42" s="131" t="s">
-        <v>563</v>
+      <c r="D42" s="135" t="s">
+        <v>639</v>
       </c>
       <c r="E42" s="64"/>
       <c r="F42" s="64"/>
@@ -13394,7 +13449,7 @@
         <v>431</v>
       </c>
       <c r="L42" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M42" s="64" t="s">
         <v>432</v>
@@ -13404,16 +13459,14 @@
       </c>
       <c r="O42" s="65"/>
       <c r="P42" s="65" t="s">
-        <v>440</v>
+        <v>617</v>
       </c>
     </row>
     <row r="43" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="133" t="s">
-        <v>454</v>
-      </c>
+      <c r="B43" s="133"/>
       <c r="C43" s="65"/>
-      <c r="D43" s="131" t="s">
-        <v>564</v>
+      <c r="D43" s="135" t="s">
+        <v>640</v>
       </c>
       <c r="E43" s="64"/>
       <c r="F43" s="64"/>
@@ -13427,7 +13480,7 @@
         <v>431</v>
       </c>
       <c r="L43" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M43" s="64" t="s">
         <v>432</v>
@@ -13437,16 +13490,16 @@
       </c>
       <c r="O43" s="65"/>
       <c r="P43" s="65" t="s">
-        <v>442</v>
+        <v>618</v>
       </c>
     </row>
     <row r="44" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="133" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C44" s="65"/>
-      <c r="D44" s="131" t="s">
-        <v>565</v>
+      <c r="D44" s="135" t="s">
+        <v>641</v>
       </c>
       <c r="E44" s="64"/>
       <c r="F44" s="64"/>
@@ -13460,7 +13513,7 @@
         <v>431</v>
       </c>
       <c r="L44" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M44" s="64" t="s">
         <v>432</v>
@@ -13470,16 +13523,14 @@
       </c>
       <c r="O44" s="65"/>
       <c r="P44" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="133" t="s">
-        <v>456</v>
-      </c>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="133"/>
       <c r="C45" s="65"/>
-      <c r="D45" s="131" t="s">
-        <v>566</v>
+      <c r="D45" s="135" t="s">
+        <v>642</v>
       </c>
       <c r="E45" s="64"/>
       <c r="F45" s="64"/>
@@ -13493,7 +13544,7 @@
         <v>431</v>
       </c>
       <c r="L45" s="64" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="M45" s="64" t="s">
         <v>432</v>
@@ -13503,16 +13554,14 @@
       </c>
       <c r="O45" s="65"/>
       <c r="P45" s="65" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="133" t="s">
-        <v>457</v>
-      </c>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="133"/>
       <c r="C46" s="65"/>
-      <c r="D46" s="131" t="s">
-        <v>567</v>
+      <c r="D46" s="135" t="s">
+        <v>643</v>
       </c>
       <c r="E46" s="64"/>
       <c r="F46" s="64"/>
@@ -13526,7 +13575,7 @@
         <v>431</v>
       </c>
       <c r="L46" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M46" s="64" t="s">
         <v>432</v>
@@ -13536,16 +13585,16 @@
       </c>
       <c r="O46" s="65"/>
       <c r="P46" s="65" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="133" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="C47" s="65"/>
-      <c r="D47" s="131" t="s">
-        <v>568</v>
+      <c r="D47" s="135" t="s">
+        <v>644</v>
       </c>
       <c r="E47" s="64"/>
       <c r="F47" s="64"/>
@@ -13559,7 +13608,7 @@
         <v>431</v>
       </c>
       <c r="L47" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M47" s="64" t="s">
         <v>432</v>
@@ -13569,16 +13618,14 @@
       </c>
       <c r="O47" s="65"/>
       <c r="P47" s="65" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="48" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="133" t="s">
-        <v>460</v>
-      </c>
+        <v>611</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="133"/>
       <c r="C48" s="65"/>
-      <c r="D48" s="131" t="s">
-        <v>569</v>
+      <c r="D48" s="135" t="s">
+        <v>645</v>
       </c>
       <c r="E48" s="64"/>
       <c r="F48" s="64"/>
@@ -13592,7 +13639,7 @@
         <v>431</v>
       </c>
       <c r="L48" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M48" s="64" t="s">
         <v>432</v>
@@ -13602,16 +13649,14 @@
       </c>
       <c r="O48" s="65"/>
       <c r="P48" s="65" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="133" t="s">
-        <v>461</v>
-      </c>
+        <v>616</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="133"/>
       <c r="C49" s="65"/>
-      <c r="D49" s="131" t="s">
-        <v>570</v>
+      <c r="D49" s="135" t="s">
+        <v>646</v>
       </c>
       <c r="E49" s="64"/>
       <c r="F49" s="64"/>
@@ -13625,7 +13670,7 @@
         <v>431</v>
       </c>
       <c r="L49" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M49" s="64" t="s">
         <v>432</v>
@@ -13635,16 +13680,14 @@
       </c>
       <c r="O49" s="65"/>
       <c r="P49" s="65" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="133" t="s">
-        <v>462</v>
-      </c>
+        <v>619</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="133"/>
       <c r="C50" s="65"/>
-      <c r="D50" s="131" t="s">
-        <v>571</v>
+      <c r="D50" s="135" t="s">
+        <v>647</v>
       </c>
       <c r="E50" s="64"/>
       <c r="F50" s="64"/>
@@ -13658,7 +13701,7 @@
         <v>431</v>
       </c>
       <c r="L50" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M50" s="64" t="s">
         <v>432</v>
@@ -13668,16 +13711,16 @@
       </c>
       <c r="O50" s="65"/>
       <c r="P50" s="65" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="133" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="C51" s="65"/>
-      <c r="D51" s="131" t="s">
-        <v>572</v>
+      <c r="D51" s="135" t="s">
+        <v>648</v>
       </c>
       <c r="E51" s="64"/>
       <c r="F51" s="64"/>
@@ -13691,7 +13734,7 @@
         <v>431</v>
       </c>
       <c r="L51" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M51" s="64" t="s">
         <v>432</v>
@@ -13701,16 +13744,14 @@
       </c>
       <c r="O51" s="65"/>
       <c r="P51" s="65" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="133" t="s">
-        <v>464</v>
-      </c>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="133"/>
       <c r="C52" s="65"/>
-      <c r="D52" s="131" t="s">
-        <v>573</v>
+      <c r="D52" s="135" t="s">
+        <v>649</v>
       </c>
       <c r="E52" s="64"/>
       <c r="F52" s="64"/>
@@ -13724,7 +13765,7 @@
         <v>431</v>
       </c>
       <c r="L52" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M52" s="64" t="s">
         <v>432</v>
@@ -13734,16 +13775,16 @@
       </c>
       <c r="O52" s="65"/>
       <c r="P52" s="65" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="133" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="C53" s="65"/>
-      <c r="D53" s="131" t="s">
-        <v>574</v>
+      <c r="D53" s="135" t="s">
+        <v>650</v>
       </c>
       <c r="E53" s="64"/>
       <c r="F53" s="64"/>
@@ -13757,7 +13798,7 @@
         <v>431</v>
       </c>
       <c r="L53" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M53" s="64" t="s">
         <v>432</v>
@@ -13767,16 +13808,14 @@
       </c>
       <c r="O53" s="65"/>
       <c r="P53" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="54" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="133" t="s">
-        <v>466</v>
-      </c>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="133"/>
       <c r="C54" s="65"/>
-      <c r="D54" s="131" t="s">
-        <v>575</v>
+      <c r="D54" s="135" t="s">
+        <v>651</v>
       </c>
       <c r="E54" s="64"/>
       <c r="F54" s="64"/>
@@ -13790,7 +13829,7 @@
         <v>431</v>
       </c>
       <c r="L54" s="64" t="s">
-        <v>458</v>
+        <v>633</v>
       </c>
       <c r="M54" s="64" t="s">
         <v>432</v>
@@ -13800,16 +13839,14 @@
       </c>
       <c r="O54" s="65"/>
       <c r="P54" s="65" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="133" t="s">
-        <v>467</v>
-      </c>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="133"/>
       <c r="C55" s="65"/>
-      <c r="D55" s="131" t="s">
-        <v>576</v>
+      <c r="D55" s="135" t="s">
+        <v>652</v>
       </c>
       <c r="E55" s="64"/>
       <c r="F55" s="64"/>
@@ -13823,7 +13860,7 @@
         <v>431</v>
       </c>
       <c r="L55" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M55" s="64" t="s">
         <v>432</v>
@@ -13833,16 +13870,14 @@
       </c>
       <c r="O55" s="65"/>
       <c r="P55" s="65" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="56" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="133" t="s">
-        <v>469</v>
-      </c>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="133"/>
       <c r="C56" s="65"/>
-      <c r="D56" s="131" t="s">
-        <v>577</v>
+      <c r="D56" s="135" t="s">
+        <v>653</v>
       </c>
       <c r="E56" s="64"/>
       <c r="F56" s="64"/>
@@ -13856,7 +13891,7 @@
         <v>431</v>
       </c>
       <c r="L56" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M56" s="64" t="s">
         <v>432</v>
@@ -13866,16 +13901,16 @@
       </c>
       <c r="O56" s="65"/>
       <c r="P56" s="65" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="57" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="133" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C57" s="65"/>
-      <c r="D57" s="131" t="s">
-        <v>578</v>
+      <c r="D57" s="135" t="s">
+        <v>654</v>
       </c>
       <c r="E57" s="64"/>
       <c r="F57" s="64"/>
@@ -13889,7 +13924,7 @@
         <v>431</v>
       </c>
       <c r="L57" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M57" s="64" t="s">
         <v>432</v>
@@ -13899,16 +13934,14 @@
       </c>
       <c r="O57" s="65"/>
       <c r="P57" s="65" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="58" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="133" t="s">
-        <v>471</v>
-      </c>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="133"/>
       <c r="C58" s="65"/>
-      <c r="D58" s="131" t="s">
-        <v>579</v>
+      <c r="D58" s="135" t="s">
+        <v>655</v>
       </c>
       <c r="E58" s="64"/>
       <c r="F58" s="64"/>
@@ -13922,7 +13955,7 @@
         <v>431</v>
       </c>
       <c r="L58" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M58" s="64" t="s">
         <v>432</v>
@@ -13932,16 +13965,14 @@
       </c>
       <c r="O58" s="65"/>
       <c r="P58" s="65" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="133" t="s">
-        <v>472</v>
-      </c>
+        <v>663</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="133"/>
       <c r="C59" s="65"/>
-      <c r="D59" s="131" t="s">
-        <v>580</v>
+      <c r="D59" s="135" t="s">
+        <v>656</v>
       </c>
       <c r="E59" s="64"/>
       <c r="F59" s="64"/>
@@ -13955,7 +13986,7 @@
         <v>431</v>
       </c>
       <c r="L59" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M59" s="64" t="s">
         <v>432</v>
@@ -13965,16 +13996,16 @@
       </c>
       <c r="O59" s="65"/>
       <c r="P59" s="65" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="60" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="133" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="C60" s="65"/>
-      <c r="D60" s="131" t="s">
-        <v>581</v>
+      <c r="D60" s="135" t="s">
+        <v>657</v>
       </c>
       <c r="E60" s="64"/>
       <c r="F60" s="64"/>
@@ -13988,7 +14019,7 @@
         <v>431</v>
       </c>
       <c r="L60" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M60" s="64" t="s">
         <v>432</v>
@@ -13998,16 +14029,14 @@
       </c>
       <c r="O60" s="65"/>
       <c r="P60" s="65" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="61" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="133" t="s">
-        <v>474</v>
-      </c>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="133"/>
       <c r="C61" s="65"/>
-      <c r="D61" s="131" t="s">
-        <v>582</v>
+      <c r="D61" s="135" t="s">
+        <v>658</v>
       </c>
       <c r="E61" s="64"/>
       <c r="F61" s="64"/>
@@ -14021,7 +14050,7 @@
         <v>431</v>
       </c>
       <c r="L61" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M61" s="64" t="s">
         <v>432</v>
@@ -14031,16 +14060,16 @@
       </c>
       <c r="O61" s="65"/>
       <c r="P61" s="65" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="62" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="133" t="s">
-        <v>475</v>
+        <v>455</v>
       </c>
       <c r="C62" s="65"/>
-      <c r="D62" s="131" t="s">
-        <v>583</v>
+      <c r="D62" s="135" t="s">
+        <v>659</v>
       </c>
       <c r="E62" s="64"/>
       <c r="F62" s="64"/>
@@ -14054,7 +14083,7 @@
         <v>431</v>
       </c>
       <c r="L62" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M62" s="64" t="s">
         <v>432</v>
@@ -14064,16 +14093,14 @@
       </c>
       <c r="O62" s="65"/>
       <c r="P62" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="133" t="s">
-        <v>476</v>
-      </c>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="133"/>
       <c r="C63" s="65"/>
-      <c r="D63" s="131" t="s">
-        <v>584</v>
+      <c r="D63" s="135" t="s">
+        <v>660</v>
       </c>
       <c r="E63" s="64"/>
       <c r="F63" s="64"/>
@@ -14087,7 +14114,7 @@
         <v>431</v>
       </c>
       <c r="L63" s="64" t="s">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="M63" s="64" t="s">
         <v>432</v>
@@ -14097,94 +14124,688 @@
       </c>
       <c r="O63" s="65"/>
       <c r="P63" s="65" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="133" t="s">
+        <v>456</v>
+      </c>
+      <c r="C64" s="65"/>
+      <c r="D64" s="131" t="s">
+        <v>557</v>
+      </c>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="64"/>
+      <c r="H64" s="64"/>
+      <c r="I64" s="64"/>
+      <c r="J64" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K64" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L64" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M64" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N64" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O64" s="65"/>
+      <c r="P64" s="65" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="65" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="133" t="s">
+        <v>458</v>
+      </c>
+      <c r="C65" s="65"/>
+      <c r="D65" s="131" t="s">
+        <v>558</v>
+      </c>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="64"/>
+      <c r="I65" s="64"/>
+      <c r="J65" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K65" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L65" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M65" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N65" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O65" s="65"/>
+      <c r="P65" s="65" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="133" t="s">
+        <v>459</v>
+      </c>
+      <c r="C66" s="65"/>
+      <c r="D66" s="131" t="s">
+        <v>559</v>
+      </c>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="64"/>
+      <c r="H66" s="64"/>
+      <c r="I66" s="64"/>
+      <c r="J66" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K66" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L66" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M66" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N66" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O66" s="65"/>
+      <c r="P66" s="65" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="133" t="s">
+        <v>460</v>
+      </c>
+      <c r="C67" s="65"/>
+      <c r="D67" s="131" t="s">
+        <v>560</v>
+      </c>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="64"/>
+      <c r="I67" s="64"/>
+      <c r="J67" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K67" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L67" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M67" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N67" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O67" s="65"/>
+      <c r="P67" s="65" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="133" t="s">
+        <v>461</v>
+      </c>
+      <c r="C68" s="65"/>
+      <c r="D68" s="131" t="s">
+        <v>561</v>
+      </c>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="64"/>
+      <c r="H68" s="64"/>
+      <c r="I68" s="64"/>
+      <c r="J68" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K68" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L68" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M68" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N68" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O68" s="65"/>
+      <c r="P68" s="65" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="69" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="133" t="s">
+        <v>462</v>
+      </c>
+      <c r="C69" s="65"/>
+      <c r="D69" s="131" t="s">
+        <v>562</v>
+      </c>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="64"/>
+      <c r="H69" s="64"/>
+      <c r="I69" s="64"/>
+      <c r="J69" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K69" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L69" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M69" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N69" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O69" s="65"/>
+      <c r="P69" s="65" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="133" t="s">
+        <v>463</v>
+      </c>
+      <c r="C70" s="65"/>
+      <c r="D70" s="131" t="s">
+        <v>563</v>
+      </c>
+      <c r="E70" s="64"/>
+      <c r="F70" s="64"/>
+      <c r="G70" s="64"/>
+      <c r="H70" s="64"/>
+      <c r="I70" s="64"/>
+      <c r="J70" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K70" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L70" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M70" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N70" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O70" s="65"/>
+      <c r="P70" s="65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="71" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="133" t="s">
+        <v>464</v>
+      </c>
+      <c r="C71" s="65"/>
+      <c r="D71" s="131" t="s">
+        <v>564</v>
+      </c>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="64"/>
+      <c r="H71" s="64"/>
+      <c r="I71" s="64"/>
+      <c r="J71" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K71" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L71" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M71" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N71" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O71" s="65"/>
+      <c r="P71" s="65" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="72" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="133" t="s">
+        <v>465</v>
+      </c>
+      <c r="C72" s="65"/>
+      <c r="D72" s="131" t="s">
+        <v>565</v>
+      </c>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
+      <c r="H72" s="64"/>
+      <c r="I72" s="64"/>
+      <c r="J72" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K72" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L72" s="64" t="s">
+        <v>457</v>
+      </c>
+      <c r="M72" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N72" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O72" s="65"/>
+      <c r="P72" s="65" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="64" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="107"/>
-      <c r="C64" s="108"/>
-      <c r="D64" s="108"/>
-      <c r="E64" s="109"/>
-      <c r="F64" s="109"/>
-      <c r="G64" s="109"/>
-      <c r="H64" s="109"/>
-      <c r="I64" s="109"/>
-      <c r="J64" s="108"/>
-      <c r="K64" s="109"/>
-      <c r="L64" s="109"/>
-      <c r="M64" s="109"/>
-      <c r="N64" s="109"/>
-      <c r="O64" s="108"/>
-      <c r="P64" s="108"/>
-    </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B65" s="89"/>
-      <c r="C65" s="91" t="s">
+    <row r="73" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="133" t="s">
+        <v>466</v>
+      </c>
+      <c r="C73" s="65"/>
+      <c r="D73" s="131" t="s">
+        <v>566</v>
+      </c>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="64"/>
+      <c r="H73" s="64"/>
+      <c r="I73" s="64"/>
+      <c r="J73" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K73" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L73" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M73" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N73" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O73" s="65"/>
+      <c r="P73" s="65" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="133" t="s">
+        <v>468</v>
+      </c>
+      <c r="C74" s="65"/>
+      <c r="D74" s="131" t="s">
+        <v>567</v>
+      </c>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="64"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="64"/>
+      <c r="J74" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K74" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L74" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M74" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N74" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O74" s="65"/>
+      <c r="P74" s="65" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="133" t="s">
+        <v>469</v>
+      </c>
+      <c r="C75" s="65"/>
+      <c r="D75" s="131" t="s">
+        <v>568</v>
+      </c>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="64"/>
+      <c r="H75" s="64"/>
+      <c r="I75" s="64"/>
+      <c r="J75" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K75" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L75" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M75" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N75" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O75" s="65"/>
+      <c r="P75" s="65" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="133" t="s">
+        <v>470</v>
+      </c>
+      <c r="C76" s="65"/>
+      <c r="D76" s="131" t="s">
+        <v>569</v>
+      </c>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="64"/>
+      <c r="H76" s="64"/>
+      <c r="I76" s="64"/>
+      <c r="J76" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K76" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L76" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M76" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N76" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O76" s="65"/>
+      <c r="P76" s="65" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="133" t="s">
+        <v>471</v>
+      </c>
+      <c r="C77" s="65"/>
+      <c r="D77" s="131" t="s">
+        <v>570</v>
+      </c>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="64"/>
+      <c r="H77" s="64"/>
+      <c r="I77" s="64"/>
+      <c r="J77" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K77" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L77" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M77" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N77" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O77" s="65"/>
+      <c r="P77" s="65" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="133" t="s">
+        <v>472</v>
+      </c>
+      <c r="C78" s="65"/>
+      <c r="D78" s="131" t="s">
+        <v>571</v>
+      </c>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="64"/>
+      <c r="H78" s="64"/>
+      <c r="I78" s="64"/>
+      <c r="J78" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K78" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L78" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M78" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N78" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O78" s="65"/>
+      <c r="P78" s="65" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="133" t="s">
+        <v>473</v>
+      </c>
+      <c r="C79" s="65"/>
+      <c r="D79" s="131" t="s">
+        <v>572</v>
+      </c>
+      <c r="E79" s="64"/>
+      <c r="F79" s="64"/>
+      <c r="G79" s="64"/>
+      <c r="H79" s="64"/>
+      <c r="I79" s="64"/>
+      <c r="J79" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K79" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L79" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M79" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N79" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O79" s="65"/>
+      <c r="P79" s="65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="133" t="s">
+        <v>474</v>
+      </c>
+      <c r="C80" s="65"/>
+      <c r="D80" s="131" t="s">
+        <v>573</v>
+      </c>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="64"/>
+      <c r="H80" s="64"/>
+      <c r="I80" s="64"/>
+      <c r="J80" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K80" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L80" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M80" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N80" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O80" s="65"/>
+      <c r="P80" s="65" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="133" t="s">
+        <v>475</v>
+      </c>
+      <c r="C81" s="65"/>
+      <c r="D81" s="131" t="s">
+        <v>574</v>
+      </c>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="64"/>
+      <c r="H81" s="64"/>
+      <c r="I81" s="64"/>
+      <c r="J81" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K81" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L81" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="M81" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N81" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O81" s="65"/>
+      <c r="P81" s="65" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="82" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="107"/>
+      <c r="C82" s="108"/>
+      <c r="D82" s="108"/>
+      <c r="E82" s="109"/>
+      <c r="F82" s="109"/>
+      <c r="G82" s="109"/>
+      <c r="H82" s="109"/>
+      <c r="I82" s="109"/>
+      <c r="J82" s="108"/>
+      <c r="K82" s="109"/>
+      <c r="L82" s="109"/>
+      <c r="M82" s="109"/>
+      <c r="N82" s="109"/>
+      <c r="O82" s="108"/>
+      <c r="P82" s="108"/>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B83" s="89"/>
+      <c r="C83" s="91" t="s">
         <v>297</v>
       </c>
-      <c r="D65" s="91"/>
-      <c r="E65" s="92">
+      <c r="D83" s="91"/>
+      <c r="E83" s="92">
         <v>0</v>
       </c>
-      <c r="F65" s="92">
+      <c r="F83" s="92">
         <v>0</v>
       </c>
-      <c r="G65" s="92">
+      <c r="G83" s="92">
         <v>0</v>
       </c>
-      <c r="H65" s="92">
+      <c r="H83" s="92">
         <v>0</v>
       </c>
-      <c r="I65" s="92">
+      <c r="I83" s="92">
         <v>0</v>
       </c>
-      <c r="J65" s="92">
+      <c r="J83" s="92">
         <v>36</v>
       </c>
-      <c r="K65" s="93"/>
-      <c r="L65" s="93"/>
-      <c r="M65" s="93"/>
-      <c r="N65" s="90"/>
-      <c r="O65" s="90"/>
-      <c r="P65" s="90"/>
-    </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B66" s="90"/>
-      <c r="C66" s="91"/>
-      <c r="D66" s="93"/>
-      <c r="E66" s="93"/>
-      <c r="F66" s="93"/>
-      <c r="G66" s="93"/>
-      <c r="H66" s="93"/>
-      <c r="I66" s="93"/>
-      <c r="J66" s="93"/>
-      <c r="K66" s="93"/>
-      <c r="L66" s="93"/>
-      <c r="M66" s="93"/>
-      <c r="N66" s="90"/>
-      <c r="O66" s="90"/>
-      <c r="P66" s="90"/>
-    </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B67" s="90"/>
-      <c r="C67" s="90"/>
-      <c r="D67" s="93"/>
-      <c r="E67" s="94"/>
-      <c r="F67" s="94"/>
-      <c r="G67" s="94"/>
-      <c r="H67" s="94"/>
-      <c r="I67" s="94"/>
-      <c r="J67" s="95" t="s">
+      <c r="K83" s="93"/>
+      <c r="L83" s="93"/>
+      <c r="M83" s="93"/>
+      <c r="N83" s="90"/>
+      <c r="O83" s="90"/>
+      <c r="P83" s="90"/>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B84" s="90"/>
+      <c r="C84" s="91"/>
+      <c r="D84" s="93"/>
+      <c r="E84" s="93"/>
+      <c r="F84" s="93"/>
+      <c r="G84" s="93"/>
+      <c r="H84" s="93"/>
+      <c r="I84" s="93"/>
+      <c r="J84" s="93"/>
+      <c r="K84" s="93"/>
+      <c r="L84" s="93"/>
+      <c r="M84" s="93"/>
+      <c r="N84" s="90"/>
+      <c r="O84" s="90"/>
+      <c r="P84" s="90"/>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B85" s="90"/>
+      <c r="C85" s="90"/>
+      <c r="D85" s="93"/>
+      <c r="E85" s="94"/>
+      <c r="F85" s="94"/>
+      <c r="G85" s="94"/>
+      <c r="H85" s="94"/>
+      <c r="I85" s="94"/>
+      <c r="J85" s="95" t="s">
         <v>299</v>
       </c>
-      <c r="K67" s="96">
+      <c r="K85" s="96">
         <v>36</v>
       </c>
-      <c r="L67" s="93"/>
-      <c r="M67" s="93"/>
-      <c r="N67" s="90"/>
-      <c r="O67" s="90"/>
-      <c r="P67" s="90"/>
+      <c r="L85" s="93"/>
+      <c r="M85" s="93"/>
+      <c r="N85" s="90"/>
+      <c r="O85" s="90"/>
+      <c r="P85" s="90"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -14220,6 +14841,33 @@
     <hyperlink ref="D34" r:id="rId30" location="'Metadatos V'!B33" xr:uid="{8FA923E8-C75C-4DAD-835A-7B7C5B507A30}"/>
     <hyperlink ref="D35" r:id="rId31" location="'Metadatos V'!B34" xr:uid="{B5999E1E-211B-4435-BB6C-42AFE3F80781}"/>
     <hyperlink ref="D36" r:id="rId32" location="'Metadatos V'!B35" xr:uid="{26BB993F-1B41-4033-BF0E-ED5CF3051DDC}"/>
+    <hyperlink ref="D37" r:id="rId33" location="'Metadatos V'!B36" xr:uid="{5DC6534B-D04D-4242-9646-F0FAA0291387}"/>
+    <hyperlink ref="D38" r:id="rId34" location="'Metadatos V'!B37" xr:uid="{B7E9ACDF-9AE5-430A-89B4-7F4FC6DAD00D}"/>
+    <hyperlink ref="D39" r:id="rId35" location="'Metadatos V'!B38" xr:uid="{F81FCAB0-12FE-4C77-8F6C-E71C9F83A220}"/>
+    <hyperlink ref="D40" r:id="rId36" location="'Metadatos V'!B39" xr:uid="{E8EF32C9-65F3-458A-BB02-2F5B85A0E865}"/>
+    <hyperlink ref="D41" r:id="rId37" location="'Metadatos V'!B40" xr:uid="{FE8F22C0-A4ED-4DC9-8FE4-F5193CB430A8}"/>
+    <hyperlink ref="D42" r:id="rId38" location="'Metadatos V'!B41" xr:uid="{611CCAD4-E3D3-48C6-AA4B-42B238D619DF}"/>
+    <hyperlink ref="D43" r:id="rId39" location="'Metadatos V'!B42" xr:uid="{4431A1B8-44C8-466A-AE56-0F168CB9B636}"/>
+    <hyperlink ref="D44" r:id="rId40" location="'Metadatos V'!B43" xr:uid="{EB1F7E80-0D83-4458-AE23-369FD416E4D8}"/>
+    <hyperlink ref="D45" r:id="rId41" location="'Metadatos V'!B44" xr:uid="{4EB72B41-4A3D-4D69-BD0F-5B675CC32D1A}"/>
+    <hyperlink ref="D46" r:id="rId42" location="'Metadatos V'!B45" xr:uid="{DFC2FAED-C44D-4B6E-9977-7627939B79FB}"/>
+    <hyperlink ref="D47" r:id="rId43" location="'Metadatos V'!B46" xr:uid="{758CD3FF-D014-479D-AA40-5B6F2D399B81}"/>
+    <hyperlink ref="D48" r:id="rId44" location="'Metadatos V'!B47" xr:uid="{C73B7DC1-C05D-4BBA-A740-F1E59C8CF20D}"/>
+    <hyperlink ref="D49" r:id="rId45" location="'Metadatos V'!B48" xr:uid="{8F709861-DF23-4922-82A3-5F98509FC099}"/>
+    <hyperlink ref="D50" r:id="rId46" location="'Metadatos V'!B49" xr:uid="{F3A3531F-67C1-4B8F-81C1-6AC88D0871E5}"/>
+    <hyperlink ref="D51" r:id="rId47" location="'Metadatos V'!B50" xr:uid="{EB39E6AD-04AC-4307-9F1C-70ABEBE2A1C7}"/>
+    <hyperlink ref="D52" r:id="rId48" location="'Metadatos V'!B51" xr:uid="{331F9CC0-B011-4423-9B7D-ADC49A168239}"/>
+    <hyperlink ref="D53" r:id="rId49" location="'Metadatos V'!B52" xr:uid="{0A40D78E-4DC0-4F2C-959B-3F41165C5074}"/>
+    <hyperlink ref="D54" r:id="rId50" location="'Metadatos V'!B53" xr:uid="{13D20A73-E747-4FA4-80E4-065483949905}"/>
+    <hyperlink ref="D55" r:id="rId51" location="'Metadatos V'!B54" xr:uid="{E039E482-93C8-4D11-837C-09A0D06B09FB}"/>
+    <hyperlink ref="D56" r:id="rId52" location="'Metadatos V'!B55" xr:uid="{869122C2-96B0-4932-AF49-CB7D5A8C4C10}"/>
+    <hyperlink ref="D57" r:id="rId53" location="'Metadatos V'!B56" xr:uid="{D9F5CA8F-4875-4DFE-A5AB-0C0F4678D467}"/>
+    <hyperlink ref="D58" r:id="rId54" location="'Metadatos V'!B57" xr:uid="{264FD871-64FA-4A24-B82D-3355988CBB39}"/>
+    <hyperlink ref="D59" r:id="rId55" location="'Metadatos V'!B58" xr:uid="{42574E0D-98E1-43C0-ACD1-72370EC18DA2}"/>
+    <hyperlink ref="D60" r:id="rId56" location="'Metadatos V'!B59" xr:uid="{41B6464B-6A96-44E4-BD36-A338F82E7021}"/>
+    <hyperlink ref="D61" r:id="rId57" location="'Metadatos V'!B60" xr:uid="{867385BA-5C99-4E73-8BEE-1E3EE123B5D4}"/>
+    <hyperlink ref="D62" r:id="rId58" location="'Metadatos V'!B61" xr:uid="{F68D4250-64DB-493A-820D-EE086A8A1CFC}"/>
+    <hyperlink ref="D63" r:id="rId59" location="'Metadatos V'!B62" xr:uid="{9998FF29-5F84-40EF-A583-87AB3A11616B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -14252,7 +14900,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>409</v>
@@ -14352,10 +15000,10 @@
         <v>285</v>
       </c>
       <c r="C5" s="110" t="s">
+        <v>477</v>
+      </c>
+      <c r="D5" s="129" t="s">
         <v>478</v>
-      </c>
-      <c r="D5" s="129" t="s">
-        <v>479</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
@@ -14373,18 +15021,18 @@
         <v>207</v>
       </c>
       <c r="N5" s="58" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O5" s="59"/>
       <c r="P5" s="56" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="134"/>
       <c r="C6" s="65"/>
       <c r="D6" s="130" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
@@ -14402,11 +15050,11 @@
         <v>207</v>
       </c>
       <c r="N6" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O6" s="65"/>
       <c r="P6" s="62" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -14414,10 +15062,10 @@
         <v>292</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D7" s="130" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E7" s="64"/>
       <c r="F7" s="64"/>
@@ -14435,11 +15083,11 @@
         <v>207</v>
       </c>
       <c r="N7" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O7" s="65"/>
       <c r="P7" s="62" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -14448,7 +15096,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="130" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="64"/>
@@ -14466,11 +15114,11 @@
       </c>
       <c r="M8" s="64"/>
       <c r="N8" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O8" s="65"/>
       <c r="P8" s="62" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14479,7 +15127,7 @@
         <v>420</v>
       </c>
       <c r="D9" s="130" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E9" s="64"/>
       <c r="F9" s="64"/>
@@ -14497,11 +15145,11 @@
       </c>
       <c r="M9" s="64"/>
       <c r="N9" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O9" s="65"/>
       <c r="P9" s="62" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14512,7 +15160,7 @@
         <v>420</v>
       </c>
       <c r="D10" s="130" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E10" s="64"/>
       <c r="F10" s="64"/>
@@ -14530,11 +15178,11 @@
       </c>
       <c r="M10" s="64"/>
       <c r="N10" s="64" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O10" s="65"/>
       <c r="P10" s="62" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14545,7 +15193,7 @@
         <v>420</v>
       </c>
       <c r="D11" s="130" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E11" s="64"/>
       <c r="F11" s="64"/>
@@ -14563,11 +15211,11 @@
       </c>
       <c r="M11" s="64"/>
       <c r="N11" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O11" s="65"/>
       <c r="P11" s="62" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14578,7 +15226,7 @@
         <v>420</v>
       </c>
       <c r="D12" s="130" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -14598,7 +15246,7 @@
       <c r="N12" s="64"/>
       <c r="O12" s="65"/>
       <c r="P12" s="62" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -14607,7 +15255,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="130" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E13" s="64" t="s">
         <v>200</v>
@@ -14625,13 +15273,13 @@
         <v>207</v>
       </c>
       <c r="N13" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O13" s="65" t="s">
+        <v>497</v>
+      </c>
+      <c r="P13" s="62" t="s">
         <v>498</v>
-      </c>
-      <c r="P13" s="62" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14642,7 +15290,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="130" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
@@ -14660,20 +15308,20 @@
       </c>
       <c r="M14" s="64"/>
       <c r="N14" s="64" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="O14" s="65"/>
       <c r="P14" s="62" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="134"/>
       <c r="C15" s="100" t="s">
+        <v>502</v>
+      </c>
+      <c r="D15" s="130" t="s">
         <v>503</v>
-      </c>
-      <c r="D15" s="130" t="s">
-        <v>504</v>
       </c>
       <c r="E15" s="64"/>
       <c r="F15" s="64"/>
@@ -14691,16 +15339,16 @@
       <c r="N15" s="64"/>
       <c r="O15" s="65"/>
       <c r="P15" s="62" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="134"/>
       <c r="C16" s="100" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D16" s="130" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E16" s="64"/>
       <c r="F16" s="64"/>
@@ -14718,7 +15366,7 @@
       <c r="N16" s="64"/>
       <c r="O16" s="65"/>
       <c r="P16" s="62" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14729,7 +15377,7 @@
         <v>420</v>
       </c>
       <c r="D17" s="130" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="64"/>
@@ -14747,11 +15395,11 @@
       </c>
       <c r="M17" s="64"/>
       <c r="N17" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O17" s="65"/>
       <c r="P17" s="62" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14762,7 +15410,7 @@
         <v>420</v>
       </c>
       <c r="D18" s="130" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
@@ -14780,11 +15428,11 @@
         <v>207</v>
       </c>
       <c r="N18" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O18" s="65"/>
       <c r="P18" s="62" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14793,7 +15441,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="130" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
@@ -14811,11 +15459,11 @@
         <v>207</v>
       </c>
       <c r="N19" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O19" s="65"/>
       <c r="P19" s="62" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14826,7 +15474,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="130" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E20" s="64"/>
       <c r="F20" s="64"/>
@@ -14844,22 +15492,22 @@
         <v>207</v>
       </c>
       <c r="N20" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O20" s="65"/>
       <c r="P20" s="62" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="127" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C21" s="100" t="s">
         <v>420</v>
       </c>
       <c r="D21" s="130" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E21" s="64"/>
       <c r="F21" s="64"/>
@@ -14877,22 +15525,22 @@
         <v>207</v>
       </c>
       <c r="N21" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O21" s="65"/>
       <c r="P21" s="62" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="127" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C22" s="100" t="s">
         <v>420</v>
       </c>
       <c r="D22" s="130" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="64"/>
@@ -14910,22 +15558,22 @@
         <v>207</v>
       </c>
       <c r="N22" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O22" s="65"/>
       <c r="P22" s="62" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="127" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C23" s="100">
         <v>2</v>
       </c>
       <c r="D23" s="130" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E23" s="64" t="s">
         <v>200</v>
@@ -14943,11 +15591,11 @@
         <v>207</v>
       </c>
       <c r="N23" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O23" s="65"/>
       <c r="P23" s="62" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14956,7 +15604,7 @@
         <v>420</v>
       </c>
       <c r="D24" s="130" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E24" s="64"/>
       <c r="F24" s="64"/>
@@ -14974,11 +15622,11 @@
         <v>207</v>
       </c>
       <c r="N24" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O24" s="65"/>
       <c r="P24" s="62" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14987,7 +15635,7 @@
         <v>420</v>
       </c>
       <c r="D25" s="130" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E25" s="64"/>
       <c r="F25" s="64"/>
@@ -15005,22 +15653,22 @@
         <v>207</v>
       </c>
       <c r="N25" s="64" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O25" s="65"/>
       <c r="P25" s="62" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="134" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C26" s="100">
         <v>1</v>
       </c>
       <c r="D26" s="130" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E26" s="64"/>
       <c r="F26" s="64"/>
@@ -15038,22 +15686,22 @@
         <v>207</v>
       </c>
       <c r="N26" s="64" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="O26" s="65"/>
       <c r="P26" s="62" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="134" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C27" s="100" t="s">
         <v>420</v>
       </c>
       <c r="D27" s="130" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E27" s="64"/>
       <c r="F27" s="64"/>
@@ -15073,16 +15721,16 @@
       <c r="N27" s="64"/>
       <c r="O27" s="65"/>
       <c r="P27" s="62" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="134" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C28" s="65"/>
       <c r="D28" s="130" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E28" s="64"/>
       <c r="F28" s="64"/>
@@ -15100,16 +15748,16 @@
       <c r="N28" s="64"/>
       <c r="O28" s="65"/>
       <c r="P28" s="62" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="134" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="130" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E29" s="64"/>
       <c r="F29" s="64"/>
@@ -15127,16 +15775,16 @@
       <c r="N29" s="64"/>
       <c r="O29" s="65"/>
       <c r="P29" s="62" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="134" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C30" s="65"/>
       <c r="D30" s="130" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E30" s="64" t="s">
         <v>200</v>
@@ -15154,16 +15802,16 @@
       <c r="N30" s="64"/>
       <c r="O30" s="65"/>
       <c r="P30" s="62" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="134" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="130" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E31" s="64" t="s">
         <v>200</v>
@@ -15180,19 +15828,19 @@
       <c r="M31" s="64"/>
       <c r="N31" s="64"/>
       <c r="O31" s="65" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P31" s="62" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="134" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="130" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E32" s="64" t="s">
         <v>200</v>
@@ -15209,19 +15857,19 @@
       <c r="M32" s="64"/>
       <c r="N32" s="64"/>
       <c r="O32" s="65" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P32" s="62" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="134" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C33" s="65"/>
       <c r="D33" s="130" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E33" s="64"/>
       <c r="F33" s="64"/>
@@ -15239,7 +15887,7 @@
       <c r="N33" s="64"/>
       <c r="O33" s="65"/>
       <c r="P33" s="62" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bruja voice added to Game/media/audio/voices. Chesheet and metadata table updated
</commit_message>
<xml_diff>
--- a/Docs/TDS/CueSheet.xlsx
+++ b/Docs/TDS/CueSheet.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="684">
   <si>
     <t>Cue-Sheets</t>
   </si>
@@ -1525,9 +1525,6 @@
     <t>3.1</t>
   </si>
   <si>
-    <t>Personaje 3</t>
-  </si>
-  <si>
     <t>3.2</t>
   </si>
   <si>
@@ -1825,60 +1822,6 @@
     <t>Musica de fondo del nivel 1</t>
   </si>
   <si>
-    <t>V-310 V-315</t>
-  </si>
-  <si>
-    <t>V-320 V-325</t>
-  </si>
-  <si>
-    <t>V-330 V-335</t>
-  </si>
-  <si>
-    <t>V-340 V-345</t>
-  </si>
-  <si>
-    <t>V-350 V-355</t>
-  </si>
-  <si>
-    <t>V-360 V-365</t>
-  </si>
-  <si>
-    <t>V-370 V-375</t>
-  </si>
-  <si>
-    <t>V-380 V-385</t>
-  </si>
-  <si>
-    <t>V-390 V-395</t>
-  </si>
-  <si>
-    <t>V-410 V-415</t>
-  </si>
-  <si>
-    <t>V-420 V-425</t>
-  </si>
-  <si>
-    <t>V-430 V-435</t>
-  </si>
-  <si>
-    <t>V-440 V-445</t>
-  </si>
-  <si>
-    <t>V-450 V-455</t>
-  </si>
-  <si>
-    <t>V-460 V-465</t>
-  </si>
-  <si>
-    <t>V-470 V-475</t>
-  </si>
-  <si>
-    <t>V-480 V-485</t>
-  </si>
-  <si>
-    <t>V-490 V-495</t>
-  </si>
-  <si>
     <t>Punk</t>
   </si>
   <si>
@@ -2144,6 +2087,123 @@
   </si>
   <si>
     <t>Victoria 1</t>
+  </si>
+  <si>
+    <t>V-310</t>
+  </si>
+  <si>
+    <t>V-315</t>
+  </si>
+  <si>
+    <t>V-320</t>
+  </si>
+  <si>
+    <t>V-321</t>
+  </si>
+  <si>
+    <t>V-325</t>
+  </si>
+  <si>
+    <t>V-326</t>
+  </si>
+  <si>
+    <t>V-330</t>
+  </si>
+  <si>
+    <t>V-335</t>
+  </si>
+  <si>
+    <t>V-340</t>
+  </si>
+  <si>
+    <t>V-341</t>
+  </si>
+  <si>
+    <t>V-342</t>
+  </si>
+  <si>
+    <t>V-345</t>
+  </si>
+  <si>
+    <t>V-346</t>
+  </si>
+  <si>
+    <t>V-350</t>
+  </si>
+  <si>
+    <t>V-351</t>
+  </si>
+  <si>
+    <t>V-352</t>
+  </si>
+  <si>
+    <t>V-355</t>
+  </si>
+  <si>
+    <t>V-356</t>
+  </si>
+  <si>
+    <t>V-357</t>
+  </si>
+  <si>
+    <t>V-360</t>
+  </si>
+  <si>
+    <t>V-361</t>
+  </si>
+  <si>
+    <t>V-365</t>
+  </si>
+  <si>
+    <t>V-366</t>
+  </si>
+  <si>
+    <t>V-370</t>
+  </si>
+  <si>
+    <t>V-375</t>
+  </si>
+  <si>
+    <t>V-380</t>
+  </si>
+  <si>
+    <t>V-381</t>
+  </si>
+  <si>
+    <t>V-385</t>
+  </si>
+  <si>
+    <t>V-390</t>
+  </si>
+  <si>
+    <t>V-391</t>
+  </si>
+  <si>
+    <t>V-392</t>
+  </si>
+  <si>
+    <t>V-395</t>
+  </si>
+  <si>
+    <t>V-396</t>
+  </si>
+  <si>
+    <t>V-397</t>
+  </si>
+  <si>
+    <t>Bruja</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 1.2</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 2.2</t>
+  </si>
+  <si>
+    <t>Voz de que algo ha salido mal 2.2 (INGLÉS)</t>
+  </si>
+  <si>
+    <t>Derrota 1</t>
   </si>
 </sst>
 </file>
@@ -2311,7 +2371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -2897,12 +2957,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3333,6 +3456,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -4240,27 +4378,27 @@
         <v>15</v>
       </c>
       <c r="C7" s="17">
-        <f>Personajes!E83</f>
+        <f>Personajes!E112</f>
         <v>0</v>
       </c>
       <c r="D7" s="17">
-        <f>Personajes!F83</f>
+        <f>Personajes!F112</f>
         <v>0</v>
       </c>
       <c r="E7" s="17">
-        <f>Personajes!G83</f>
+        <f>Personajes!G112</f>
         <v>0</v>
       </c>
       <c r="F7" s="17">
-        <f>Personajes!H83</f>
+        <f>Personajes!H112</f>
         <v>0</v>
       </c>
       <c r="G7" s="17">
-        <f>Personajes!I83</f>
+        <f>Personajes!I112</f>
         <v>0</v>
       </c>
       <c r="H7" s="17">
-        <f>Personajes!J83</f>
+        <f>Personajes!J112</f>
         <v>36</v>
       </c>
       <c r="I7" s="18">
@@ -4393,7 +4531,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>409</v>
@@ -4471,7 +4609,7 @@
     </row>
     <row r="4" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="49"/>
@@ -4496,7 +4634,7 @@
         <v>414</v>
       </c>
       <c r="D5" s="129" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>200</v>
@@ -4513,10 +4651,10 @@
       <c r="M5" s="57"/>
       <c r="N5" s="57"/>
       <c r="O5" s="56" t="s">
+        <v>554</v>
+      </c>
+      <c r="P5" s="56" t="s">
         <v>555</v>
-      </c>
-      <c r="P5" s="56" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -12142,10 +12280,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK85"/>
+  <dimension ref="A1:AMK114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S93" sqref="S93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -12268,7 +12406,7 @@
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="143" t="s">
-        <v>576</v>
+        <v>557</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
@@ -12282,7 +12420,7 @@
         <v>431</v>
       </c>
       <c r="L5" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M5" s="138" t="s">
         <v>432</v>
@@ -12299,7 +12437,7 @@
       <c r="B6" s="141"/>
       <c r="C6" s="142"/>
       <c r="D6" s="144" t="s">
-        <v>577</v>
+        <v>558</v>
       </c>
       <c r="E6" s="139"/>
       <c r="F6" s="139"/>
@@ -12313,7 +12451,7 @@
         <v>431</v>
       </c>
       <c r="L6" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M6" s="138" t="s">
         <v>432</v>
@@ -12323,7 +12461,7 @@
       </c>
       <c r="O6" s="142"/>
       <c r="P6" s="142" t="s">
-        <v>608</v>
+        <v>589</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12332,7 +12470,7 @@
       </c>
       <c r="C7" s="65"/>
       <c r="D7" s="135" t="s">
-        <v>578</v>
+        <v>559</v>
       </c>
       <c r="E7" s="64"/>
       <c r="F7" s="64"/>
@@ -12346,7 +12484,7 @@
         <v>431</v>
       </c>
       <c r="L7" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M7" s="138" t="s">
         <v>432</v>
@@ -12356,14 +12494,14 @@
       </c>
       <c r="O7" s="65"/>
       <c r="P7" s="65" t="s">
-        <v>609</v>
+        <v>590</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="133"/>
       <c r="C8" s="65"/>
       <c r="D8" s="135" t="s">
-        <v>579</v>
+        <v>560</v>
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="64"/>
@@ -12377,7 +12515,7 @@
         <v>431</v>
       </c>
       <c r="L8" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M8" s="138" t="s">
         <v>432</v>
@@ -12387,14 +12525,14 @@
       </c>
       <c r="O8" s="65"/>
       <c r="P8" s="65" t="s">
-        <v>612</v>
+        <v>593</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="133"/>
       <c r="C9" s="65"/>
       <c r="D9" s="135" t="s">
-        <v>580</v>
+        <v>561</v>
       </c>
       <c r="E9" s="64"/>
       <c r="F9" s="64"/>
@@ -12408,7 +12546,7 @@
         <v>431</v>
       </c>
       <c r="L9" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M9" s="138" t="s">
         <v>432</v>
@@ -12418,14 +12556,14 @@
       </c>
       <c r="O9" s="65"/>
       <c r="P9" s="65" t="s">
-        <v>613</v>
+        <v>594</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="133"/>
       <c r="C10" s="65"/>
       <c r="D10" s="135" t="s">
-        <v>581</v>
+        <v>562</v>
       </c>
       <c r="E10" s="64"/>
       <c r="F10" s="64"/>
@@ -12439,7 +12577,7 @@
         <v>431</v>
       </c>
       <c r="L10" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M10" s="138" t="s">
         <v>432</v>
@@ -12449,14 +12587,14 @@
       </c>
       <c r="O10" s="65"/>
       <c r="P10" s="65" t="s">
-        <v>617</v>
+        <v>598</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="133"/>
       <c r="C11" s="65"/>
       <c r="D11" s="135" t="s">
-        <v>582</v>
+        <v>563</v>
       </c>
       <c r="E11" s="64"/>
       <c r="F11" s="64"/>
@@ -12470,7 +12608,7 @@
         <v>431</v>
       </c>
       <c r="L11" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M11" s="138" t="s">
         <v>432</v>
@@ -12480,7 +12618,7 @@
       </c>
       <c r="O11" s="65"/>
       <c r="P11" s="65" t="s">
-        <v>618</v>
+        <v>599</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12489,7 +12627,7 @@
       </c>
       <c r="C12" s="65"/>
       <c r="D12" s="135" t="s">
-        <v>583</v>
+        <v>564</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -12503,7 +12641,7 @@
         <v>431</v>
       </c>
       <c r="L12" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M12" s="138" t="s">
         <v>432</v>
@@ -12520,7 +12658,7 @@
       <c r="B13" s="133"/>
       <c r="C13" s="65"/>
       <c r="D13" s="135" t="s">
-        <v>584</v>
+        <v>565</v>
       </c>
       <c r="E13" s="64"/>
       <c r="F13" s="64"/>
@@ -12534,7 +12672,7 @@
         <v>431</v>
       </c>
       <c r="L13" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M13" s="138" t="s">
         <v>432</v>
@@ -12544,14 +12682,14 @@
       </c>
       <c r="O13" s="65"/>
       <c r="P13" s="65" t="s">
-        <v>614</v>
+        <v>595</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="133"/>
       <c r="C14" s="65"/>
       <c r="D14" s="135" t="s">
-        <v>585</v>
+        <v>566</v>
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
@@ -12565,7 +12703,7 @@
         <v>431</v>
       </c>
       <c r="L14" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M14" s="138" t="s">
         <v>432</v>
@@ -12575,14 +12713,14 @@
       </c>
       <c r="O14" s="65"/>
       <c r="P14" s="65" t="s">
-        <v>610</v>
+        <v>591</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="133"/>
       <c r="C15" s="65"/>
       <c r="D15" s="135" t="s">
-        <v>586</v>
+        <v>567</v>
       </c>
       <c r="E15" s="64"/>
       <c r="F15" s="64"/>
@@ -12596,7 +12734,7 @@
         <v>431</v>
       </c>
       <c r="L15" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M15" s="138" t="s">
         <v>432</v>
@@ -12606,7 +12744,7 @@
       </c>
       <c r="O15" s="65"/>
       <c r="P15" s="65" t="s">
-        <v>615</v>
+        <v>596</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12615,7 +12753,7 @@
       </c>
       <c r="C16" s="65"/>
       <c r="D16" s="135" t="s">
-        <v>587</v>
+        <v>568</v>
       </c>
       <c r="E16" s="64"/>
       <c r="F16" s="64"/>
@@ -12629,7 +12767,7 @@
         <v>431</v>
       </c>
       <c r="L16" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M16" s="138" t="s">
         <v>432</v>
@@ -12639,14 +12777,14 @@
       </c>
       <c r="O16" s="65"/>
       <c r="P16" s="65" t="s">
-        <v>611</v>
+        <v>592</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="133"/>
       <c r="C17" s="65"/>
       <c r="D17" s="135" t="s">
-        <v>588</v>
+        <v>569</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="64"/>
@@ -12660,7 +12798,7 @@
         <v>431</v>
       </c>
       <c r="L17" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M17" s="138" t="s">
         <v>432</v>
@@ -12670,14 +12808,14 @@
       </c>
       <c r="O17" s="65"/>
       <c r="P17" s="65" t="s">
-        <v>616</v>
+        <v>597</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="133"/>
       <c r="C18" s="65"/>
       <c r="D18" s="135" t="s">
-        <v>589</v>
+        <v>570</v>
       </c>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
@@ -12691,7 +12829,7 @@
         <v>431</v>
       </c>
       <c r="L18" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M18" s="138" t="s">
         <v>432</v>
@@ -12701,14 +12839,14 @@
       </c>
       <c r="O18" s="65"/>
       <c r="P18" s="65" t="s">
-        <v>619</v>
+        <v>600</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="133"/>
       <c r="C19" s="65"/>
       <c r="D19" s="135" t="s">
-        <v>590</v>
+        <v>571</v>
       </c>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
@@ -12722,7 +12860,7 @@
         <v>431</v>
       </c>
       <c r="L19" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M19" s="138" t="s">
         <v>432</v>
@@ -12732,7 +12870,7 @@
       </c>
       <c r="O19" s="65"/>
       <c r="P19" s="65" t="s">
-        <v>620</v>
+        <v>601</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12741,7 +12879,7 @@
       </c>
       <c r="C20" s="65"/>
       <c r="D20" s="135" t="s">
-        <v>591</v>
+        <v>572</v>
       </c>
       <c r="E20" s="64"/>
       <c r="F20" s="64"/>
@@ -12755,7 +12893,7 @@
         <v>431</v>
       </c>
       <c r="L20" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M20" s="138" t="s">
         <v>432</v>
@@ -12772,7 +12910,7 @@
       <c r="B21" s="133"/>
       <c r="C21" s="65"/>
       <c r="D21" s="135" t="s">
-        <v>592</v>
+        <v>573</v>
       </c>
       <c r="E21" s="64"/>
       <c r="F21" s="64"/>
@@ -12786,7 +12924,7 @@
         <v>431</v>
       </c>
       <c r="L21" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M21" s="138" t="s">
         <v>432</v>
@@ -12796,14 +12934,14 @@
       </c>
       <c r="O21" s="65"/>
       <c r="P21" s="65" t="s">
-        <v>621</v>
+        <v>602</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="133"/>
       <c r="C22" s="65"/>
       <c r="D22" s="135" t="s">
-        <v>593</v>
+        <v>574</v>
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="64"/>
@@ -12817,7 +12955,7 @@
         <v>431</v>
       </c>
       <c r="L22" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M22" s="138" t="s">
         <v>432</v>
@@ -12827,14 +12965,14 @@
       </c>
       <c r="O22" s="65"/>
       <c r="P22" s="65" t="s">
-        <v>622</v>
+        <v>603</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="133"/>
       <c r="C23" s="65"/>
       <c r="D23" s="135" t="s">
-        <v>594</v>
+        <v>575</v>
       </c>
       <c r="E23" s="64"/>
       <c r="F23" s="64"/>
@@ -12848,7 +12986,7 @@
         <v>431</v>
       </c>
       <c r="L23" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M23" s="138" t="s">
         <v>432</v>
@@ -12858,7 +12996,7 @@
       </c>
       <c r="O23" s="65"/>
       <c r="P23" s="65" t="s">
-        <v>623</v>
+        <v>604</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12867,7 +13005,7 @@
       </c>
       <c r="C24" s="65"/>
       <c r="D24" s="135" t="s">
-        <v>595</v>
+        <v>576</v>
       </c>
       <c r="E24" s="64"/>
       <c r="F24" s="64"/>
@@ -12881,7 +13019,7 @@
         <v>431</v>
       </c>
       <c r="L24" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M24" s="138" t="s">
         <v>432</v>
@@ -12898,7 +13036,7 @@
       <c r="B25" s="133"/>
       <c r="C25" s="65"/>
       <c r="D25" s="135" t="s">
-        <v>596</v>
+        <v>577</v>
       </c>
       <c r="E25" s="64"/>
       <c r="F25" s="64"/>
@@ -12912,7 +13050,7 @@
         <v>431</v>
       </c>
       <c r="L25" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M25" s="138" t="s">
         <v>432</v>
@@ -12922,14 +13060,14 @@
       </c>
       <c r="O25" s="65"/>
       <c r="P25" s="65" t="s">
-        <v>624</v>
+        <v>605</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="133"/>
       <c r="C26" s="65"/>
       <c r="D26" s="135" t="s">
-        <v>597</v>
+        <v>578</v>
       </c>
       <c r="E26" s="64"/>
       <c r="F26" s="64"/>
@@ -12943,7 +13081,7 @@
         <v>431</v>
       </c>
       <c r="L26" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M26" s="138" t="s">
         <v>432</v>
@@ -12953,7 +13091,7 @@
       </c>
       <c r="O26" s="65"/>
       <c r="P26" s="65" t="s">
-        <v>625</v>
+        <v>606</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12962,7 +13100,7 @@
       </c>
       <c r="C27" s="65"/>
       <c r="D27" s="135" t="s">
-        <v>598</v>
+        <v>579</v>
       </c>
       <c r="E27" s="64"/>
       <c r="F27" s="64"/>
@@ -12976,7 +13114,7 @@
         <v>431</v>
       </c>
       <c r="L27" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M27" s="138" t="s">
         <v>432</v>
@@ -12993,7 +13131,7 @@
       <c r="B28" s="133"/>
       <c r="C28" s="65"/>
       <c r="D28" s="135" t="s">
-        <v>599</v>
+        <v>580</v>
       </c>
       <c r="E28" s="64"/>
       <c r="F28" s="64"/>
@@ -13007,7 +13145,7 @@
         <v>431</v>
       </c>
       <c r="L28" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M28" s="138" t="s">
         <v>432</v>
@@ -13017,7 +13155,7 @@
       </c>
       <c r="O28" s="65"/>
       <c r="P28" s="65" t="s">
-        <v>626</v>
+        <v>607</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13026,7 +13164,7 @@
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="135" t="s">
-        <v>600</v>
+        <v>581</v>
       </c>
       <c r="E29" s="64"/>
       <c r="F29" s="64"/>
@@ -13040,7 +13178,7 @@
         <v>431</v>
       </c>
       <c r="L29" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M29" s="138" t="s">
         <v>432</v>
@@ -13057,7 +13195,7 @@
       <c r="B30" s="133"/>
       <c r="C30" s="65"/>
       <c r="D30" s="135" t="s">
-        <v>601</v>
+        <v>582</v>
       </c>
       <c r="E30" s="64"/>
       <c r="F30" s="64"/>
@@ -13071,7 +13209,7 @@
         <v>431</v>
       </c>
       <c r="L30" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M30" s="138" t="s">
         <v>432</v>
@@ -13081,7 +13219,7 @@
       </c>
       <c r="O30" s="65"/>
       <c r="P30" s="65" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13090,7 +13228,7 @@
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="135" t="s">
-        <v>602</v>
+        <v>583</v>
       </c>
       <c r="E31" s="64"/>
       <c r="F31" s="64"/>
@@ -13104,7 +13242,7 @@
         <v>431</v>
       </c>
       <c r="L31" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M31" s="138" t="s">
         <v>432</v>
@@ -13121,7 +13259,7 @@
       <c r="B32" s="133"/>
       <c r="C32" s="65"/>
       <c r="D32" s="135" t="s">
-        <v>603</v>
+        <v>584</v>
       </c>
       <c r="E32" s="64"/>
       <c r="F32" s="64"/>
@@ -13135,7 +13273,7 @@
         <v>431</v>
       </c>
       <c r="L32" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M32" s="138" t="s">
         <v>432</v>
@@ -13145,14 +13283,14 @@
       </c>
       <c r="O32" s="65"/>
       <c r="P32" s="65" t="s">
-        <v>628</v>
+        <v>609</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="133"/>
       <c r="C33" s="65"/>
       <c r="D33" s="135" t="s">
-        <v>604</v>
+        <v>585</v>
       </c>
       <c r="E33" s="64"/>
       <c r="F33" s="64"/>
@@ -13166,7 +13304,7 @@
         <v>431</v>
       </c>
       <c r="L33" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M33" s="138" t="s">
         <v>432</v>
@@ -13176,14 +13314,14 @@
       </c>
       <c r="O33" s="65"/>
       <c r="P33" s="65" t="s">
-        <v>629</v>
+        <v>610</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="133"/>
       <c r="C34" s="65"/>
       <c r="D34" s="135" t="s">
-        <v>605</v>
+        <v>586</v>
       </c>
       <c r="E34" s="64"/>
       <c r="F34" s="64"/>
@@ -13197,7 +13335,7 @@
         <v>431</v>
       </c>
       <c r="L34" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M34" s="138" t="s">
         <v>432</v>
@@ -13207,14 +13345,14 @@
       </c>
       <c r="O34" s="65"/>
       <c r="P34" s="65" t="s">
-        <v>630</v>
+        <v>611</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="133"/>
       <c r="C35" s="65"/>
       <c r="D35" s="135" t="s">
-        <v>606</v>
+        <v>587</v>
       </c>
       <c r="E35" s="64"/>
       <c r="F35" s="64"/>
@@ -13228,7 +13366,7 @@
         <v>431</v>
       </c>
       <c r="L35" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M35" s="138" t="s">
         <v>432</v>
@@ -13238,14 +13376,14 @@
       </c>
       <c r="O35" s="65"/>
       <c r="P35" s="65" t="s">
-        <v>631</v>
+        <v>612</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="133"/>
       <c r="C36" s="65"/>
       <c r="D36" s="135" t="s">
-        <v>607</v>
+        <v>588</v>
       </c>
       <c r="E36" s="64"/>
       <c r="F36" s="64"/>
@@ -13259,7 +13397,7 @@
         <v>431</v>
       </c>
       <c r="L36" s="140" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="M36" s="138" t="s">
         <v>432</v>
@@ -13269,7 +13407,7 @@
       </c>
       <c r="O36" s="65"/>
       <c r="P36" s="65" t="s">
-        <v>632</v>
+        <v>613</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13278,7 +13416,7 @@
       </c>
       <c r="C37" s="65"/>
       <c r="D37" s="135" t="s">
-        <v>634</v>
+        <v>615</v>
       </c>
       <c r="E37" s="64"/>
       <c r="F37" s="64"/>
@@ -13292,7 +13430,7 @@
         <v>431</v>
       </c>
       <c r="L37" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M37" s="64" t="s">
         <v>432</v>
@@ -13309,7 +13447,7 @@
       <c r="B38" s="133"/>
       <c r="C38" s="65"/>
       <c r="D38" s="135" t="s">
-        <v>635</v>
+        <v>616</v>
       </c>
       <c r="E38" s="64"/>
       <c r="F38" s="64"/>
@@ -13323,7 +13461,7 @@
         <v>431</v>
       </c>
       <c r="L38" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M38" s="64" t="s">
         <v>432</v>
@@ -13333,14 +13471,14 @@
       </c>
       <c r="O38" s="65"/>
       <c r="P38" s="65" t="s">
-        <v>661</v>
+        <v>642</v>
       </c>
     </row>
     <row r="39" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="133"/>
       <c r="C39" s="65"/>
       <c r="D39" s="135" t="s">
-        <v>636</v>
+        <v>617</v>
       </c>
       <c r="E39" s="64"/>
       <c r="F39" s="64"/>
@@ -13354,7 +13492,7 @@
         <v>431</v>
       </c>
       <c r="L39" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M39" s="64" t="s">
         <v>432</v>
@@ -13364,7 +13502,7 @@
       </c>
       <c r="O39" s="65"/>
       <c r="P39" s="65" t="s">
-        <v>608</v>
+        <v>589</v>
       </c>
     </row>
     <row r="40" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13373,7 +13511,7 @@
       </c>
       <c r="C40" s="65"/>
       <c r="D40" s="135" t="s">
-        <v>637</v>
+        <v>618</v>
       </c>
       <c r="E40" s="64"/>
       <c r="F40" s="64"/>
@@ -13387,7 +13525,7 @@
         <v>431</v>
       </c>
       <c r="L40" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M40" s="64" t="s">
         <v>432</v>
@@ -13397,14 +13535,14 @@
       </c>
       <c r="O40" s="65"/>
       <c r="P40" s="65" t="s">
-        <v>609</v>
+        <v>590</v>
       </c>
     </row>
     <row r="41" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="133"/>
       <c r="C41" s="65"/>
       <c r="D41" s="135" t="s">
-        <v>638</v>
+        <v>619</v>
       </c>
       <c r="E41" s="64"/>
       <c r="F41" s="64"/>
@@ -13418,7 +13556,7 @@
         <v>431</v>
       </c>
       <c r="L41" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M41" s="64" t="s">
         <v>432</v>
@@ -13428,14 +13566,14 @@
       </c>
       <c r="O41" s="65"/>
       <c r="P41" s="65" t="s">
-        <v>612</v>
+        <v>593</v>
       </c>
     </row>
     <row r="42" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="133"/>
       <c r="C42" s="65"/>
       <c r="D42" s="135" t="s">
-        <v>639</v>
+        <v>620</v>
       </c>
       <c r="E42" s="64"/>
       <c r="F42" s="64"/>
@@ -13449,7 +13587,7 @@
         <v>431</v>
       </c>
       <c r="L42" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M42" s="64" t="s">
         <v>432</v>
@@ -13459,14 +13597,14 @@
       </c>
       <c r="O42" s="65"/>
       <c r="P42" s="65" t="s">
-        <v>617</v>
+        <v>598</v>
       </c>
     </row>
     <row r="43" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="133"/>
       <c r="C43" s="65"/>
       <c r="D43" s="135" t="s">
-        <v>640</v>
+        <v>621</v>
       </c>
       <c r="E43" s="64"/>
       <c r="F43" s="64"/>
@@ -13480,7 +13618,7 @@
         <v>431</v>
       </c>
       <c r="L43" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M43" s="64" t="s">
         <v>432</v>
@@ -13490,7 +13628,7 @@
       </c>
       <c r="O43" s="65"/>
       <c r="P43" s="65" t="s">
-        <v>618</v>
+        <v>599</v>
       </c>
     </row>
     <row r="44" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13499,7 +13637,7 @@
       </c>
       <c r="C44" s="65"/>
       <c r="D44" s="135" t="s">
-        <v>641</v>
+        <v>622</v>
       </c>
       <c r="E44" s="64"/>
       <c r="F44" s="64"/>
@@ -13513,7 +13651,7 @@
         <v>431</v>
       </c>
       <c r="L44" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M44" s="64" t="s">
         <v>432</v>
@@ -13530,7 +13668,7 @@
       <c r="B45" s="133"/>
       <c r="C45" s="65"/>
       <c r="D45" s="135" t="s">
-        <v>642</v>
+        <v>623</v>
       </c>
       <c r="E45" s="64"/>
       <c r="F45" s="64"/>
@@ -13544,7 +13682,7 @@
         <v>431</v>
       </c>
       <c r="L45" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M45" s="64" t="s">
         <v>432</v>
@@ -13554,14 +13692,14 @@
       </c>
       <c r="O45" s="65"/>
       <c r="P45" s="65" t="s">
-        <v>610</v>
+        <v>591</v>
       </c>
     </row>
     <row r="46" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="133"/>
       <c r="C46" s="65"/>
       <c r="D46" s="135" t="s">
-        <v>643</v>
+        <v>624</v>
       </c>
       <c r="E46" s="64"/>
       <c r="F46" s="64"/>
@@ -13575,7 +13713,7 @@
         <v>431</v>
       </c>
       <c r="L46" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M46" s="64" t="s">
         <v>432</v>
@@ -13585,7 +13723,7 @@
       </c>
       <c r="O46" s="65"/>
       <c r="P46" s="65" t="s">
-        <v>615</v>
+        <v>596</v>
       </c>
     </row>
     <row r="47" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13594,7 +13732,7 @@
       </c>
       <c r="C47" s="65"/>
       <c r="D47" s="135" t="s">
-        <v>644</v>
+        <v>625</v>
       </c>
       <c r="E47" s="64"/>
       <c r="F47" s="64"/>
@@ -13608,7 +13746,7 @@
         <v>431</v>
       </c>
       <c r="L47" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M47" s="64" t="s">
         <v>432</v>
@@ -13618,14 +13756,14 @@
       </c>
       <c r="O47" s="65"/>
       <c r="P47" s="65" t="s">
-        <v>611</v>
+        <v>592</v>
       </c>
     </row>
     <row r="48" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="133"/>
       <c r="C48" s="65"/>
       <c r="D48" s="135" t="s">
-        <v>645</v>
+        <v>626</v>
       </c>
       <c r="E48" s="64"/>
       <c r="F48" s="64"/>
@@ -13639,7 +13777,7 @@
         <v>431</v>
       </c>
       <c r="L48" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M48" s="64" t="s">
         <v>432</v>
@@ -13649,14 +13787,14 @@
       </c>
       <c r="O48" s="65"/>
       <c r="P48" s="65" t="s">
-        <v>616</v>
+        <v>597</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="133"/>
       <c r="C49" s="65"/>
       <c r="D49" s="135" t="s">
-        <v>646</v>
+        <v>627</v>
       </c>
       <c r="E49" s="64"/>
       <c r="F49" s="64"/>
@@ -13670,7 +13808,7 @@
         <v>431</v>
       </c>
       <c r="L49" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M49" s="64" t="s">
         <v>432</v>
@@ -13680,14 +13818,14 @@
       </c>
       <c r="O49" s="65"/>
       <c r="P49" s="65" t="s">
-        <v>619</v>
+        <v>600</v>
       </c>
     </row>
     <row r="50" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="133"/>
       <c r="C50" s="65"/>
       <c r="D50" s="135" t="s">
-        <v>647</v>
+        <v>628</v>
       </c>
       <c r="E50" s="64"/>
       <c r="F50" s="64"/>
@@ -13701,7 +13839,7 @@
         <v>431</v>
       </c>
       <c r="L50" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M50" s="64" t="s">
         <v>432</v>
@@ -13711,7 +13849,7 @@
       </c>
       <c r="O50" s="65"/>
       <c r="P50" s="65" t="s">
-        <v>620</v>
+        <v>601</v>
       </c>
     </row>
     <row r="51" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13720,7 +13858,7 @@
       </c>
       <c r="C51" s="65"/>
       <c r="D51" s="135" t="s">
-        <v>648</v>
+        <v>629</v>
       </c>
       <c r="E51" s="64"/>
       <c r="F51" s="64"/>
@@ -13734,7 +13872,7 @@
         <v>431</v>
       </c>
       <c r="L51" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M51" s="64" t="s">
         <v>432</v>
@@ -13751,7 +13889,7 @@
       <c r="B52" s="133"/>
       <c r="C52" s="65"/>
       <c r="D52" s="135" t="s">
-        <v>649</v>
+        <v>630</v>
       </c>
       <c r="E52" s="64"/>
       <c r="F52" s="64"/>
@@ -13765,7 +13903,7 @@
         <v>431</v>
       </c>
       <c r="L52" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M52" s="64" t="s">
         <v>432</v>
@@ -13775,7 +13913,7 @@
       </c>
       <c r="O52" s="65"/>
       <c r="P52" s="65" t="s">
-        <v>622</v>
+        <v>603</v>
       </c>
     </row>
     <row r="53" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13784,7 +13922,7 @@
       </c>
       <c r="C53" s="65"/>
       <c r="D53" s="135" t="s">
-        <v>650</v>
+        <v>631</v>
       </c>
       <c r="E53" s="64"/>
       <c r="F53" s="64"/>
@@ -13798,7 +13936,7 @@
         <v>431</v>
       </c>
       <c r="L53" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M53" s="64" t="s">
         <v>432</v>
@@ -13815,7 +13953,7 @@
       <c r="B54" s="133"/>
       <c r="C54" s="65"/>
       <c r="D54" s="135" t="s">
-        <v>651</v>
+        <v>632</v>
       </c>
       <c r="E54" s="64"/>
       <c r="F54" s="64"/>
@@ -13829,7 +13967,7 @@
         <v>431</v>
       </c>
       <c r="L54" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M54" s="64" t="s">
         <v>432</v>
@@ -13839,14 +13977,14 @@
       </c>
       <c r="O54" s="65"/>
       <c r="P54" s="65" t="s">
-        <v>624</v>
+        <v>605</v>
       </c>
     </row>
     <row r="55" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="133"/>
       <c r="C55" s="65"/>
       <c r="D55" s="135" t="s">
-        <v>652</v>
+        <v>633</v>
       </c>
       <c r="E55" s="64"/>
       <c r="F55" s="64"/>
@@ -13860,7 +13998,7 @@
         <v>431</v>
       </c>
       <c r="L55" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M55" s="64" t="s">
         <v>432</v>
@@ -13870,14 +14008,14 @@
       </c>
       <c r="O55" s="65"/>
       <c r="P55" s="65" t="s">
-        <v>625</v>
+        <v>606</v>
       </c>
     </row>
     <row r="56" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="133"/>
       <c r="C56" s="65"/>
       <c r="D56" s="135" t="s">
-        <v>653</v>
+        <v>634</v>
       </c>
       <c r="E56" s="64"/>
       <c r="F56" s="64"/>
@@ -13891,7 +14029,7 @@
         <v>431</v>
       </c>
       <c r="L56" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M56" s="64" t="s">
         <v>432</v>
@@ -13901,7 +14039,7 @@
       </c>
       <c r="O56" s="65"/>
       <c r="P56" s="65" t="s">
-        <v>662</v>
+        <v>643</v>
       </c>
     </row>
     <row r="57" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13910,7 +14048,7 @@
       </c>
       <c r="C57" s="65"/>
       <c r="D57" s="135" t="s">
-        <v>654</v>
+        <v>635</v>
       </c>
       <c r="E57" s="64"/>
       <c r="F57" s="64"/>
@@ -13924,7 +14062,7 @@
         <v>431</v>
       </c>
       <c r="L57" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M57" s="64" t="s">
         <v>432</v>
@@ -13941,7 +14079,7 @@
       <c r="B58" s="133"/>
       <c r="C58" s="65"/>
       <c r="D58" s="135" t="s">
-        <v>655</v>
+        <v>636</v>
       </c>
       <c r="E58" s="64"/>
       <c r="F58" s="64"/>
@@ -13955,7 +14093,7 @@
         <v>431</v>
       </c>
       <c r="L58" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M58" s="64" t="s">
         <v>432</v>
@@ -13965,14 +14103,14 @@
       </c>
       <c r="O58" s="65"/>
       <c r="P58" s="65" t="s">
-        <v>663</v>
+        <v>644</v>
       </c>
     </row>
     <row r="59" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="133"/>
       <c r="C59" s="65"/>
       <c r="D59" s="135" t="s">
-        <v>656</v>
+        <v>637</v>
       </c>
       <c r="E59" s="64"/>
       <c r="F59" s="64"/>
@@ -13986,7 +14124,7 @@
         <v>431</v>
       </c>
       <c r="L59" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M59" s="64" t="s">
         <v>432</v>
@@ -13996,7 +14134,7 @@
       </c>
       <c r="O59" s="65"/>
       <c r="P59" s="65" t="s">
-        <v>626</v>
+        <v>607</v>
       </c>
     </row>
     <row r="60" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -14005,7 +14143,7 @@
       </c>
       <c r="C60" s="65"/>
       <c r="D60" s="135" t="s">
-        <v>657</v>
+        <v>638</v>
       </c>
       <c r="E60" s="64"/>
       <c r="F60" s="64"/>
@@ -14019,7 +14157,7 @@
         <v>431</v>
       </c>
       <c r="L60" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M60" s="64" t="s">
         <v>432</v>
@@ -14036,7 +14174,7 @@
       <c r="B61" s="133"/>
       <c r="C61" s="65"/>
       <c r="D61" s="135" t="s">
-        <v>658</v>
+        <v>639</v>
       </c>
       <c r="E61" s="64"/>
       <c r="F61" s="64"/>
@@ -14050,7 +14188,7 @@
         <v>431</v>
       </c>
       <c r="L61" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M61" s="64" t="s">
         <v>432</v>
@@ -14060,7 +14198,7 @@
       </c>
       <c r="O61" s="65"/>
       <c r="P61" s="65" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
     </row>
     <row r="62" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -14069,7 +14207,7 @@
       </c>
       <c r="C62" s="65"/>
       <c r="D62" s="135" t="s">
-        <v>659</v>
+        <v>640</v>
       </c>
       <c r="E62" s="64"/>
       <c r="F62" s="64"/>
@@ -14083,7 +14221,7 @@
         <v>431</v>
       </c>
       <c r="L62" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M62" s="64" t="s">
         <v>432</v>
@@ -14100,7 +14238,7 @@
       <c r="B63" s="133"/>
       <c r="C63" s="65"/>
       <c r="D63" s="135" t="s">
-        <v>660</v>
+        <v>641</v>
       </c>
       <c r="E63" s="64"/>
       <c r="F63" s="64"/>
@@ -14114,7 +14252,7 @@
         <v>431</v>
       </c>
       <c r="L63" s="64" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="M63" s="64" t="s">
         <v>432</v>
@@ -14124,18 +14262,18 @@
       </c>
       <c r="O63" s="65"/>
       <c r="P63" s="65" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="64" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="133" t="s">
         <v>456</v>
       </c>
       <c r="C64" s="65"/>
-      <c r="D64" s="131" t="s">
-        <v>557</v>
-      </c>
-      <c r="E64" s="64"/>
+      <c r="D64" s="156" t="s">
+        <v>645</v>
+      </c>
+      <c r="E64" s="138"/>
       <c r="F64" s="64"/>
       <c r="G64" s="64"/>
       <c r="H64" s="64"/>
@@ -14147,7 +14285,7 @@
         <v>431</v>
       </c>
       <c r="L64" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M64" s="64" t="s">
         <v>432</v>
@@ -14160,15 +14298,13 @@
         <v>433</v>
       </c>
     </row>
-    <row r="65" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="133" t="s">
-        <v>458</v>
-      </c>
+    <row r="65" spans="2:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="133"/>
       <c r="C65" s="65"/>
-      <c r="D65" s="131" t="s">
-        <v>558</v>
-      </c>
-      <c r="E65" s="64"/>
+      <c r="D65" s="157" t="s">
+        <v>646</v>
+      </c>
+      <c r="E65" s="138"/>
       <c r="F65" s="64"/>
       <c r="G65" s="64"/>
       <c r="H65" s="64"/>
@@ -14180,7 +14316,7 @@
         <v>431</v>
       </c>
       <c r="L65" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M65" s="64" t="s">
         <v>432</v>
@@ -14190,18 +14326,18 @@
       </c>
       <c r="O65" s="65"/>
       <c r="P65" s="65" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="66" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="133" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C66" s="65"/>
-      <c r="D66" s="131" t="s">
-        <v>559</v>
-      </c>
-      <c r="E66" s="64"/>
+      <c r="D66" s="157" t="s">
+        <v>647</v>
+      </c>
+      <c r="E66" s="138"/>
       <c r="F66" s="64"/>
       <c r="G66" s="64"/>
       <c r="H66" s="64"/>
@@ -14213,7 +14349,7 @@
         <v>431</v>
       </c>
       <c r="L66" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M66" s="64" t="s">
         <v>432</v>
@@ -14223,18 +14359,16 @@
       </c>
       <c r="O66" s="65"/>
       <c r="P66" s="65" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="67" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="133" t="s">
-        <v>460</v>
-      </c>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="133"/>
       <c r="C67" s="65"/>
-      <c r="D67" s="131" t="s">
-        <v>560</v>
-      </c>
-      <c r="E67" s="64"/>
+      <c r="D67" s="157" t="s">
+        <v>648</v>
+      </c>
+      <c r="E67" s="138"/>
       <c r="F67" s="64"/>
       <c r="G67" s="64"/>
       <c r="H67" s="64"/>
@@ -14246,7 +14380,7 @@
         <v>431</v>
       </c>
       <c r="L67" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M67" s="64" t="s">
         <v>432</v>
@@ -14256,18 +14390,16 @@
       </c>
       <c r="O67" s="65"/>
       <c r="P67" s="65" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="68" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="133" t="s">
-        <v>461</v>
-      </c>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="133"/>
       <c r="C68" s="65"/>
-      <c r="D68" s="131" t="s">
-        <v>561</v>
-      </c>
-      <c r="E68" s="64"/>
+      <c r="D68" s="157" t="s">
+        <v>649</v>
+      </c>
+      <c r="E68" s="138"/>
       <c r="F68" s="64"/>
       <c r="G68" s="64"/>
       <c r="H68" s="64"/>
@@ -14279,7 +14411,7 @@
         <v>431</v>
       </c>
       <c r="L68" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M68" s="64" t="s">
         <v>432</v>
@@ -14289,18 +14421,16 @@
       </c>
       <c r="O68" s="65"/>
       <c r="P68" s="65" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="69" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="133" t="s">
-        <v>462</v>
-      </c>
+        <v>598</v>
+      </c>
+    </row>
+    <row r="69" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="133"/>
       <c r="C69" s="65"/>
-      <c r="D69" s="131" t="s">
-        <v>562</v>
-      </c>
-      <c r="E69" s="64"/>
+      <c r="D69" s="157" t="s">
+        <v>650</v>
+      </c>
+      <c r="E69" s="138"/>
       <c r="F69" s="64"/>
       <c r="G69" s="64"/>
       <c r="H69" s="64"/>
@@ -14312,7 +14442,7 @@
         <v>431</v>
       </c>
       <c r="L69" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M69" s="64" t="s">
         <v>432</v>
@@ -14322,18 +14452,18 @@
       </c>
       <c r="O69" s="65"/>
       <c r="P69" s="65" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="70" spans="2:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="133" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C70" s="65"/>
-      <c r="D70" s="131" t="s">
-        <v>563</v>
-      </c>
-      <c r="E70" s="64"/>
+      <c r="D70" s="157" t="s">
+        <v>651</v>
+      </c>
+      <c r="E70" s="138"/>
       <c r="F70" s="64"/>
       <c r="G70" s="64"/>
       <c r="H70" s="64"/>
@@ -14345,7 +14475,7 @@
         <v>431</v>
       </c>
       <c r="L70" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M70" s="64" t="s">
         <v>432</v>
@@ -14355,18 +14485,16 @@
       </c>
       <c r="O70" s="65"/>
       <c r="P70" s="65" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="71" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="133" t="s">
-        <v>464</v>
-      </c>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="71" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="133"/>
       <c r="C71" s="65"/>
-      <c r="D71" s="131" t="s">
-        <v>564</v>
-      </c>
-      <c r="E71" s="64"/>
+      <c r="D71" s="157" t="s">
+        <v>652</v>
+      </c>
+      <c r="E71" s="138"/>
       <c r="F71" s="64"/>
       <c r="G71" s="64"/>
       <c r="H71" s="64"/>
@@ -14378,7 +14506,7 @@
         <v>431</v>
       </c>
       <c r="L71" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M71" s="64" t="s">
         <v>432</v>
@@ -14388,18 +14516,18 @@
       </c>
       <c r="O71" s="65"/>
       <c r="P71" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="72" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="72" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="133" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="C72" s="65"/>
-      <c r="D72" s="131" t="s">
-        <v>565</v>
-      </c>
-      <c r="E72" s="64"/>
+      <c r="D72" s="157" t="s">
+        <v>653</v>
+      </c>
+      <c r="E72" s="138"/>
       <c r="F72" s="64"/>
       <c r="G72" s="64"/>
       <c r="H72" s="64"/>
@@ -14411,7 +14539,7 @@
         <v>431</v>
       </c>
       <c r="L72" s="64" t="s">
-        <v>457</v>
+        <v>679</v>
       </c>
       <c r="M72" s="64" t="s">
         <v>432</v>
@@ -14421,18 +14549,16 @@
       </c>
       <c r="O72" s="65"/>
       <c r="P72" s="65" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="73" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="133" t="s">
-        <v>466</v>
-      </c>
+        <v>592</v>
+      </c>
+    </row>
+    <row r="73" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="133"/>
       <c r="C73" s="65"/>
-      <c r="D73" s="131" t="s">
-        <v>566</v>
-      </c>
-      <c r="E73" s="64"/>
+      <c r="D73" s="157" t="s">
+        <v>654</v>
+      </c>
+      <c r="E73" s="138"/>
       <c r="F73" s="64"/>
       <c r="G73" s="64"/>
       <c r="H73" s="64"/>
@@ -14444,7 +14570,7 @@
         <v>431</v>
       </c>
       <c r="L73" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M73" s="64" t="s">
         <v>432</v>
@@ -14454,18 +14580,16 @@
       </c>
       <c r="O73" s="65"/>
       <c r="P73" s="65" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="74" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="133" t="s">
-        <v>468</v>
-      </c>
+        <v>597</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="133"/>
       <c r="C74" s="65"/>
-      <c r="D74" s="131" t="s">
-        <v>567</v>
-      </c>
-      <c r="E74" s="64"/>
+      <c r="D74" s="157" t="s">
+        <v>655</v>
+      </c>
+      <c r="E74" s="138"/>
       <c r="F74" s="64"/>
       <c r="G74" s="64"/>
       <c r="H74" s="64"/>
@@ -14477,7 +14601,7 @@
         <v>431</v>
       </c>
       <c r="L74" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M74" s="64" t="s">
         <v>432</v>
@@ -14487,18 +14611,16 @@
       </c>
       <c r="O74" s="65"/>
       <c r="P74" s="65" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="75" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="133" t="s">
-        <v>469</v>
-      </c>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="133"/>
       <c r="C75" s="65"/>
-      <c r="D75" s="131" t="s">
-        <v>568</v>
-      </c>
-      <c r="E75" s="64"/>
+      <c r="D75" s="157" t="s">
+        <v>656</v>
+      </c>
+      <c r="E75" s="138"/>
       <c r="F75" s="64"/>
       <c r="G75" s="64"/>
       <c r="H75" s="64"/>
@@ -14510,7 +14632,7 @@
         <v>431</v>
       </c>
       <c r="L75" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M75" s="64" t="s">
         <v>432</v>
@@ -14520,18 +14642,16 @@
       </c>
       <c r="O75" s="65"/>
       <c r="P75" s="65" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="76" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="133" t="s">
-        <v>470</v>
-      </c>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="133"/>
       <c r="C76" s="65"/>
-      <c r="D76" s="131" t="s">
-        <v>569</v>
-      </c>
-      <c r="E76" s="64"/>
+      <c r="D76" s="157" t="s">
+        <v>657</v>
+      </c>
+      <c r="E76" s="138"/>
       <c r="F76" s="64"/>
       <c r="G76" s="64"/>
       <c r="H76" s="64"/>
@@ -14543,7 +14663,7 @@
         <v>431</v>
       </c>
       <c r="L76" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M76" s="64" t="s">
         <v>432</v>
@@ -14553,18 +14673,18 @@
       </c>
       <c r="O76" s="65"/>
       <c r="P76" s="65" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="77" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="133" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="C77" s="65"/>
-      <c r="D77" s="131" t="s">
-        <v>570</v>
-      </c>
-      <c r="E77" s="64"/>
+      <c r="D77" s="157" t="s">
+        <v>658</v>
+      </c>
+      <c r="E77" s="138"/>
       <c r="F77" s="64"/>
       <c r="G77" s="64"/>
       <c r="H77" s="64"/>
@@ -14576,7 +14696,7 @@
         <v>431</v>
       </c>
       <c r="L77" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M77" s="64" t="s">
         <v>432</v>
@@ -14589,15 +14709,13 @@
         <v>438</v>
       </c>
     </row>
-    <row r="78" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="133" t="s">
-        <v>472</v>
-      </c>
+    <row r="78" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="133"/>
       <c r="C78" s="65"/>
-      <c r="D78" s="131" t="s">
-        <v>571</v>
-      </c>
-      <c r="E78" s="64"/>
+      <c r="D78" s="157" t="s">
+        <v>659</v>
+      </c>
+      <c r="E78" s="138"/>
       <c r="F78" s="64"/>
       <c r="G78" s="64"/>
       <c r="H78" s="64"/>
@@ -14609,7 +14727,7 @@
         <v>431</v>
       </c>
       <c r="L78" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M78" s="64" t="s">
         <v>432</v>
@@ -14619,18 +14737,16 @@
       </c>
       <c r="O78" s="65"/>
       <c r="P78" s="65" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="79" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="133" t="s">
-        <v>473</v>
-      </c>
+        <v>602</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="133"/>
       <c r="C79" s="65"/>
-      <c r="D79" s="131" t="s">
-        <v>572</v>
-      </c>
-      <c r="E79" s="64"/>
+      <c r="D79" s="157" t="s">
+        <v>660</v>
+      </c>
+      <c r="E79" s="138"/>
       <c r="F79" s="64"/>
       <c r="G79" s="64"/>
       <c r="H79" s="64"/>
@@ -14642,7 +14758,7 @@
         <v>431</v>
       </c>
       <c r="L79" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M79" s="64" t="s">
         <v>432</v>
@@ -14652,18 +14768,16 @@
       </c>
       <c r="O79" s="65"/>
       <c r="P79" s="65" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="80" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="133" t="s">
-        <v>474</v>
-      </c>
+        <v>681</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="133"/>
       <c r="C80" s="65"/>
-      <c r="D80" s="131" t="s">
-        <v>573</v>
-      </c>
-      <c r="E80" s="64"/>
+      <c r="D80" s="157" t="s">
+        <v>661</v>
+      </c>
+      <c r="E80" s="138"/>
       <c r="F80" s="64"/>
       <c r="G80" s="64"/>
       <c r="H80" s="64"/>
@@ -14675,7 +14789,7 @@
         <v>431</v>
       </c>
       <c r="L80" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M80" s="64" t="s">
         <v>432</v>
@@ -14685,18 +14799,16 @@
       </c>
       <c r="O80" s="65"/>
       <c r="P80" s="65" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="81" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="133" t="s">
-        <v>475</v>
-      </c>
+        <v>603</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="133"/>
       <c r="C81" s="65"/>
-      <c r="D81" s="131" t="s">
-        <v>574</v>
-      </c>
-      <c r="E81" s="64"/>
+      <c r="D81" s="157" t="s">
+        <v>662</v>
+      </c>
+      <c r="E81" s="138"/>
       <c r="F81" s="64"/>
       <c r="G81" s="64"/>
       <c r="H81" s="64"/>
@@ -14708,7 +14820,7 @@
         <v>431</v>
       </c>
       <c r="L81" s="64" t="s">
-        <v>467</v>
+        <v>679</v>
       </c>
       <c r="M81" s="64" t="s">
         <v>432</v>
@@ -14718,94 +14830,945 @@
       </c>
       <c r="O81" s="65"/>
       <c r="P81" s="65" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="82" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="133"/>
+      <c r="C82" s="65"/>
+      <c r="D82" s="157" t="s">
+        <v>663</v>
+      </c>
+      <c r="E82" s="138"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="64"/>
+      <c r="H82" s="64"/>
+      <c r="I82" s="64"/>
+      <c r="J82" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K82" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L82" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M82" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N82" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O82" s="65"/>
+      <c r="P82" s="65" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="83" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="133" t="s">
+        <v>461</v>
+      </c>
+      <c r="C83" s="65"/>
+      <c r="D83" s="157" t="s">
+        <v>664</v>
+      </c>
+      <c r="E83" s="138"/>
+      <c r="F83" s="64"/>
+      <c r="G83" s="64"/>
+      <c r="H83" s="64"/>
+      <c r="I83" s="64"/>
+      <c r="J83" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K83" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L83" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M83" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N83" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O83" s="65"/>
+      <c r="P83" s="65" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="84" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="133"/>
+      <c r="C84" s="65"/>
+      <c r="D84" s="157" t="s">
+        <v>665</v>
+      </c>
+      <c r="E84" s="138"/>
+      <c r="F84" s="64"/>
+      <c r="G84" s="64"/>
+      <c r="H84" s="64"/>
+      <c r="I84" s="64"/>
+      <c r="J84" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K84" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L84" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M84" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N84" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O84" s="65"/>
+      <c r="P84" s="65" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="85" spans="2:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="133"/>
+      <c r="C85" s="65"/>
+      <c r="D85" s="157" t="s">
+        <v>666</v>
+      </c>
+      <c r="E85" s="138"/>
+      <c r="F85" s="64"/>
+      <c r="G85" s="64"/>
+      <c r="H85" s="64"/>
+      <c r="I85" s="64"/>
+      <c r="J85" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K85" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L85" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M85" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N85" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O85" s="65"/>
+      <c r="P85" s="65" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="86" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="133"/>
+      <c r="C86" s="65"/>
+      <c r="D86" s="157" t="s">
+        <v>667</v>
+      </c>
+      <c r="E86" s="138"/>
+      <c r="F86" s="64"/>
+      <c r="G86" s="64"/>
+      <c r="H86" s="64"/>
+      <c r="I86" s="64"/>
+      <c r="J86" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K86" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L86" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M86" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N86" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O86" s="65"/>
+      <c r="P86" s="65" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="87" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="133" t="s">
+        <v>462</v>
+      </c>
+      <c r="C87" s="65"/>
+      <c r="D87" s="157" t="s">
+        <v>668</v>
+      </c>
+      <c r="E87" s="138"/>
+      <c r="F87" s="64"/>
+      <c r="G87" s="64"/>
+      <c r="H87" s="64"/>
+      <c r="I87" s="64"/>
+      <c r="J87" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K87" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L87" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M87" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N87" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O87" s="65"/>
+      <c r="P87" s="65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="88" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="133"/>
+      <c r="C88" s="65"/>
+      <c r="D88" s="157" t="s">
+        <v>669</v>
+      </c>
+      <c r="E88" s="138"/>
+      <c r="F88" s="64"/>
+      <c r="G88" s="64"/>
+      <c r="H88" s="64"/>
+      <c r="I88" s="64"/>
+      <c r="J88" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K88" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L88" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M88" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N88" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O88" s="65"/>
+      <c r="P88" s="65" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="89" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="133" t="s">
+        <v>463</v>
+      </c>
+      <c r="C89" s="65"/>
+      <c r="D89" s="157" t="s">
+        <v>670</v>
+      </c>
+      <c r="E89" s="138"/>
+      <c r="F89" s="64"/>
+      <c r="G89" s="64"/>
+      <c r="H89" s="64"/>
+      <c r="I89" s="64"/>
+      <c r="J89" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K89" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L89" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M89" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N89" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O89" s="65"/>
+      <c r="P89" s="65" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="90" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="133"/>
+      <c r="C90" s="65"/>
+      <c r="D90" s="157" t="s">
+        <v>671</v>
+      </c>
+      <c r="E90" s="138"/>
+      <c r="F90" s="64"/>
+      <c r="G90" s="64"/>
+      <c r="H90" s="64"/>
+      <c r="I90" s="64"/>
+      <c r="J90" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K90" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L90" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M90" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N90" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O90" s="65"/>
+      <c r="P90" s="65" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="133"/>
+      <c r="C91" s="65"/>
+      <c r="D91" s="157" t="s">
+        <v>672</v>
+      </c>
+      <c r="E91" s="138"/>
+      <c r="F91" s="64"/>
+      <c r="G91" s="64"/>
+      <c r="H91" s="64"/>
+      <c r="I91" s="64"/>
+      <c r="J91" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K91" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L91" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M91" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N91" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O91" s="65"/>
+      <c r="P91" s="65" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="92" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="133" t="s">
+        <v>464</v>
+      </c>
+      <c r="C92" s="65"/>
+      <c r="D92" s="157" t="s">
+        <v>673</v>
+      </c>
+      <c r="E92" s="138"/>
+      <c r="F92" s="64"/>
+      <c r="G92" s="64"/>
+      <c r="H92" s="64"/>
+      <c r="I92" s="64"/>
+      <c r="J92" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K92" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L92" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M92" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N92" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O92" s="65"/>
+      <c r="P92" s="65" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="82" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="107"/>
-      <c r="C82" s="108"/>
-      <c r="D82" s="108"/>
-      <c r="E82" s="109"/>
-      <c r="F82" s="109"/>
-      <c r="G82" s="109"/>
-      <c r="H82" s="109"/>
-      <c r="I82" s="109"/>
-      <c r="J82" s="108"/>
-      <c r="K82" s="109"/>
-      <c r="L82" s="109"/>
-      <c r="M82" s="109"/>
-      <c r="N82" s="109"/>
-      <c r="O82" s="108"/>
-      <c r="P82" s="108"/>
-    </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B83" s="89"/>
-      <c r="C83" s="91" t="s">
+    <row r="93" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="133"/>
+      <c r="C93" s="65"/>
+      <c r="D93" s="157" t="s">
+        <v>674</v>
+      </c>
+      <c r="E93" s="138"/>
+      <c r="F93" s="64"/>
+      <c r="G93" s="64"/>
+      <c r="H93" s="64"/>
+      <c r="I93" s="64"/>
+      <c r="J93" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K93" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L93" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M93" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N93" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O93" s="65"/>
+      <c r="P93" s="65" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="94" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="133"/>
+      <c r="C94" s="65"/>
+      <c r="D94" s="157" t="s">
+        <v>675</v>
+      </c>
+      <c r="E94" s="138"/>
+      <c r="F94" s="64"/>
+      <c r="G94" s="64"/>
+      <c r="H94" s="64"/>
+      <c r="I94" s="64"/>
+      <c r="J94" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K94" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L94" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M94" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N94" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O94" s="65"/>
+      <c r="P94" s="65" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="95" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="133"/>
+      <c r="C95" s="65"/>
+      <c r="D95" s="157" t="s">
+        <v>676</v>
+      </c>
+      <c r="E95" s="138"/>
+      <c r="F95" s="64"/>
+      <c r="G95" s="64"/>
+      <c r="H95" s="64"/>
+      <c r="I95" s="64"/>
+      <c r="J95" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K95" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L95" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M95" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N95" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O95" s="65"/>
+      <c r="P95" s="65" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="96" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="133"/>
+      <c r="C96" s="65"/>
+      <c r="D96" s="157" t="s">
+        <v>677</v>
+      </c>
+      <c r="E96" s="138"/>
+      <c r="F96" s="64"/>
+      <c r="G96" s="64"/>
+      <c r="H96" s="64"/>
+      <c r="I96" s="64"/>
+      <c r="J96" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K96" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L96" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M96" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N96" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O96" s="65"/>
+      <c r="P96" s="65" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="97" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="133"/>
+      <c r="C97" s="65"/>
+      <c r="D97" s="158" t="s">
+        <v>678</v>
+      </c>
+      <c r="E97" s="138"/>
+      <c r="F97" s="64"/>
+      <c r="G97" s="64"/>
+      <c r="H97" s="64"/>
+      <c r="I97" s="64"/>
+      <c r="J97" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K97" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L97" s="64" t="s">
+        <v>679</v>
+      </c>
+      <c r="M97" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N97" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O97" s="65"/>
+      <c r="P97" s="65" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="98" spans="2:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="133" t="s">
+        <v>465</v>
+      </c>
+      <c r="C98" s="65"/>
+      <c r="D98" s="131"/>
+      <c r="E98" s="64"/>
+      <c r="F98" s="64"/>
+      <c r="G98" s="64"/>
+      <c r="H98" s="64"/>
+      <c r="I98" s="64"/>
+      <c r="J98" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K98" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L98" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M98" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N98" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O98" s="65"/>
+      <c r="P98" s="65" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="99" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="133" t="s">
+        <v>467</v>
+      </c>
+      <c r="C99" s="65"/>
+      <c r="D99" s="131"/>
+      <c r="E99" s="64"/>
+      <c r="F99" s="64"/>
+      <c r="G99" s="64"/>
+      <c r="H99" s="64"/>
+      <c r="I99" s="64"/>
+      <c r="J99" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K99" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L99" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M99" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N99" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O99" s="65"/>
+      <c r="P99" s="65" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="100" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="133" t="s">
+        <v>468</v>
+      </c>
+      <c r="C100" s="65"/>
+      <c r="D100" s="131"/>
+      <c r="E100" s="64"/>
+      <c r="F100" s="64"/>
+      <c r="G100" s="64"/>
+      <c r="H100" s="64"/>
+      <c r="I100" s="64"/>
+      <c r="J100" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K100" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L100" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M100" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N100" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O100" s="65"/>
+      <c r="P100" s="65" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="101" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="133" t="s">
+        <v>469</v>
+      </c>
+      <c r="C101" s="65"/>
+      <c r="D101" s="131"/>
+      <c r="E101" s="64"/>
+      <c r="F101" s="64"/>
+      <c r="G101" s="64"/>
+      <c r="H101" s="64"/>
+      <c r="I101" s="64"/>
+      <c r="J101" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K101" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L101" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M101" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N101" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O101" s="65"/>
+      <c r="P101" s="65" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="102" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="133" t="s">
+        <v>470</v>
+      </c>
+      <c r="C102" s="65"/>
+      <c r="D102" s="131"/>
+      <c r="E102" s="64"/>
+      <c r="F102" s="64"/>
+      <c r="G102" s="64"/>
+      <c r="H102" s="64"/>
+      <c r="I102" s="64"/>
+      <c r="J102" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K102" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L102" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M102" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N102" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O102" s="65"/>
+      <c r="P102" s="65" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="103" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="133" t="s">
+        <v>471</v>
+      </c>
+      <c r="C103" s="65"/>
+      <c r="D103" s="131"/>
+      <c r="E103" s="64"/>
+      <c r="F103" s="64"/>
+      <c r="G103" s="64"/>
+      <c r="H103" s="64"/>
+      <c r="I103" s="64"/>
+      <c r="J103" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K103" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L103" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M103" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N103" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O103" s="65"/>
+      <c r="P103" s="65" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="104" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="133" t="s">
+        <v>472</v>
+      </c>
+      <c r="C104" s="65"/>
+      <c r="D104" s="131"/>
+      <c r="E104" s="64"/>
+      <c r="F104" s="64"/>
+      <c r="G104" s="64"/>
+      <c r="H104" s="64"/>
+      <c r="I104" s="64"/>
+      <c r="J104" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K104" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L104" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M104" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N104" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O104" s="65"/>
+      <c r="P104" s="65" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="105" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="133" t="s">
+        <v>473</v>
+      </c>
+      <c r="C105" s="65"/>
+      <c r="D105" s="131"/>
+      <c r="E105" s="64"/>
+      <c r="F105" s="64"/>
+      <c r="G105" s="64"/>
+      <c r="H105" s="64"/>
+      <c r="I105" s="64"/>
+      <c r="J105" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K105" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L105" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M105" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N105" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O105" s="65"/>
+      <c r="P105" s="65" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="106" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="133" t="s">
+        <v>474</v>
+      </c>
+      <c r="C106" s="65"/>
+      <c r="D106" s="131"/>
+      <c r="E106" s="64"/>
+      <c r="F106" s="64"/>
+      <c r="G106" s="64"/>
+      <c r="H106" s="64"/>
+      <c r="I106" s="64"/>
+      <c r="J106" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="K106" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="L106" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="M106" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="N106" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="O106" s="65"/>
+      <c r="P106" s="65" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="107" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="152"/>
+      <c r="C107" s="153"/>
+      <c r="D107" s="154"/>
+      <c r="E107" s="155"/>
+      <c r="F107" s="155"/>
+      <c r="G107" s="155"/>
+      <c r="H107" s="155"/>
+      <c r="I107" s="155"/>
+      <c r="J107" s="153"/>
+      <c r="K107" s="155"/>
+      <c r="L107" s="155"/>
+      <c r="M107" s="155"/>
+      <c r="N107" s="155"/>
+      <c r="O107" s="153"/>
+      <c r="P107" s="153"/>
+    </row>
+    <row r="108" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="152"/>
+      <c r="C108" s="153"/>
+      <c r="D108" s="154"/>
+      <c r="E108" s="155"/>
+      <c r="F108" s="155"/>
+      <c r="G108" s="155"/>
+      <c r="H108" s="155"/>
+      <c r="I108" s="155"/>
+      <c r="J108" s="153"/>
+      <c r="K108" s="155"/>
+      <c r="L108" s="155"/>
+      <c r="M108" s="155"/>
+      <c r="N108" s="155"/>
+      <c r="O108" s="153"/>
+      <c r="P108" s="153"/>
+    </row>
+    <row r="109" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="152"/>
+      <c r="C109" s="153"/>
+      <c r="D109" s="154"/>
+      <c r="E109" s="155"/>
+      <c r="F109" s="155"/>
+      <c r="G109" s="155"/>
+      <c r="H109" s="155"/>
+      <c r="I109" s="155"/>
+      <c r="J109" s="153"/>
+      <c r="K109" s="155"/>
+      <c r="L109" s="155"/>
+      <c r="M109" s="155"/>
+      <c r="N109" s="155"/>
+      <c r="O109" s="153"/>
+      <c r="P109" s="153"/>
+    </row>
+    <row r="110" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="152"/>
+      <c r="C110" s="153"/>
+      <c r="D110" s="154"/>
+      <c r="E110" s="155"/>
+      <c r="F110" s="155"/>
+      <c r="G110" s="155"/>
+      <c r="H110" s="155"/>
+      <c r="I110" s="155"/>
+      <c r="J110" s="153"/>
+      <c r="K110" s="155"/>
+      <c r="L110" s="155"/>
+      <c r="M110" s="155"/>
+      <c r="N110" s="155"/>
+      <c r="O110" s="153"/>
+      <c r="P110" s="153"/>
+    </row>
+    <row r="111" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="107"/>
+      <c r="C111" s="108"/>
+      <c r="D111" s="108"/>
+      <c r="E111" s="109"/>
+      <c r="F111" s="109"/>
+      <c r="G111" s="109"/>
+      <c r="H111" s="109"/>
+      <c r="I111" s="109"/>
+      <c r="J111" s="108"/>
+      <c r="K111" s="109"/>
+      <c r="L111" s="109"/>
+      <c r="M111" s="109"/>
+      <c r="N111" s="109"/>
+      <c r="O111" s="108"/>
+      <c r="P111" s="108"/>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B112" s="89"/>
+      <c r="C112" s="91" t="s">
         <v>297</v>
       </c>
-      <c r="D83" s="91"/>
-      <c r="E83" s="92">
+      <c r="D112" s="91"/>
+      <c r="E112" s="92">
         <v>0</v>
       </c>
-      <c r="F83" s="92">
+      <c r="F112" s="92">
         <v>0</v>
       </c>
-      <c r="G83" s="92">
+      <c r="G112" s="92">
         <v>0</v>
       </c>
-      <c r="H83" s="92">
+      <c r="H112" s="92">
         <v>0</v>
       </c>
-      <c r="I83" s="92">
+      <c r="I112" s="92">
         <v>0</v>
       </c>
-      <c r="J83" s="92">
+      <c r="J112" s="92">
         <v>36</v>
       </c>
-      <c r="K83" s="93"/>
-      <c r="L83" s="93"/>
-      <c r="M83" s="93"/>
-      <c r="N83" s="90"/>
-      <c r="O83" s="90"/>
-      <c r="P83" s="90"/>
-    </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B84" s="90"/>
-      <c r="C84" s="91"/>
-      <c r="D84" s="93"/>
-      <c r="E84" s="93"/>
-      <c r="F84" s="93"/>
-      <c r="G84" s="93"/>
-      <c r="H84" s="93"/>
-      <c r="I84" s="93"/>
-      <c r="J84" s="93"/>
-      <c r="K84" s="93"/>
-      <c r="L84" s="93"/>
-      <c r="M84" s="93"/>
-      <c r="N84" s="90"/>
-      <c r="O84" s="90"/>
-      <c r="P84" s="90"/>
-    </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B85" s="90"/>
-      <c r="C85" s="90"/>
-      <c r="D85" s="93"/>
-      <c r="E85" s="94"/>
-      <c r="F85" s="94"/>
-      <c r="G85" s="94"/>
-      <c r="H85" s="94"/>
-      <c r="I85" s="94"/>
-      <c r="J85" s="95" t="s">
+      <c r="K112" s="93"/>
+      <c r="L112" s="93"/>
+      <c r="M112" s="93"/>
+      <c r="N112" s="90"/>
+      <c r="O112" s="90"/>
+      <c r="P112" s="90"/>
+    </row>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B113" s="90"/>
+      <c r="C113" s="91"/>
+      <c r="D113" s="93"/>
+      <c r="E113" s="93"/>
+      <c r="F113" s="93"/>
+      <c r="G113" s="93"/>
+      <c r="H113" s="93"/>
+      <c r="I113" s="93"/>
+      <c r="J113" s="93"/>
+      <c r="K113" s="93"/>
+      <c r="L113" s="93"/>
+      <c r="M113" s="93"/>
+      <c r="N113" s="90"/>
+      <c r="O113" s="90"/>
+      <c r="P113" s="90"/>
+    </row>
+    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B114" s="90"/>
+      <c r="C114" s="90"/>
+      <c r="D114" s="93"/>
+      <c r="E114" s="94"/>
+      <c r="F114" s="94"/>
+      <c r="G114" s="94"/>
+      <c r="H114" s="94"/>
+      <c r="I114" s="94"/>
+      <c r="J114" s="95" t="s">
         <v>299</v>
       </c>
-      <c r="K85" s="96">
+      <c r="K114" s="96">
         <v>36</v>
       </c>
-      <c r="L85" s="93"/>
-      <c r="M85" s="93"/>
-      <c r="N85" s="90"/>
-      <c r="O85" s="90"/>
-      <c r="P85" s="90"/>
+      <c r="L114" s="93"/>
+      <c r="M114" s="93"/>
+      <c r="N114" s="90"/>
+      <c r="O114" s="90"/>
+      <c r="P114" s="90"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -14868,6 +15831,40 @@
     <hyperlink ref="D61" r:id="rId57" location="'Metadatos V'!B60" xr:uid="{867385BA-5C99-4E73-8BEE-1E3EE123B5D4}"/>
     <hyperlink ref="D62" r:id="rId58" location="'Metadatos V'!B61" xr:uid="{F68D4250-64DB-493A-820D-EE086A8A1CFC}"/>
     <hyperlink ref="D63" r:id="rId59" location="'Metadatos V'!B62" xr:uid="{9998FF29-5F84-40EF-A583-87AB3A11616B}"/>
+    <hyperlink ref="D64" r:id="rId60" location="'Metadatos V'!B63" xr:uid="{2D7BC5DC-DB25-4B12-BE19-C56B4010454C}"/>
+    <hyperlink ref="D65" r:id="rId61" location="'Metadatos V'!B64" xr:uid="{44577E2E-2F0A-49D9-877E-D9F61621996C}"/>
+    <hyperlink ref="D66" r:id="rId62" location="'Metadatos V'!B65" xr:uid="{44EEC8DB-D498-46B0-B19E-F1F566EDBE39}"/>
+    <hyperlink ref="D67" r:id="rId63" location="'Metadatos V'!B66" xr:uid="{8199C4ED-EFF6-4315-9CDE-92250128AED3}"/>
+    <hyperlink ref="D68" r:id="rId64" location="'Metadatos V'!B67" xr:uid="{18B79F5C-EA24-4AF2-9FAF-E484799F8BFE}"/>
+    <hyperlink ref="D69" r:id="rId65" location="'Metadatos V'!B68" xr:uid="{35DDE0E4-8B2C-4A23-8A15-7CF2E1521818}"/>
+    <hyperlink ref="D70" r:id="rId66" location="'Metadatos V'!B69" xr:uid="{26C5BF2C-FB01-47EF-9C31-6B17F46D90FF}"/>
+    <hyperlink ref="D71" r:id="rId67" location="'Metadatos V'!B70" xr:uid="{9EFBF60B-3B9D-45EE-B242-727E79055DED}"/>
+    <hyperlink ref="D72" r:id="rId68" location="'Metadatos V'!B71" xr:uid="{2F1A0FBF-9C77-4DA1-9C7C-98E10D9E5AFB}"/>
+    <hyperlink ref="D73" r:id="rId69" location="'Metadatos V'!B72" xr:uid="{C2E1E592-46AF-4C8A-A4B7-8FF88E4007B0}"/>
+    <hyperlink ref="D74" r:id="rId70" location="'Metadatos V'!B73" xr:uid="{785DE42C-B157-4AAF-BF87-D76866B21304}"/>
+    <hyperlink ref="D75" r:id="rId71" location="'Metadatos V'!B74" xr:uid="{C09A90FF-DADA-4A81-9FC5-8581EE1408A0}"/>
+    <hyperlink ref="D76" r:id="rId72" location="'Metadatos V'!B75" xr:uid="{2E4EE3F5-DFE9-4B74-88EF-B065F0819BCB}"/>
+    <hyperlink ref="D77" r:id="rId73" location="'Metadatos V'!B76" xr:uid="{8071A742-22DE-4022-8A1B-52445D0BAD00}"/>
+    <hyperlink ref="D78" r:id="rId74" location="'Metadatos V'!B77" xr:uid="{9E0953FC-5411-4582-80EF-99E3EB9BFB03}"/>
+    <hyperlink ref="D79" r:id="rId75" location="'Metadatos V'!B78" xr:uid="{957EA248-779F-411D-9C92-33F90FAC01ED}"/>
+    <hyperlink ref="D80" r:id="rId76" location="'Metadatos V'!B79" xr:uid="{F3D2E0A7-4E78-4942-8603-6AC081E091A8}"/>
+    <hyperlink ref="D81" r:id="rId77" location="'Metadatos V'!B80" xr:uid="{0EEC220E-32ED-4517-98FD-14B91A6988DD}"/>
+    <hyperlink ref="D82" r:id="rId78" location="'Metadatos V'!B81" xr:uid="{2C845BAC-08CE-4783-8DCD-31B0906A0B71}"/>
+    <hyperlink ref="D83" r:id="rId79" location="'Metadatos V'!B82" xr:uid="{83937E7B-E380-46FC-AE0A-6604D9E367E7}"/>
+    <hyperlink ref="D84" r:id="rId80" location="'Metadatos V'!B83" xr:uid="{8ACBC8AE-0120-43DC-B04D-B281EA18E998}"/>
+    <hyperlink ref="D85" r:id="rId81" location="'Metadatos V'!B84" xr:uid="{C38F7EB3-3A7A-40C6-B1FA-2EB58AF3A860}"/>
+    <hyperlink ref="D86" r:id="rId82" location="'Metadatos V'!B85" xr:uid="{AC369211-1ADF-4F29-8D79-6A5DF8A39E76}"/>
+    <hyperlink ref="D87" r:id="rId83" location="'Metadatos V'!B86" xr:uid="{658C8416-518C-44C5-93D6-C33AE2DEA507}"/>
+    <hyperlink ref="D88" r:id="rId84" location="'Metadatos V'!B87" xr:uid="{07D08CD0-A4E2-4BF0-AEEE-0BDA4C0ED9C2}"/>
+    <hyperlink ref="D89" r:id="rId85" location="'Metadatos V'!B88" xr:uid="{8ED3EED8-8124-4AE9-893A-6789CA7BA82B}"/>
+    <hyperlink ref="D90" r:id="rId86" location="'Metadatos V'!B89" xr:uid="{5D9DDE3F-C4CE-4306-850B-28A6F2933129}"/>
+    <hyperlink ref="D91" r:id="rId87" location="'Metadatos V'!B90" xr:uid="{6DCF71A9-ACB2-40E1-8C16-B38C3ADDFBF3}"/>
+    <hyperlink ref="D92" r:id="rId88" location="'Metadatos V'!B91" xr:uid="{AAEE01E7-70F7-44BE-89AB-1103E0EED55F}"/>
+    <hyperlink ref="D93" r:id="rId89" location="'Metadatos V'!B92" xr:uid="{D3BC58EF-0F32-4625-900A-22DC20676723}"/>
+    <hyperlink ref="D94" r:id="rId90" location="'Metadatos V'!B93" xr:uid="{5F6FC726-F8A8-4339-804D-7A9044E1D5B0}"/>
+    <hyperlink ref="D95" r:id="rId91" location="'Metadatos V'!B94" xr:uid="{C6838503-3A6A-4FE0-B3E6-B970FD3F9AB4}"/>
+    <hyperlink ref="D96" r:id="rId92" location="'Metadatos V'!B95" xr:uid="{EBE3EA12-B8C7-4B06-8E77-2413C24BBEEF}"/>
+    <hyperlink ref="D97" r:id="rId93" location="'Metadatos V'!B96" xr:uid="{58806871-1A47-4734-8C4F-F8703FF8C055}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -14900,7 +15897,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>409</v>
@@ -15000,10 +15997,10 @@
         <v>285</v>
       </c>
       <c r="C5" s="110" t="s">
+        <v>476</v>
+      </c>
+      <c r="D5" s="129" t="s">
         <v>477</v>
-      </c>
-      <c r="D5" s="129" t="s">
-        <v>478</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
@@ -15021,18 +16018,18 @@
         <v>207</v>
       </c>
       <c r="N5" s="58" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O5" s="59"/>
       <c r="P5" s="56" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="134"/>
       <c r="C6" s="65"/>
       <c r="D6" s="130" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E6" s="64"/>
       <c r="F6" s="64"/>
@@ -15050,11 +16047,11 @@
         <v>207</v>
       </c>
       <c r="N6" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O6" s="65"/>
       <c r="P6" s="62" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -15062,10 +16059,10 @@
         <v>292</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D7" s="130" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E7" s="64"/>
       <c r="F7" s="64"/>
@@ -15083,11 +16080,11 @@
         <v>207</v>
       </c>
       <c r="N7" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O7" s="65"/>
       <c r="P7" s="62" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -15096,7 +16093,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="130" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="64"/>
@@ -15114,11 +16111,11 @@
       </c>
       <c r="M8" s="64"/>
       <c r="N8" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O8" s="65"/>
       <c r="P8" s="62" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15127,7 +16124,7 @@
         <v>420</v>
       </c>
       <c r="D9" s="130" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E9" s="64"/>
       <c r="F9" s="64"/>
@@ -15145,11 +16142,11 @@
       </c>
       <c r="M9" s="64"/>
       <c r="N9" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O9" s="65"/>
       <c r="P9" s="62" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15160,7 +16157,7 @@
         <v>420</v>
       </c>
       <c r="D10" s="130" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E10" s="64"/>
       <c r="F10" s="64"/>
@@ -15178,11 +16175,11 @@
       </c>
       <c r="M10" s="64"/>
       <c r="N10" s="64" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="O10" s="65"/>
       <c r="P10" s="62" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15193,7 +16190,7 @@
         <v>420</v>
       </c>
       <c r="D11" s="130" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E11" s="64"/>
       <c r="F11" s="64"/>
@@ -15211,11 +16208,11 @@
       </c>
       <c r="M11" s="64"/>
       <c r="N11" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O11" s="65"/>
       <c r="P11" s="62" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15226,7 +16223,7 @@
         <v>420</v>
       </c>
       <c r="D12" s="130" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -15246,7 +16243,7 @@
       <c r="N12" s="64"/>
       <c r="O12" s="65"/>
       <c r="P12" s="62" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -15255,7 +16252,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="130" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E13" s="64" t="s">
         <v>200</v>
@@ -15273,13 +16270,13 @@
         <v>207</v>
       </c>
       <c r="N13" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O13" s="65" t="s">
+        <v>496</v>
+      </c>
+      <c r="P13" s="62" t="s">
         <v>497</v>
-      </c>
-      <c r="P13" s="62" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15290,7 +16287,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="130" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
@@ -15308,20 +16305,20 @@
       </c>
       <c r="M14" s="64"/>
       <c r="N14" s="64" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="O14" s="65"/>
       <c r="P14" s="62" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="134"/>
       <c r="C15" s="100" t="s">
+        <v>501</v>
+      </c>
+      <c r="D15" s="130" t="s">
         <v>502</v>
-      </c>
-      <c r="D15" s="130" t="s">
-        <v>503</v>
       </c>
       <c r="E15" s="64"/>
       <c r="F15" s="64"/>
@@ -15339,16 +16336,16 @@
       <c r="N15" s="64"/>
       <c r="O15" s="65"/>
       <c r="P15" s="62" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="134"/>
       <c r="C16" s="100" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D16" s="130" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E16" s="64"/>
       <c r="F16" s="64"/>
@@ -15366,7 +16363,7 @@
       <c r="N16" s="64"/>
       <c r="O16" s="65"/>
       <c r="P16" s="62" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15377,7 +16374,7 @@
         <v>420</v>
       </c>
       <c r="D17" s="130" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="64"/>
@@ -15395,11 +16392,11 @@
       </c>
       <c r="M17" s="64"/>
       <c r="N17" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O17" s="65"/>
       <c r="P17" s="62" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15410,7 +16407,7 @@
         <v>420</v>
       </c>
       <c r="D18" s="130" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E18" s="64"/>
       <c r="F18" s="64"/>
@@ -15428,11 +16425,11 @@
         <v>207</v>
       </c>
       <c r="N18" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O18" s="65"/>
       <c r="P18" s="62" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15441,7 +16438,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="130" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E19" s="64"/>
       <c r="F19" s="64"/>
@@ -15459,11 +16456,11 @@
         <v>207</v>
       </c>
       <c r="N19" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O19" s="65"/>
       <c r="P19" s="62" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15474,7 +16471,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="130" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E20" s="64"/>
       <c r="F20" s="64"/>
@@ -15492,22 +16489,22 @@
         <v>207</v>
       </c>
       <c r="N20" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O20" s="65"/>
       <c r="P20" s="62" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="127" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C21" s="100" t="s">
         <v>420</v>
       </c>
       <c r="D21" s="130" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E21" s="64"/>
       <c r="F21" s="64"/>
@@ -15525,22 +16522,22 @@
         <v>207</v>
       </c>
       <c r="N21" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O21" s="65"/>
       <c r="P21" s="62" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="127" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C22" s="100" t="s">
         <v>420</v>
       </c>
       <c r="D22" s="130" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="64"/>
@@ -15558,22 +16555,22 @@
         <v>207</v>
       </c>
       <c r="N22" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O22" s="65"/>
       <c r="P22" s="62" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="127" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C23" s="100">
         <v>2</v>
       </c>
       <c r="D23" s="130" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E23" s="64" t="s">
         <v>200</v>
@@ -15591,11 +16588,11 @@
         <v>207</v>
       </c>
       <c r="N23" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O23" s="65"/>
       <c r="P23" s="62" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15604,7 +16601,7 @@
         <v>420</v>
       </c>
       <c r="D24" s="130" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E24" s="64"/>
       <c r="F24" s="64"/>
@@ -15622,11 +16619,11 @@
         <v>207</v>
       </c>
       <c r="N24" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O24" s="65"/>
       <c r="P24" s="62" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15635,7 +16632,7 @@
         <v>420</v>
       </c>
       <c r="D25" s="130" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E25" s="64"/>
       <c r="F25" s="64"/>
@@ -15653,22 +16650,22 @@
         <v>207</v>
       </c>
       <c r="N25" s="64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O25" s="65"/>
       <c r="P25" s="62" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="134" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C26" s="100">
         <v>1</v>
       </c>
       <c r="D26" s="130" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E26" s="64"/>
       <c r="F26" s="64"/>
@@ -15686,22 +16683,22 @@
         <v>207</v>
       </c>
       <c r="N26" s="64" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="O26" s="65"/>
       <c r="P26" s="62" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="134" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C27" s="100" t="s">
         <v>420</v>
       </c>
       <c r="D27" s="130" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E27" s="64"/>
       <c r="F27" s="64"/>
@@ -15721,16 +16718,16 @@
       <c r="N27" s="64"/>
       <c r="O27" s="65"/>
       <c r="P27" s="62" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="134" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C28" s="65"/>
       <c r="D28" s="130" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E28" s="64"/>
       <c r="F28" s="64"/>
@@ -15748,16 +16745,16 @@
       <c r="N28" s="64"/>
       <c r="O28" s="65"/>
       <c r="P28" s="62" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="134" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="130" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E29" s="64"/>
       <c r="F29" s="64"/>
@@ -15775,16 +16772,16 @@
       <c r="N29" s="64"/>
       <c r="O29" s="65"/>
       <c r="P29" s="62" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="134" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C30" s="65"/>
       <c r="D30" s="130" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E30" s="64" t="s">
         <v>200</v>
@@ -15802,16 +16799,16 @@
       <c r="N30" s="64"/>
       <c r="O30" s="65"/>
       <c r="P30" s="62" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="134" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C31" s="65"/>
       <c r="D31" s="130" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E31" s="64" t="s">
         <v>200</v>
@@ -15828,19 +16825,19 @@
       <c r="M31" s="64"/>
       <c r="N31" s="64"/>
       <c r="O31" s="65" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="P31" s="62" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="134" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="130" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E32" s="64" t="s">
         <v>200</v>
@@ -15857,19 +16854,19 @@
       <c r="M32" s="64"/>
       <c r="N32" s="64"/>
       <c r="O32" s="65" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="P32" s="62" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="134" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C33" s="65"/>
       <c r="D33" s="130" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E33" s="64"/>
       <c r="F33" s="64"/>
@@ -15887,7 +16884,7 @@
       <c r="N33" s="64"/>
       <c r="O33" s="65"/>
       <c r="P33" s="62" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hoja de metadatos actualizada al completo
</commit_message>
<xml_diff>
--- a/Docs/TDS/CueSheet.xlsx
+++ b/Docs/TDS/CueSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\Wasted-Racing-master\Wasted-Racing-master\Docs\TDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo-PT\Desktop\Wasted-Racing-master\Wasted-Racing-master\Docs\TDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="617" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="617"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -3634,6 +3634,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3868,6 +3869,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3916,7 +3918,7 @@
         <xdr:cNvPr id="2" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4236,7 +4238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -12325,7 +12327,7 @@
   <dimension ref="A1:AMK128"/>
   <sheetViews>
     <sheetView topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M127" sqref="M127"/>
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -16175,7 +16177,7 @@
         <v>469</v>
       </c>
       <c r="C123" s="65"/>
-      <c r="D123" s="147" t="s">
+      <c r="D123" s="8" t="s">
         <v>703</v>
       </c>
       <c r="E123" s="64"/>
@@ -16206,7 +16208,7 @@
     <row r="124" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B124" s="132"/>
       <c r="C124" s="65"/>
-      <c r="D124" s="147" t="s">
+      <c r="D124" s="8" t="s">
         <v>704</v>
       </c>
       <c r="E124" s="64"/>
@@ -16440,11 +16442,9 @@
     <hyperlink ref="D120" r:id="rId116" location="'Metadatos V'!B119"/>
     <hyperlink ref="D121" r:id="rId117" location="'Metadatos V'!B120"/>
     <hyperlink ref="D122" r:id="rId118" location="'Metadatos V'!B121"/>
-    <hyperlink ref="D123" r:id="rId119" location="'Metadatos V'!B122"/>
-    <hyperlink ref="D124" r:id="rId120" location="'Metadatos V'!B123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId121"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId119"/>
 </worksheet>
 </file>
 
@@ -16452,7 +16452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualizacion! Hoja de metadatos y cuesheet
</commit_message>
<xml_diff>
--- a/Docs/TDS/CueSheet.xlsx
+++ b/Docs/TDS/CueSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -2206,9 +2206,6 @@
     <t>Fade in, Fade out</t>
   </si>
   <si>
-    <t>Indica el periodo act()ivo de la invulnerabilidad</t>
-  </si>
-  <si>
     <t>F-004</t>
   </si>
   <si>
@@ -2738,6 +2735,9 @@
   </si>
   <si>
     <t>Derrota (INGLÉS) / "Gameee Oveer"</t>
+  </si>
+  <si>
+    <t>Indica el periodo activo de la invulnerabilidad</t>
   </si>
 </sst>
 </file>
@@ -5264,7 +5264,7 @@
   <dimension ref="A1:AMK22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -5285,7 +5285,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>472</v>
@@ -5363,7 +5363,7 @@
     </row>
     <row r="4" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="49"/>
@@ -5388,7 +5388,7 @@
         <v>477</v>
       </c>
       <c r="D5" s="177" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>200</v>
@@ -5405,10 +5405,10 @@
       <c r="M5" s="58"/>
       <c r="N5" s="58"/>
       <c r="O5" s="58" t="s">
+        <v>744</v>
+      </c>
+      <c r="P5" s="60" t="s">
         <v>745</v>
-      </c>
-      <c r="P5" s="60" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5419,7 +5419,7 @@
         <v>477</v>
       </c>
       <c r="D6" s="175" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E6" s="141" t="s">
         <v>200</v>
@@ -5436,10 +5436,10 @@
       <c r="M6" s="141"/>
       <c r="N6" s="141"/>
       <c r="O6" s="141" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="P6" s="179" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5450,7 +5450,7 @@
         <v>477</v>
       </c>
       <c r="D7" s="176" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E7" s="141" t="s">
         <v>200</v>
@@ -5467,10 +5467,10 @@
       <c r="M7" s="141"/>
       <c r="N7" s="141"/>
       <c r="O7" s="141" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="P7" s="179" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -13516,7 +13516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P122" sqref="P122"/>
     </sheetView>
   </sheetViews>
@@ -13664,7 +13664,7 @@
       </c>
       <c r="O5" s="95"/>
       <c r="P5" s="129" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13695,7 +13695,7 @@
       </c>
       <c r="O6" s="126"/>
       <c r="P6" s="126" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13728,7 +13728,7 @@
       </c>
       <c r="O7" s="97"/>
       <c r="P7" s="97" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13759,7 +13759,7 @@
       </c>
       <c r="O8" s="97"/>
       <c r="P8" s="97" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13790,7 +13790,7 @@
       </c>
       <c r="O9" s="97"/>
       <c r="P9" s="97" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13821,7 +13821,7 @@
       </c>
       <c r="O10" s="97"/>
       <c r="P10" s="97" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13852,7 +13852,7 @@
       </c>
       <c r="O11" s="97"/>
       <c r="P11" s="97" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13885,7 +13885,7 @@
       </c>
       <c r="O12" s="97"/>
       <c r="P12" s="97" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13916,7 +13916,7 @@
       </c>
       <c r="O13" s="97"/>
       <c r="P13" s="97" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13947,7 +13947,7 @@
       </c>
       <c r="O14" s="97"/>
       <c r="P14" s="97" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13978,7 +13978,7 @@
       </c>
       <c r="O15" s="97"/>
       <c r="P15" s="97" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14011,7 +14011,7 @@
       </c>
       <c r="O16" s="97"/>
       <c r="P16" s="97" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14042,7 +14042,7 @@
       </c>
       <c r="O17" s="97"/>
       <c r="P17" s="97" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14073,7 +14073,7 @@
       </c>
       <c r="O18" s="97"/>
       <c r="P18" s="97" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14104,7 +14104,7 @@
       </c>
       <c r="O19" s="97"/>
       <c r="P19" s="97" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14137,7 +14137,7 @@
       </c>
       <c r="O20" s="97"/>
       <c r="P20" s="97" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14168,7 +14168,7 @@
       </c>
       <c r="O21" s="97"/>
       <c r="P21" s="97" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14199,7 +14199,7 @@
       </c>
       <c r="O22" s="97"/>
       <c r="P22" s="97" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14230,7 +14230,7 @@
       </c>
       <c r="O23" s="97"/>
       <c r="P23" s="97" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14263,7 +14263,7 @@
       </c>
       <c r="O24" s="97"/>
       <c r="P24" s="97" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14294,7 +14294,7 @@
       </c>
       <c r="O25" s="97"/>
       <c r="P25" s="97" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14325,7 +14325,7 @@
       </c>
       <c r="O26" s="97"/>
       <c r="P26" s="97" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14358,7 +14358,7 @@
       </c>
       <c r="O27" s="97"/>
       <c r="P27" s="97" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14389,7 +14389,7 @@
       </c>
       <c r="O28" s="97"/>
       <c r="P28" s="97" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14422,7 +14422,7 @@
       </c>
       <c r="O29" s="97"/>
       <c r="P29" s="97" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14453,7 +14453,7 @@
       </c>
       <c r="O30" s="97"/>
       <c r="P30" s="97" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14486,7 +14486,7 @@
       </c>
       <c r="O31" s="97"/>
       <c r="P31" s="97" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14517,7 +14517,7 @@
       </c>
       <c r="O32" s="97"/>
       <c r="P32" s="97" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14548,7 +14548,7 @@
       </c>
       <c r="O33" s="97"/>
       <c r="P33" s="97" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14579,7 +14579,7 @@
       </c>
       <c r="O34" s="97"/>
       <c r="P34" s="97" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14610,7 +14610,7 @@
       </c>
       <c r="O35" s="97"/>
       <c r="P35" s="97" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14641,7 +14641,7 @@
       </c>
       <c r="O36" s="97"/>
       <c r="P36" s="97" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14674,7 +14674,7 @@
       </c>
       <c r="O37" s="97"/>
       <c r="P37" s="97" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="38" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14705,7 +14705,7 @@
       </c>
       <c r="O38" s="97"/>
       <c r="P38" s="97" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="39" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14736,7 +14736,7 @@
       </c>
       <c r="O39" s="97"/>
       <c r="P39" s="97" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="40" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14769,7 +14769,7 @@
       </c>
       <c r="O40" s="97"/>
       <c r="P40" s="97" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="41" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14800,7 +14800,7 @@
       </c>
       <c r="O41" s="97"/>
       <c r="P41" s="97" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="42" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14831,7 +14831,7 @@
       </c>
       <c r="O42" s="97"/>
       <c r="P42" s="97" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="43" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14862,7 +14862,7 @@
       </c>
       <c r="O43" s="97"/>
       <c r="P43" s="97" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="44" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14895,7 +14895,7 @@
       </c>
       <c r="O44" s="97"/>
       <c r="P44" s="97" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="45" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14926,7 +14926,7 @@
       </c>
       <c r="O45" s="97"/>
       <c r="P45" s="97" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="46" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14957,7 +14957,7 @@
       </c>
       <c r="O46" s="97"/>
       <c r="P46" s="97" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="47" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14990,7 +14990,7 @@
       </c>
       <c r="O47" s="97"/>
       <c r="P47" s="97" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="48" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15021,7 +15021,7 @@
       </c>
       <c r="O48" s="97"/>
       <c r="P48" s="97" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15052,7 +15052,7 @@
       </c>
       <c r="O49" s="97"/>
       <c r="P49" s="97" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="50" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15083,7 +15083,7 @@
       </c>
       <c r="O50" s="97"/>
       <c r="P50" s="97" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="51" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15116,7 +15116,7 @@
       </c>
       <c r="O51" s="97"/>
       <c r="P51" s="97" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="52" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15147,7 +15147,7 @@
       </c>
       <c r="O52" s="97"/>
       <c r="P52" s="97" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="53" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15180,7 +15180,7 @@
       </c>
       <c r="O53" s="97"/>
       <c r="P53" s="97" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="54" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15211,7 +15211,7 @@
       </c>
       <c r="O54" s="97"/>
       <c r="P54" s="97" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="55" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15242,7 +15242,7 @@
       </c>
       <c r="O55" s="97"/>
       <c r="P55" s="97" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="56" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15273,7 +15273,7 @@
       </c>
       <c r="O56" s="97"/>
       <c r="P56" s="97" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="57" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15306,7 +15306,7 @@
       </c>
       <c r="O57" s="97"/>
       <c r="P57" s="97" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="58" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15337,7 +15337,7 @@
       </c>
       <c r="O58" s="97"/>
       <c r="P58" s="97" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="59" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15368,7 +15368,7 @@
       </c>
       <c r="O59" s="97"/>
       <c r="P59" s="97" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="60" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15401,7 +15401,7 @@
       </c>
       <c r="O60" s="97"/>
       <c r="P60" s="97" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="61" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15432,7 +15432,7 @@
       </c>
       <c r="O61" s="97"/>
       <c r="P61" s="97" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="62" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15465,7 +15465,7 @@
       </c>
       <c r="O62" s="97"/>
       <c r="P62" s="97" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="63" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15496,7 +15496,7 @@
       </c>
       <c r="O63" s="97"/>
       <c r="P63" s="97" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="64" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15529,7 +15529,7 @@
       </c>
       <c r="O64" s="97"/>
       <c r="P64" s="97" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="65" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15560,7 +15560,7 @@
       </c>
       <c r="O65" s="97"/>
       <c r="P65" s="97" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="66" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15593,7 +15593,7 @@
       </c>
       <c r="O66" s="97"/>
       <c r="P66" s="97" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="67" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15624,7 +15624,7 @@
       </c>
       <c r="O67" s="97"/>
       <c r="P67" s="97" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="68" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15655,7 +15655,7 @@
       </c>
       <c r="O68" s="97"/>
       <c r="P68" s="97" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="69" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15686,7 +15686,7 @@
       </c>
       <c r="O69" s="97"/>
       <c r="P69" s="97" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="70" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15719,7 +15719,7 @@
       </c>
       <c r="O70" s="97"/>
       <c r="P70" s="97" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="71" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15750,7 +15750,7 @@
       </c>
       <c r="O71" s="97"/>
       <c r="P71" s="97" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="72" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15783,7 +15783,7 @@
       </c>
       <c r="O72" s="97"/>
       <c r="P72" s="97" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="73" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15814,7 +15814,7 @@
       </c>
       <c r="O73" s="97"/>
       <c r="P73" s="97" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="74" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15845,7 +15845,7 @@
       </c>
       <c r="O74" s="97"/>
       <c r="P74" s="97" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="75" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15876,7 +15876,7 @@
       </c>
       <c r="O75" s="97"/>
       <c r="P75" s="97" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="76" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15907,7 +15907,7 @@
       </c>
       <c r="O76" s="97"/>
       <c r="P76" s="97" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="77" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15940,7 +15940,7 @@
       </c>
       <c r="O77" s="97"/>
       <c r="P77" s="97" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="78" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15971,7 +15971,7 @@
       </c>
       <c r="O78" s="97"/>
       <c r="P78" s="97" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="79" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16002,7 +16002,7 @@
       </c>
       <c r="O79" s="97"/>
       <c r="P79" s="97" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="80" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16033,7 +16033,7 @@
       </c>
       <c r="O80" s="97"/>
       <c r="P80" s="97" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="81" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16064,7 +16064,7 @@
       </c>
       <c r="O81" s="97"/>
       <c r="P81" s="97" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="82" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16095,7 +16095,7 @@
       </c>
       <c r="O82" s="97"/>
       <c r="P82" s="97" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="83" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16128,7 +16128,7 @@
       </c>
       <c r="O83" s="97"/>
       <c r="P83" s="97" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="84" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16159,7 +16159,7 @@
       </c>
       <c r="O84" s="97"/>
       <c r="P84" s="97" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="85" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16190,7 +16190,7 @@
       </c>
       <c r="O85" s="97"/>
       <c r="P85" s="97" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="86" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16221,7 +16221,7 @@
       </c>
       <c r="O86" s="97"/>
       <c r="P86" s="97" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="87" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16254,7 +16254,7 @@
       </c>
       <c r="O87" s="97"/>
       <c r="P87" s="97" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="88" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16285,7 +16285,7 @@
       </c>
       <c r="O88" s="97"/>
       <c r="P88" s="97" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="89" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16318,7 +16318,7 @@
       </c>
       <c r="O89" s="97"/>
       <c r="P89" s="97" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="90" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16349,7 +16349,7 @@
       </c>
       <c r="O90" s="97"/>
       <c r="P90" s="97" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="91" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16380,7 +16380,7 @@
       </c>
       <c r="O91" s="97"/>
       <c r="P91" s="97" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="92" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16413,7 +16413,7 @@
       </c>
       <c r="O92" s="97"/>
       <c r="P92" s="97" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="93" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16444,7 +16444,7 @@
       </c>
       <c r="O93" s="97"/>
       <c r="P93" s="97" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="94" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16475,7 +16475,7 @@
       </c>
       <c r="O94" s="97"/>
       <c r="P94" s="97" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="95" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16506,7 +16506,7 @@
       </c>
       <c r="O95" s="97"/>
       <c r="P95" s="97" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="96" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16537,7 +16537,7 @@
       </c>
       <c r="O96" s="97"/>
       <c r="P96" s="97" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="97" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16568,7 +16568,7 @@
       </c>
       <c r="O97" s="97"/>
       <c r="P97" s="97" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="98" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16601,7 +16601,7 @@
       </c>
       <c r="O98" s="97"/>
       <c r="P98" s="97" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="99" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16632,7 +16632,7 @@
       </c>
       <c r="O99" s="97"/>
       <c r="P99" s="97" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="100" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16663,7 +16663,7 @@
       </c>
       <c r="O100" s="97"/>
       <c r="P100" s="97" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="101" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16696,7 +16696,7 @@
       </c>
       <c r="O101" s="97"/>
       <c r="P101" s="97" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="102" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16727,7 +16727,7 @@
       </c>
       <c r="O102" s="97"/>
       <c r="P102" s="97" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="103" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16758,7 +16758,7 @@
       </c>
       <c r="O103" s="97"/>
       <c r="P103" s="97" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="104" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16791,7 +16791,7 @@
       </c>
       <c r="O104" s="97"/>
       <c r="P104" s="97" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="105" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16822,7 +16822,7 @@
       </c>
       <c r="O105" s="97"/>
       <c r="P105" s="97" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="106" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16853,7 +16853,7 @@
       </c>
       <c r="O106" s="97"/>
       <c r="P106" s="97" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="107" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16884,7 +16884,7 @@
       </c>
       <c r="O107" s="97"/>
       <c r="P107" s="97" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="108" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16917,7 +16917,7 @@
       </c>
       <c r="O108" s="97"/>
       <c r="P108" s="97" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="109" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16948,7 +16948,7 @@
       </c>
       <c r="O109" s="97"/>
       <c r="P109" s="97" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="110" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16979,7 +16979,7 @@
       </c>
       <c r="O110" s="97"/>
       <c r="P110" s="97" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="111" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17012,7 +17012,7 @@
       </c>
       <c r="O111" s="97"/>
       <c r="P111" s="97" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="112" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17043,7 +17043,7 @@
       </c>
       <c r="O112" s="97"/>
       <c r="P112" s="97" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="113" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17074,7 +17074,7 @@
       </c>
       <c r="O113" s="97"/>
       <c r="P113" s="97" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="114" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17105,7 +17105,7 @@
       </c>
       <c r="O114" s="97"/>
       <c r="P114" s="97" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="115" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17138,7 +17138,7 @@
       </c>
       <c r="O115" s="97"/>
       <c r="P115" s="97" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="116" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17169,7 +17169,7 @@
       </c>
       <c r="O116" s="97"/>
       <c r="P116" s="97" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="117" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17200,7 +17200,7 @@
       </c>
       <c r="O117" s="97"/>
       <c r="P117" s="97" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="118" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17231,7 +17231,7 @@
       </c>
       <c r="O118" s="97"/>
       <c r="P118" s="97" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="119" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17264,7 +17264,7 @@
       </c>
       <c r="O119" s="97"/>
       <c r="P119" s="97" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="120" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17295,7 +17295,7 @@
       </c>
       <c r="O120" s="97"/>
       <c r="P120" s="97" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="121" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17328,7 +17328,7 @@
       </c>
       <c r="O121" s="97"/>
       <c r="P121" s="97" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="122" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17359,7 +17359,7 @@
       </c>
       <c r="O122" s="97"/>
       <c r="P122" s="97" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="123" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17645,8 +17645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -18020,9 +18020,9 @@
     <row r="13" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="157"/>
       <c r="C13" s="165">
-        <v>8</v>
-      </c>
-      <c r="D13" s="161" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="162" t="s">
         <v>682</v>
       </c>
       <c r="E13" s="128" t="s">
@@ -18047,7 +18047,7 @@
         <v>683</v>
       </c>
       <c r="P13" s="67" t="s">
-        <v>684</v>
+        <v>861</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18058,7 +18058,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="161" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E14" s="128"/>
       <c r="F14" s="96"/>
@@ -18076,20 +18076,20 @@
       </c>
       <c r="M14" s="96"/>
       <c r="N14" s="96" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="O14" s="127"/>
       <c r="P14" s="67" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="157"/>
       <c r="C15" s="165" t="s">
+        <v>687</v>
+      </c>
+      <c r="D15" s="162" t="s">
         <v>688</v>
-      </c>
-      <c r="D15" s="162" t="s">
-        <v>689</v>
       </c>
       <c r="E15" s="128"/>
       <c r="F15" s="96"/>
@@ -18107,16 +18107,16 @@
       <c r="N15" s="96"/>
       <c r="O15" s="127"/>
       <c r="P15" s="67" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="157"/>
       <c r="C16" s="165" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D16" s="162" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E16" s="128"/>
       <c r="F16" s="96"/>
@@ -18136,7 +18136,7 @@
       <c r="N16" s="96"/>
       <c r="O16" s="127"/>
       <c r="P16" s="67" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18147,7 +18147,7 @@
         <v>672</v>
       </c>
       <c r="D17" s="162" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E17" s="128"/>
       <c r="F17" s="96"/>
@@ -18169,7 +18169,7 @@
       </c>
       <c r="O17" s="127"/>
       <c r="P17" s="67" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -18178,7 +18178,7 @@
       </c>
       <c r="C18" s="165"/>
       <c r="D18" s="155" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E18" s="128"/>
       <c r="F18" s="96"/>
@@ -18200,14 +18200,14 @@
       </c>
       <c r="O18" s="127"/>
       <c r="P18" s="67" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="158"/>
       <c r="C19" s="165"/>
       <c r="D19" s="155" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E19" s="128"/>
       <c r="F19" s="96"/>
@@ -18229,7 +18229,7 @@
       </c>
       <c r="O19" s="127"/>
       <c r="P19" s="67" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18240,7 +18240,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="161" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E20" s="128"/>
       <c r="F20" s="96"/>
@@ -18262,18 +18262,18 @@
       </c>
       <c r="O20" s="127"/>
       <c r="P20" s="67" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="158" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C21" s="165" t="s">
         <v>672</v>
       </c>
       <c r="D21" s="161" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E21" s="128"/>
       <c r="F21" s="96"/>
@@ -18295,18 +18295,18 @@
       </c>
       <c r="O21" s="127"/>
       <c r="P21" s="67" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="158" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C22" s="165" t="s">
         <v>672</v>
       </c>
       <c r="D22" s="161" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E22" s="128"/>
       <c r="F22" s="96"/>
@@ -18328,18 +18328,18 @@
       </c>
       <c r="O22" s="127"/>
       <c r="P22" s="67" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="158" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C23" s="165">
         <v>2</v>
       </c>
       <c r="D23" s="162" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E23" s="128" t="s">
         <v>200</v>
@@ -18361,7 +18361,7 @@
       </c>
       <c r="O23" s="127"/>
       <c r="P23" s="67" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18370,7 +18370,7 @@
         <v>672</v>
       </c>
       <c r="D24" s="162" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E24" s="128"/>
       <c r="F24" s="96"/>
@@ -18392,7 +18392,7 @@
       </c>
       <c r="O24" s="127"/>
       <c r="P24" s="67" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18401,7 +18401,7 @@
         <v>672</v>
       </c>
       <c r="D25" s="161" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E25" s="128"/>
       <c r="F25" s="96"/>
@@ -18423,18 +18423,18 @@
       </c>
       <c r="O25" s="127"/>
       <c r="P25" s="67" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="157" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C26" s="165">
         <v>1</v>
       </c>
       <c r="D26" s="161" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E26" s="128"/>
       <c r="F26" s="96"/>
@@ -18452,22 +18452,22 @@
         <v>207</v>
       </c>
       <c r="N26" s="96" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="O26" s="127"/>
       <c r="P26" s="67" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="157" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C27" s="165" t="s">
         <v>672</v>
       </c>
       <c r="D27" s="161" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E27" s="128"/>
       <c r="F27" s="96"/>
@@ -18487,16 +18487,16 @@
       <c r="N27" s="96"/>
       <c r="O27" s="127"/>
       <c r="P27" s="67" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="157" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C28" s="164"/>
       <c r="D28" s="161" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E28" s="128"/>
       <c r="F28" s="96"/>
@@ -18516,16 +18516,16 @@
       <c r="N28" s="96"/>
       <c r="O28" s="127"/>
       <c r="P28" s="67" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="157" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C29" s="164"/>
       <c r="D29" s="155" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E29" s="128"/>
       <c r="F29" s="96"/>
@@ -18545,16 +18545,16 @@
       <c r="N29" s="96"/>
       <c r="O29" s="127"/>
       <c r="P29" s="67" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="157" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C30" s="164"/>
       <c r="D30" s="161" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E30" s="128" t="s">
         <v>200</v>
@@ -18572,16 +18572,16 @@
       <c r="N30" s="96"/>
       <c r="O30" s="127"/>
       <c r="P30" s="67" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="157" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C31" s="164"/>
       <c r="D31" s="162" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E31" s="128" t="s">
         <v>200</v>
@@ -18601,16 +18601,16 @@
       <c r="N31" s="96"/>
       <c r="O31" s="127"/>
       <c r="P31" s="67" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="157" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C32" s="164"/>
       <c r="D32" s="162" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E32" s="128" t="s">
         <v>200</v>
@@ -18630,16 +18630,16 @@
         <v>683</v>
       </c>
       <c r="P32" s="67" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="157" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C33" s="164"/>
       <c r="D33" s="155" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E33" s="128"/>
       <c r="F33" s="96"/>
@@ -18659,16 +18659,16 @@
       <c r="N33" s="96"/>
       <c r="O33" s="127"/>
       <c r="P33" s="67" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="157" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C34" s="165"/>
       <c r="D34" s="162" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E34" s="128"/>
       <c r="F34" s="96"/>
@@ -18688,7 +18688,7 @@
       <c r="N34" s="96"/>
       <c r="O34" s="137"/>
       <c r="P34" s="113" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18883,8 +18883,9 @@
     <hyperlink ref="D32" r:id="rId11" location="'Metadatos M'!B6"/>
     <hyperlink ref="D33" r:id="rId12" location="'Metadatos H'!B9"/>
     <hyperlink ref="D34" r:id="rId13" location="'Metadatos D'!B6"/>
+    <hyperlink ref="D13" r:id="rId14" location="'Metadatos M'!B11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
añadida nueva victoria y nueva derrota
</commit_message>
<xml_diff>
--- a/Docs/TDS/CueSheet.xlsx
+++ b/Docs/TDS/CueSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo-PT\Desktop\Wasted-Racing-master\Wasted-Racing-master\Docs\TDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo-PT\Desktop\Proyectos GitHub\Wasted-Racing\Docs\TDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2548" uniqueCount="859">
   <si>
     <t>Cue-Sheets</t>
   </si>
@@ -2338,9 +2338,6 @@
     <t>M-004</t>
   </si>
   <si>
-    <t>Musica final de carrera</t>
-  </si>
-  <si>
     <t>1.18</t>
   </si>
   <si>
@@ -2368,9 +2365,6 @@
     <t>Sonido del personaje al pasar por linea de meta en cualquier vuelta que no sea la última</t>
   </si>
   <si>
-    <t>1.21</t>
-  </si>
-  <si>
     <t>D-014</t>
   </si>
   <si>
@@ -2399,9 +2393,6 @@
   </si>
   <si>
     <t>Musica de fondo del nivel 1. Ultima vuelta</t>
-  </si>
-  <si>
-    <t>M-010</t>
   </si>
   <si>
     <t>Voz de selección / "Mis pedos apestan a anarquia"</t>
@@ -4402,6 +4393,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4569,7 +4561,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -4612,6 +4604,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4955,7 +4948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -5164,32 +5157,32 @@
         <v>16</v>
       </c>
       <c r="C8" s="16">
-        <f>Niveles!E41</f>
-        <v>5</v>
+        <f>Niveles!E40</f>
+        <v>4</v>
       </c>
       <c r="D8" s="14">
-        <f>Niveles!F41</f>
+        <f>Niveles!F40</f>
         <v>0</v>
       </c>
       <c r="E8" s="14">
-        <f>Niveles!G41</f>
+        <f>Niveles!G40</f>
         <v>8</v>
       </c>
       <c r="F8" s="14">
-        <f>Niveles!H41</f>
+        <f>Niveles!H40</f>
         <v>6</v>
       </c>
       <c r="G8" s="14">
-        <f>Niveles!I41</f>
+        <f>Niveles!I40</f>
         <v>11</v>
       </c>
       <c r="H8" s="14">
-        <f>Niveles!J41</f>
+        <f>Niveles!J40</f>
         <v>0</v>
       </c>
       <c r="I8" s="17">
         <f>SUM(C8:H8)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -5218,7 +5211,7 @@
       </c>
       <c r="C11" s="25">
         <f t="shared" ref="C11:I11" si="0">SUM(C4:C10)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="25">
         <f t="shared" si="0"/>
@@ -5242,7 +5235,7 @@
       </c>
       <c r="I11" s="25">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -5264,7 +5257,7 @@
   <dimension ref="A1:AMK22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -5285,7 +5278,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>472</v>
@@ -5363,7 +5356,7 @@
     </row>
     <row r="4" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="49"/>
@@ -5388,7 +5381,7 @@
         <v>477</v>
       </c>
       <c r="D5" s="177" t="s">
-        <v>743</v>
+        <v>732</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>200</v>
@@ -5405,10 +5398,10 @@
       <c r="M5" s="58"/>
       <c r="N5" s="58"/>
       <c r="O5" s="58" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="P5" s="60" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5419,7 +5412,7 @@
         <v>477</v>
       </c>
       <c r="D6" s="175" t="s">
-        <v>747</v>
+        <v>500</v>
       </c>
       <c r="E6" s="141" t="s">
         <v>200</v>
@@ -5436,10 +5429,10 @@
       <c r="M6" s="141"/>
       <c r="N6" s="141"/>
       <c r="O6" s="141" t="s">
+        <v>742</v>
+      </c>
+      <c r="P6" s="179" t="s">
         <v>744</v>
-      </c>
-      <c r="P6" s="179" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5450,7 +5443,7 @@
         <v>477</v>
       </c>
       <c r="D7" s="176" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E7" s="141" t="s">
         <v>200</v>
@@ -5467,10 +5460,10 @@
       <c r="M7" s="141"/>
       <c r="N7" s="141"/>
       <c r="O7" s="141" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="P7" s="179" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -13264,7 +13257,7 @@
       </c>
       <c r="C11" s="98"/>
       <c r="D11" s="145" t="s">
-        <v>500</v>
+        <v>741</v>
       </c>
       <c r="E11" s="96" t="s">
         <v>200</v>
@@ -13664,7 +13657,7 @@
       </c>
       <c r="O5" s="95"/>
       <c r="P5" s="129" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13695,7 +13688,7 @@
       </c>
       <c r="O6" s="126"/>
       <c r="P6" s="126" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13728,7 +13721,7 @@
       </c>
       <c r="O7" s="97"/>
       <c r="P7" s="97" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13759,7 +13752,7 @@
       </c>
       <c r="O8" s="97"/>
       <c r="P8" s="97" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13790,7 +13783,7 @@
       </c>
       <c r="O9" s="97"/>
       <c r="P9" s="97" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13821,7 +13814,7 @@
       </c>
       <c r="O10" s="97"/>
       <c r="P10" s="97" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13852,7 +13845,7 @@
       </c>
       <c r="O11" s="97"/>
       <c r="P11" s="97" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13885,7 +13878,7 @@
       </c>
       <c r="O12" s="97"/>
       <c r="P12" s="97" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13916,7 +13909,7 @@
       </c>
       <c r="O13" s="97"/>
       <c r="P13" s="97" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13947,7 +13940,7 @@
       </c>
       <c r="O14" s="97"/>
       <c r="P14" s="97" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13978,7 +13971,7 @@
       </c>
       <c r="O15" s="97"/>
       <c r="P15" s="97" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14011,7 +14004,7 @@
       </c>
       <c r="O16" s="97"/>
       <c r="P16" s="97" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14042,7 +14035,7 @@
       </c>
       <c r="O17" s="97"/>
       <c r="P17" s="97" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14073,7 +14066,7 @@
       </c>
       <c r="O18" s="97"/>
       <c r="P18" s="97" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14104,7 +14097,7 @@
       </c>
       <c r="O19" s="97"/>
       <c r="P19" s="97" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14137,7 +14130,7 @@
       </c>
       <c r="O20" s="97"/>
       <c r="P20" s="97" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14168,7 +14161,7 @@
       </c>
       <c r="O21" s="97"/>
       <c r="P21" s="97" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14199,7 +14192,7 @@
       </c>
       <c r="O22" s="97"/>
       <c r="P22" s="97" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14230,7 +14223,7 @@
       </c>
       <c r="O23" s="97"/>
       <c r="P23" s="97" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14263,7 +14256,7 @@
       </c>
       <c r="O24" s="97"/>
       <c r="P24" s="97" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14294,7 +14287,7 @@
       </c>
       <c r="O25" s="97"/>
       <c r="P25" s="97" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14325,7 +14318,7 @@
       </c>
       <c r="O26" s="97"/>
       <c r="P26" s="97" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14358,7 +14351,7 @@
       </c>
       <c r="O27" s="97"/>
       <c r="P27" s="97" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14389,7 +14382,7 @@
       </c>
       <c r="O28" s="97"/>
       <c r="P28" s="97" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14422,7 +14415,7 @@
       </c>
       <c r="O29" s="97"/>
       <c r="P29" s="97" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14453,7 +14446,7 @@
       </c>
       <c r="O30" s="97"/>
       <c r="P30" s="97" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14486,7 +14479,7 @@
       </c>
       <c r="O31" s="97"/>
       <c r="P31" s="97" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14517,7 +14510,7 @@
       </c>
       <c r="O32" s="97"/>
       <c r="P32" s="97" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -14548,7 +14541,7 @@
       </c>
       <c r="O33" s="97"/>
       <c r="P33" s="97" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14579,7 +14572,7 @@
       </c>
       <c r="O34" s="97"/>
       <c r="P34" s="97" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14610,7 +14603,7 @@
       </c>
       <c r="O35" s="97"/>
       <c r="P35" s="97" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14641,7 +14634,7 @@
       </c>
       <c r="O36" s="97"/>
       <c r="P36" s="97" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14674,7 +14667,7 @@
       </c>
       <c r="O37" s="97"/>
       <c r="P37" s="97" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="38" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14705,7 +14698,7 @@
       </c>
       <c r="O38" s="97"/>
       <c r="P38" s="97" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="39" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14736,7 +14729,7 @@
       </c>
       <c r="O39" s="97"/>
       <c r="P39" s="97" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
     </row>
     <row r="40" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14769,7 +14762,7 @@
       </c>
       <c r="O40" s="97"/>
       <c r="P40" s="97" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
     </row>
     <row r="41" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14800,7 +14793,7 @@
       </c>
       <c r="O41" s="97"/>
       <c r="P41" s="97" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="42" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14831,7 +14824,7 @@
       </c>
       <c r="O42" s="97"/>
       <c r="P42" s="97" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="43" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14862,7 +14855,7 @@
       </c>
       <c r="O43" s="97"/>
       <c r="P43" s="97" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
     </row>
     <row r="44" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -14895,7 +14888,7 @@
       </c>
       <c r="O44" s="97"/>
       <c r="P44" s="97" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="45" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14926,7 +14919,7 @@
       </c>
       <c r="O45" s="97"/>
       <c r="P45" s="97" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="46" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14957,7 +14950,7 @@
       </c>
       <c r="O46" s="97"/>
       <c r="P46" s="97" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
     </row>
     <row r="47" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14990,7 +14983,7 @@
       </c>
       <c r="O47" s="97"/>
       <c r="P47" s="97" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="48" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15021,7 +15014,7 @@
       </c>
       <c r="O48" s="97"/>
       <c r="P48" s="97" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15052,7 +15045,7 @@
       </c>
       <c r="O49" s="97"/>
       <c r="P49" s="97" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="50" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15083,7 +15076,7 @@
       </c>
       <c r="O50" s="97"/>
       <c r="P50" s="97" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="51" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15116,7 +15109,7 @@
       </c>
       <c r="O51" s="97"/>
       <c r="P51" s="97" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="52" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15147,7 +15140,7 @@
       </c>
       <c r="O52" s="97"/>
       <c r="P52" s="97" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
     </row>
     <row r="53" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15180,7 +15173,7 @@
       </c>
       <c r="O53" s="97"/>
       <c r="P53" s="97" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="54" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15211,7 +15204,7 @@
       </c>
       <c r="O54" s="97"/>
       <c r="P54" s="97" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="55" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15242,7 +15235,7 @@
       </c>
       <c r="O55" s="97"/>
       <c r="P55" s="97" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
     </row>
     <row r="56" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15273,7 +15266,7 @@
       </c>
       <c r="O56" s="97"/>
       <c r="P56" s="97" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="57" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15306,7 +15299,7 @@
       </c>
       <c r="O57" s="97"/>
       <c r="P57" s="97" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="58" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15337,7 +15330,7 @@
       </c>
       <c r="O58" s="97"/>
       <c r="P58" s="97" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
     </row>
     <row r="59" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15368,7 +15361,7 @@
       </c>
       <c r="O59" s="97"/>
       <c r="P59" s="97" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="60" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15401,7 +15394,7 @@
       </c>
       <c r="O60" s="97"/>
       <c r="P60" s="97" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
     </row>
     <row r="61" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15432,7 +15425,7 @@
       </c>
       <c r="O61" s="97"/>
       <c r="P61" s="97" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="62" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15465,7 +15458,7 @@
       </c>
       <c r="O62" s="97"/>
       <c r="P62" s="97" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
     </row>
     <row r="63" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15496,7 +15489,7 @@
       </c>
       <c r="O63" s="97"/>
       <c r="P63" s="97" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
     <row r="64" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15529,7 +15522,7 @@
       </c>
       <c r="O64" s="97"/>
       <c r="P64" s="97" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="65" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15560,7 +15553,7 @@
       </c>
       <c r="O65" s="97"/>
       <c r="P65" s="97" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="66" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15593,7 +15586,7 @@
       </c>
       <c r="O66" s="97"/>
       <c r="P66" s="97" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
     </row>
     <row r="67" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15624,7 +15617,7 @@
       </c>
       <c r="O67" s="97"/>
       <c r="P67" s="97" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="68" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15655,7 +15648,7 @@
       </c>
       <c r="O68" s="97"/>
       <c r="P68" s="97" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="69" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15686,7 +15679,7 @@
       </c>
       <c r="O69" s="97"/>
       <c r="P69" s="97" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
     </row>
     <row r="70" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15719,7 +15712,7 @@
       </c>
       <c r="O70" s="97"/>
       <c r="P70" s="97" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
     </row>
     <row r="71" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15750,7 +15743,7 @@
       </c>
       <c r="O71" s="97"/>
       <c r="P71" s="97" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="72" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15783,7 +15776,7 @@
       </c>
       <c r="O72" s="97"/>
       <c r="P72" s="97" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="73" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15814,7 +15807,7 @@
       </c>
       <c r="O73" s="97"/>
       <c r="P73" s="97" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
     </row>
     <row r="74" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15845,7 +15838,7 @@
       </c>
       <c r="O74" s="97"/>
       <c r="P74" s="97" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="75" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15876,7 +15869,7 @@
       </c>
       <c r="O75" s="97"/>
       <c r="P75" s="97" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="76" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15907,7 +15900,7 @@
       </c>
       <c r="O76" s="97"/>
       <c r="P76" s="97" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="77" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15940,7 +15933,7 @@
       </c>
       <c r="O77" s="97"/>
       <c r="P77" s="97" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="78" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15971,7 +15964,7 @@
       </c>
       <c r="O78" s="97"/>
       <c r="P78" s="97" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="79" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16002,7 +15995,7 @@
       </c>
       <c r="O79" s="97"/>
       <c r="P79" s="97" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="80" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16033,7 +16026,7 @@
       </c>
       <c r="O80" s="97"/>
       <c r="P80" s="97" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="81" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16064,7 +16057,7 @@
       </c>
       <c r="O81" s="97"/>
       <c r="P81" s="97" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="82" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16095,7 +16088,7 @@
       </c>
       <c r="O82" s="97"/>
       <c r="P82" s="97" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="83" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16128,7 +16121,7 @@
       </c>
       <c r="O83" s="97"/>
       <c r="P83" s="97" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="84" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16159,7 +16152,7 @@
       </c>
       <c r="O84" s="97"/>
       <c r="P84" s="97" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
     </row>
     <row r="85" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16190,7 +16183,7 @@
       </c>
       <c r="O85" s="97"/>
       <c r="P85" s="97" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
     <row r="86" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16221,7 +16214,7 @@
       </c>
       <c r="O86" s="97"/>
       <c r="P86" s="97" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="87" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16254,7 +16247,7 @@
       </c>
       <c r="O87" s="97"/>
       <c r="P87" s="97" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
     </row>
     <row r="88" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16285,7 +16278,7 @@
       </c>
       <c r="O88" s="97"/>
       <c r="P88" s="97" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="89" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16318,7 +16311,7 @@
       </c>
       <c r="O89" s="97"/>
       <c r="P89" s="97" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
     </row>
     <row r="90" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16349,7 +16342,7 @@
       </c>
       <c r="O90" s="97"/>
       <c r="P90" s="97" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
     </row>
     <row r="91" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16380,7 +16373,7 @@
       </c>
       <c r="O91" s="97"/>
       <c r="P91" s="97" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
     </row>
     <row r="92" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16413,7 +16406,7 @@
       </c>
       <c r="O92" s="97"/>
       <c r="P92" s="97" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="93" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16444,7 +16437,7 @@
       </c>
       <c r="O93" s="97"/>
       <c r="P93" s="97" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="94" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16475,7 +16468,7 @@
       </c>
       <c r="O94" s="97"/>
       <c r="P94" s="97" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
     </row>
     <row r="95" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16506,7 +16499,7 @@
       </c>
       <c r="O95" s="97"/>
       <c r="P95" s="97" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
     </row>
     <row r="96" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16537,7 +16530,7 @@
       </c>
       <c r="O96" s="97"/>
       <c r="P96" s="97" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="97" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16568,7 +16561,7 @@
       </c>
       <c r="O97" s="97"/>
       <c r="P97" s="97" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
     </row>
     <row r="98" spans="2:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16601,7 +16594,7 @@
       </c>
       <c r="O98" s="97"/>
       <c r="P98" s="97" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="99" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16632,7 +16625,7 @@
       </c>
       <c r="O99" s="97"/>
       <c r="P99" s="97" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
     </row>
     <row r="100" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16663,7 +16656,7 @@
       </c>
       <c r="O100" s="97"/>
       <c r="P100" s="97" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="101" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16696,7 +16689,7 @@
       </c>
       <c r="O101" s="97"/>
       <c r="P101" s="97" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="102" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16727,7 +16720,7 @@
       </c>
       <c r="O102" s="97"/>
       <c r="P102" s="97" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
     </row>
     <row r="103" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16758,7 +16751,7 @@
       </c>
       <c r="O103" s="97"/>
       <c r="P103" s="97" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="104" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16791,7 +16784,7 @@
       </c>
       <c r="O104" s="97"/>
       <c r="P104" s="97" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="105" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16822,7 +16815,7 @@
       </c>
       <c r="O105" s="97"/>
       <c r="P105" s="97" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="106" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16853,7 +16846,7 @@
       </c>
       <c r="O106" s="97"/>
       <c r="P106" s="97" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="107" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16884,7 +16877,7 @@
       </c>
       <c r="O107" s="97"/>
       <c r="P107" s="97" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
     </row>
     <row r="108" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16917,7 +16910,7 @@
       </c>
       <c r="O108" s="97"/>
       <c r="P108" s="97" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
     </row>
     <row r="109" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16948,7 +16941,7 @@
       </c>
       <c r="O109" s="97"/>
       <c r="P109" s="97" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="110" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16979,7 +16972,7 @@
       </c>
       <c r="O110" s="97"/>
       <c r="P110" s="97" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
     </row>
     <row r="111" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17012,7 +17005,7 @@
       </c>
       <c r="O111" s="97"/>
       <c r="P111" s="97" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="112" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17043,7 +17036,7 @@
       </c>
       <c r="O112" s="97"/>
       <c r="P112" s="97" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
     </row>
     <row r="113" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17074,7 +17067,7 @@
       </c>
       <c r="O113" s="97"/>
       <c r="P113" s="97" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
     </row>
     <row r="114" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17105,7 +17098,7 @@
       </c>
       <c r="O114" s="97"/>
       <c r="P114" s="97" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
     </row>
     <row r="115" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17138,7 +17131,7 @@
       </c>
       <c r="O115" s="97"/>
       <c r="P115" s="97" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
     </row>
     <row r="116" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17169,7 +17162,7 @@
       </c>
       <c r="O116" s="97"/>
       <c r="P116" s="97" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
     </row>
     <row r="117" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17200,7 +17193,7 @@
       </c>
       <c r="O117" s="97"/>
       <c r="P117" s="97" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
     <row r="118" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17231,7 +17224,7 @@
       </c>
       <c r="O118" s="97"/>
       <c r="P118" s="97" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
     </row>
     <row r="119" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17264,7 +17257,7 @@
       </c>
       <c r="O119" s="97"/>
       <c r="P119" s="97" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
     </row>
     <row r="120" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17295,7 +17288,7 @@
       </c>
       <c r="O120" s="97"/>
       <c r="P120" s="97" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
     </row>
     <row r="121" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17328,7 +17321,7 @@
       </c>
       <c r="O121" s="97"/>
       <c r="P121" s="97" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
     </row>
     <row r="122" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17359,7 +17352,7 @@
       </c>
       <c r="O122" s="97"/>
       <c r="P122" s="97" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
     </row>
     <row r="123" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17643,10 +17636,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK43"/>
+  <dimension ref="A1:AMK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="31.5" x14ac:dyDescent="0.25"/>
@@ -18047,7 +18040,7 @@
         <v>683</v>
       </c>
       <c r="P13" s="67" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18519,7 +18512,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="29" spans="2:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="157" t="s">
         <v>723</v>
       </c>
@@ -18548,12 +18541,12 @@
         <v>725</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="157" t="s">
         <v>726</v>
       </c>
       <c r="C30" s="164"/>
-      <c r="D30" s="161" t="s">
+      <c r="D30" s="162" t="s">
         <v>727</v>
       </c>
       <c r="E30" s="128" t="s">
@@ -18567,21 +18560,23 @@
       <c r="K30" s="128" t="s">
         <v>289</v>
       </c>
-      <c r="L30" s="96"/>
+      <c r="L30" s="96" t="s">
+        <v>485</v>
+      </c>
       <c r="M30" s="96"/>
       <c r="N30" s="96"/>
       <c r="O30" s="127"/>
       <c r="P30" s="67" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="157" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C31" s="164"/>
       <c r="D31" s="162" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E31" s="128" t="s">
         <v>200</v>
@@ -18601,54 +18596,54 @@
       <c r="N31" s="96"/>
       <c r="O31" s="127"/>
       <c r="P31" s="67" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="157" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="157" t="s">
-        <v>732</v>
-      </c>
       <c r="C32" s="164"/>
-      <c r="D32" s="162" t="s">
-        <v>733</v>
-      </c>
-      <c r="E32" s="128" t="s">
-        <v>200</v>
-      </c>
+      <c r="D32" s="155" t="s">
+        <v>735</v>
+      </c>
+      <c r="E32" s="128"/>
       <c r="F32" s="96"/>
-      <c r="G32" s="96"/>
+      <c r="G32" s="96" t="s">
+        <v>202</v>
+      </c>
       <c r="H32" s="96"/>
       <c r="I32" s="127"/>
       <c r="J32" s="110"/>
       <c r="K32" s="128" t="s">
         <v>289</v>
       </c>
-      <c r="L32" s="96"/>
+      <c r="L32" s="96" t="s">
+        <v>485</v>
+      </c>
       <c r="M32" s="96"/>
       <c r="N32" s="96"/>
-      <c r="O32" s="127" t="s">
-        <v>683</v>
-      </c>
+      <c r="O32" s="127"/>
       <c r="P32" s="67" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="157" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="157" t="s">
-        <v>735</v>
-      </c>
-      <c r="C33" s="164"/>
-      <c r="D33" s="155" t="s">
-        <v>736</v>
+      <c r="C33" s="165"/>
+      <c r="D33" s="162" t="s">
+        <v>737</v>
       </c>
       <c r="E33" s="128"/>
       <c r="F33" s="96"/>
-      <c r="G33" s="96" t="s">
-        <v>202</v>
-      </c>
+      <c r="G33" s="96"/>
       <c r="H33" s="96"/>
-      <c r="I33" s="127"/>
-      <c r="J33" s="110"/>
+      <c r="I33" s="127" t="s">
+        <v>282</v>
+      </c>
+      <c r="J33" s="164"/>
       <c r="K33" s="128" t="s">
         <v>289</v>
       </c>
@@ -18657,39 +18652,27 @@
       </c>
       <c r="M33" s="96"/>
       <c r="N33" s="96"/>
-      <c r="O33" s="127"/>
-      <c r="P33" s="67" t="s">
-        <v>737</v>
+      <c r="O33" s="137"/>
+      <c r="P33" s="113" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="157" t="s">
-        <v>738</v>
-      </c>
-      <c r="C34" s="165"/>
-      <c r="D34" s="162" t="s">
-        <v>739</v>
-      </c>
-      <c r="E34" s="128"/>
-      <c r="F34" s="96"/>
-      <c r="G34" s="96"/>
-      <c r="H34" s="96"/>
-      <c r="I34" s="127" t="s">
-        <v>282</v>
-      </c>
-      <c r="J34" s="164"/>
-      <c r="K34" s="128" t="s">
-        <v>289</v>
-      </c>
-      <c r="L34" s="96" t="s">
-        <v>485</v>
-      </c>
-      <c r="M34" s="96"/>
-      <c r="N34" s="96"/>
-      <c r="O34" s="137"/>
-      <c r="P34" s="113" t="s">
-        <v>740</v>
-      </c>
+      <c r="B34" s="106"/>
+      <c r="C34" s="107"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="110"/>
+      <c r="F34" s="110"/>
+      <c r="G34" s="110"/>
+      <c r="H34" s="110"/>
+      <c r="I34" s="110"/>
+      <c r="J34" s="110"/>
+      <c r="K34" s="103"/>
+      <c r="L34" s="159"/>
+      <c r="M34" s="103"/>
+      <c r="N34" s="103"/>
+      <c r="O34" s="112"/>
+      <c r="P34" s="113"/>
     </row>
     <row r="35" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="106"/>
@@ -18744,84 +18727,84 @@
     </row>
     <row r="38" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="106"/>
-      <c r="C38" s="107"/>
-      <c r="D38" s="108"/>
-      <c r="E38" s="110"/>
-      <c r="F38" s="110"/>
-      <c r="G38" s="110"/>
-      <c r="H38" s="110"/>
-      <c r="I38" s="110"/>
-      <c r="J38" s="110"/>
-      <c r="K38" s="103"/>
-      <c r="L38" s="159"/>
-      <c r="M38" s="103"/>
-      <c r="N38" s="103"/>
-      <c r="O38" s="112"/>
+      <c r="C38" s="138"/>
+      <c r="D38" s="114"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="102"/>
+      <c r="G38" s="102"/>
+      <c r="H38" s="102"/>
+      <c r="I38" s="102"/>
+      <c r="J38" s="103"/>
+      <c r="K38" s="102"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="102"/>
+      <c r="N38" s="102"/>
+      <c r="O38" s="139"/>
       <c r="P38" s="113"/>
     </row>
     <row r="39" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="106"/>
-      <c r="C39" s="138"/>
-      <c r="D39" s="114"/>
-      <c r="E39" s="102"/>
-      <c r="F39" s="102"/>
-      <c r="G39" s="102"/>
-      <c r="H39" s="102"/>
-      <c r="I39" s="102"/>
-      <c r="J39" s="103"/>
-      <c r="K39" s="102"/>
-      <c r="L39" s="111"/>
-      <c r="M39" s="102"/>
-      <c r="N39" s="102"/>
-      <c r="O39" s="139"/>
-      <c r="P39" s="113"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="119"/>
+      <c r="F39" s="119"/>
+      <c r="G39" s="119"/>
+      <c r="H39" s="119"/>
+      <c r="I39" s="119"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="119"/>
+      <c r="L39" s="120"/>
+      <c r="M39" s="119"/>
+      <c r="N39" s="119"/>
+      <c r="O39" s="121"/>
+      <c r="P39" s="122"/>
     </row>
     <row r="40" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="116"/>
-      <c r="C40" s="117"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="119"/>
-      <c r="F40" s="119"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="119"/>
-      <c r="I40" s="119"/>
-      <c r="J40" s="119"/>
-      <c r="K40" s="119"/>
-      <c r="L40" s="120"/>
-      <c r="M40" s="119"/>
-      <c r="N40" s="119"/>
-      <c r="O40" s="121"/>
-      <c r="P40" s="122"/>
+      <c r="B40" s="78"/>
+      <c r="C40" s="87" t="s">
+        <v>360</v>
+      </c>
+      <c r="D40" s="87"/>
+      <c r="E40" s="88">
+        <f>COUNTA(E5:E38)</f>
+        <v>4</v>
+      </c>
+      <c r="F40" s="88">
+        <f>COUNTA(F5:F39)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="88">
+        <f>COUNTA(G5:G39)</f>
+        <v>8</v>
+      </c>
+      <c r="H40" s="88">
+        <f>COUNTA(H5:H39)</f>
+        <v>6</v>
+      </c>
+      <c r="I40" s="88">
+        <f>COUNTA(I5:I39)</f>
+        <v>11</v>
+      </c>
+      <c r="J40" s="88">
+        <v>0</v>
+      </c>
+      <c r="K40" s="71"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
+      <c r="N40" s="73"/>
+      <c r="O40" s="73"/>
+      <c r="P40" s="73"/>
     </row>
     <row r="41" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="78"/>
-      <c r="C41" s="87" t="s">
-        <v>360</v>
-      </c>
-      <c r="D41" s="87"/>
-      <c r="E41" s="88">
-        <f>COUNTA(E5:E39)</f>
-        <v>5</v>
-      </c>
-      <c r="F41" s="88">
-        <f>COUNTA(F5:F40)</f>
-        <v>0</v>
-      </c>
-      <c r="G41" s="88">
-        <f>COUNTA(G5:G40)</f>
-        <v>8</v>
-      </c>
-      <c r="H41" s="88">
-        <f>COUNTA(H5:H40)</f>
-        <v>6</v>
-      </c>
-      <c r="I41" s="88">
-        <f>COUNTA(I5:I40)</f>
-        <v>11</v>
-      </c>
-      <c r="J41" s="88">
-        <v>0</v>
-      </c>
+      <c r="B41" s="73"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
       <c r="K41" s="71"/>
       <c r="L41" s="71"/>
       <c r="M41" s="71"/>
@@ -18831,42 +18814,25 @@
     </row>
     <row r="42" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="73"/>
-      <c r="C42" s="87"/>
+      <c r="C42" s="73"/>
       <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="71"/>
-      <c r="K42" s="71"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="89"/>
+      <c r="H42" s="89"/>
+      <c r="I42" s="89"/>
+      <c r="J42" s="90" t="s">
+        <v>362</v>
+      </c>
+      <c r="K42" s="91">
+        <f>COUNTA(E5:I39)</f>
+        <v>29</v>
+      </c>
       <c r="L42" s="71"/>
       <c r="M42" s="71"/>
       <c r="N42" s="73"/>
       <c r="O42" s="73"/>
       <c r="P42" s="73"/>
-    </row>
-    <row r="43" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="73"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="89"/>
-      <c r="F43" s="89"/>
-      <c r="G43" s="89"/>
-      <c r="H43" s="89"/>
-      <c r="I43" s="89"/>
-      <c r="J43" s="90" t="s">
-        <v>362</v>
-      </c>
-      <c r="K43" s="91">
-        <f>COUNTA(E5:I40)</f>
-        <v>30</v>
-      </c>
-      <c r="L43" s="71"/>
-      <c r="M43" s="71"/>
-      <c r="N43" s="73"/>
-      <c r="O43" s="73"/>
-      <c r="P43" s="73"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -18879,10 +18845,10 @@
     <hyperlink ref="D23" r:id="rId7" location="'Metadatos M'!B4"/>
     <hyperlink ref="D24" r:id="rId8" location="'Metadatos D'!B5"/>
     <hyperlink ref="D29" r:id="rId9" location="'Metadatos H'!B10"/>
-    <hyperlink ref="D31" r:id="rId10" location="'Metadatos M'!B5"/>
-    <hyperlink ref="D32" r:id="rId11" location="'Metadatos M'!B6"/>
-    <hyperlink ref="D33" r:id="rId12" location="'Metadatos H'!B9"/>
-    <hyperlink ref="D34" r:id="rId13" location="'Metadatos D'!B6"/>
+    <hyperlink ref="D30" r:id="rId10" location="'Metadatos M'!B5"/>
+    <hyperlink ref="D31" r:id="rId11" location="'Metadatos M'!B6"/>
+    <hyperlink ref="D32" r:id="rId12" location="'Metadatos H'!B9"/>
+    <hyperlink ref="D33" r:id="rId13" location="'Metadatos D'!B6"/>
     <hyperlink ref="D13" r:id="rId14" location="'Metadatos M'!B11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>